<commit_message>
modified the scene type new way to enter scene
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Player.xlsx
+++ b/_Out/NFDataCfg/Excel/Player.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="10343" firstSheet="1" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="10343"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -477,9 +477,6 @@
     <t>Gold</t>
   </si>
   <si>
-    <t>Money</t>
-  </si>
-  <si>
     <t>Account</t>
   </si>
   <si>
@@ -1155,6 +1152,9 @@
   </si>
   <si>
     <t>HeroValue</t>
+  </si>
+  <si>
+    <t>Diamond</t>
   </si>
 </sst>
 </file>
@@ -1852,9 +1852,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A9" sqref="A9"/>
+      <selection pane="bottomLeft" activeCell="AP1" sqref="AP1:AP1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1912,25 +1912,25 @@
         <v>9</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="L1" s="28" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="M1" s="28" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="N1" s="28" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="O1" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="P1" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="Q1" s="28" t="s">
         <v>159</v>
-      </c>
-      <c r="Q1" s="28" t="s">
-        <v>160</v>
       </c>
       <c r="R1" s="28" t="s">
         <v>11</v>
@@ -1954,215 +1954,215 @@
         <v>17</v>
       </c>
       <c r="Y1" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="Z1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="Z1" s="28" t="s">
+      <c r="AA1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="AA1" s="28" t="s">
+      <c r="AB1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="AB1" s="28" t="s">
+      <c r="AC1" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="AC1" s="28" t="s">
+      <c r="AD1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="AD1" s="28" t="s">
+      <c r="AE1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="AE1" s="28" t="s">
+      <c r="AF1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="AF1" s="28" t="s">
+      <c r="AG1" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="AG1" s="28" t="s">
+      <c r="AH1" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="AH1" s="28" t="s">
+      <c r="AI1" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AI1" s="28" t="s">
+      <c r="AJ1" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="AJ1" s="28" t="s">
+      <c r="AK1" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="AK1" s="28" t="s">
+      <c r="AL1" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="AL1" s="28" t="s">
+      <c r="AM1" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="AM1" s="28" t="s">
+      <c r="AN1" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="AN1" s="28" t="s">
+      <c r="AO1" s="28" t="s">
         <v>33</v>
-      </c>
-      <c r="AO1" s="28" t="s">
-        <v>34</v>
       </c>
       <c r="AP1" s="28" t="s">
         <v>5</v>
       </c>
       <c r="AQ1" s="25" t="s">
+        <v>34</v>
+      </c>
+      <c r="AR1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="AR1" s="25" t="s">
+      <c r="AS1" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="AS1" s="25" t="s">
+      <c r="AT1" s="25" t="s">
         <v>37</v>
-      </c>
-      <c r="AT1" s="25" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:46" s="26" customFormat="1">
       <c r="A2" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>40</v>
-      </c>
       <c r="C2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="K2" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="L2" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="M2" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="N2" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="K2" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="M2" s="39" t="s">
-        <v>42</v>
-      </c>
-      <c r="N2" s="39" t="s">
-        <v>42</v>
-      </c>
       <c r="O2" s="39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P2" s="39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q2" s="39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="AB2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AC2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AD2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AE2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AF2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AH2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AL2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="AO2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="AP2" s="30" t="s">
+        <v>40</v>
+      </c>
+      <c r="AQ2" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="AR2" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="Y2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AI2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AJ2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AL2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM2" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AP2" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="AQ2" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="AR2" s="30" t="s">
-        <v>42</v>
-      </c>
       <c r="AS2" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AT2" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:46" s="26" customFormat="1">
       <c r="A3" s="29" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -2302,7 +2302,7 @@
     </row>
     <row r="4" spans="1:46" s="26" customFormat="1">
       <c r="A4" s="29" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -2442,7 +2442,7 @@
     </row>
     <row r="5" spans="1:46" s="26" customFormat="1">
       <c r="A5" s="29" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="16">
         <v>0</v>
@@ -2582,7 +2582,7 @@
     </row>
     <row r="6" spans="1:46" s="26" customFormat="1">
       <c r="A6" s="29" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
@@ -2722,7 +2722,7 @@
     </row>
     <row r="7" spans="1:46" s="16" customFormat="1">
       <c r="A7" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="16">
         <v>0</v>
@@ -2862,7 +2862,7 @@
     </row>
     <row r="8" spans="1:46" s="16" customFormat="1">
       <c r="A8" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B8" s="16">
         <v>0</v>
@@ -3002,7 +3002,7 @@
     </row>
     <row r="9" spans="1:46" s="16" customFormat="1">
       <c r="A9" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="16">
         <v>0</v>
@@ -3142,143 +3142,143 @@
     </row>
     <row r="10" spans="1:46" s="17" customFormat="1" ht="67.5">
       <c r="A10" s="23" t="s">
+        <v>48</v>
+      </c>
+      <c r="B10" s="24" t="s">
         <v>49</v>
       </c>
-      <c r="B10" s="24" t="s">
+      <c r="C10" s="24" t="s">
         <v>50</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="D10" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="F10" s="24" t="s">
+        <v>52</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>54</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>55</v>
+      </c>
+      <c r="I10" s="24" t="s">
+        <v>56</v>
+      </c>
+      <c r="J10" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="K10" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="L10" s="41" t="s">
+        <v>217</v>
+      </c>
+      <c r="M10" s="41" t="s">
+        <v>218</v>
+      </c>
+      <c r="N10" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="O10" s="41" t="s">
+        <v>217</v>
+      </c>
+      <c r="P10" s="41" t="s">
+        <v>218</v>
+      </c>
+      <c r="Q10" s="41" t="s">
+        <v>219</v>
+      </c>
+      <c r="R10" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="F10" s="24" t="s">
+      <c r="S10" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="T10" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="U10" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="V10" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="W10" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="X10" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y10" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z10" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA10" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB10" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC10" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD10" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE10" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF10" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG10" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH10" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI10" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ10" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK10" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL10" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM10" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN10" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO10" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="AP10" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="G10" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>56</v>
-      </c>
-      <c r="I10" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="J10" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="K10" s="41" t="s">
-        <v>217</v>
-      </c>
-      <c r="L10" s="41" t="s">
-        <v>218</v>
-      </c>
-      <c r="M10" s="41" t="s">
-        <v>219</v>
-      </c>
-      <c r="N10" s="41" t="s">
-        <v>220</v>
-      </c>
-      <c r="O10" s="41" t="s">
-        <v>218</v>
-      </c>
-      <c r="P10" s="41" t="s">
-        <v>219</v>
-      </c>
-      <c r="Q10" s="41" t="s">
-        <v>220</v>
-      </c>
-      <c r="R10" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="S10" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="T10" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="U10" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="V10" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="W10" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="X10" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="Y10" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="Z10" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="AA10" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB10" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="AC10" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="AD10" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="AE10" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="AF10" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="AG10" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="AH10" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="AI10" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="AJ10" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="AK10" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="AL10" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="AM10" s="24" t="s">
-        <v>80</v>
-      </c>
-      <c r="AN10" s="24" t="s">
-        <v>81</v>
-      </c>
-      <c r="AO10" s="24" t="s">
+      <c r="AQ10" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="AP10" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="AQ10" s="32" t="s">
+      <c r="AR10" s="32" t="s">
         <v>83</v>
-      </c>
-      <c r="AR10" s="32" t="s">
-        <v>84</v>
       </c>
       <c r="AS10" s="33"/>
       <c r="AT10" s="33"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:T3 AQ5:AR6 V3:AJ3 J3 K6:Q6 B5:AP5 B7:AO9 AQ7:AT9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:T3 AQ5:AR6 V3:AJ3 J3 K6:Q6 AQ7:AT9 B7:AO9 B5:AP5">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>
@@ -3307,188 +3307,188 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="D1" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="E1" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="E1" s="19" t="s">
+      <c r="F1" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>89</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="J1" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="K1" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="L1" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="M1" s="19" t="s">
         <v>95</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="N1" s="19" t="s">
         <v>96</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="O1" s="19" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="19" t="s">
+      <c r="P1" s="19" t="s">
         <v>98</v>
       </c>
-      <c r="P1" s="19" t="s">
+      <c r="Q1" s="19" t="s">
         <v>99</v>
       </c>
-      <c r="Q1" s="19" t="s">
+      <c r="R1" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="R1" s="19" t="s">
+      <c r="S1" s="19" t="s">
         <v>101</v>
       </c>
-      <c r="S1" s="19" t="s">
+      <c r="T1" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="T1" s="19" t="s">
+      <c r="U1" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="U1" s="19" t="s">
+      <c r="V1" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="V1" s="19" t="s">
+      <c r="W1" s="19" t="s">
         <v>105</v>
       </c>
-      <c r="W1" s="19" t="s">
+      <c r="X1" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="X1" s="19" t="s">
+      <c r="Y1" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="Y1" s="19" t="s">
+      <c r="Z1" s="19" t="s">
         <v>108</v>
       </c>
-      <c r="Z1" s="19" t="s">
+      <c r="AA1" s="19" t="s">
         <v>109</v>
       </c>
-      <c r="AA1" s="19" t="s">
+      <c r="AB1" s="19" t="s">
         <v>110</v>
       </c>
-      <c r="AB1" s="19" t="s">
+      <c r="AC1" s="19" t="s">
         <v>111</v>
       </c>
-      <c r="AC1" s="19" t="s">
+      <c r="AD1" s="19" t="s">
         <v>112</v>
-      </c>
-      <c r="AD1" s="19" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="2" spans="1:30" s="15" customFormat="1">
       <c r="A2" s="20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="U2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Y2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Z2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AA2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AB2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AD2" s="21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:30" s="15" customFormat="1">
       <c r="A3" s="20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="21">
         <v>1</v>
@@ -3580,7 +3580,7 @@
     </row>
     <row r="4" spans="1:30" s="15" customFormat="1">
       <c r="A4" s="20" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="21">
         <v>1</v>
@@ -3672,7 +3672,7 @@
     </row>
     <row r="5" spans="1:30" s="15" customFormat="1">
       <c r="A5" s="20" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B5" s="21">
         <v>0</v>
@@ -3764,7 +3764,7 @@
     </row>
     <row r="6" spans="1:30" s="15" customFormat="1">
       <c r="A6" s="20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B6" s="21">
         <v>0</v>
@@ -3856,7 +3856,7 @@
     </row>
     <row r="7" spans="1:30" s="16" customFormat="1">
       <c r="A7" s="22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7" s="16">
         <v>0</v>
@@ -3948,7 +3948,7 @@
     </row>
     <row r="8" spans="1:30" s="16" customFormat="1">
       <c r="A8" s="22" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B8" s="16">
         <v>0</v>
@@ -4040,7 +4040,7 @@
     </row>
     <row r="9" spans="1:30" s="16" customFormat="1">
       <c r="A9" s="22" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B9" s="16">
         <v>0</v>
@@ -4132,94 +4132,94 @@
     </row>
     <row r="10" spans="1:30" s="17" customFormat="1" ht="54">
       <c r="A10" s="23" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B10" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="C10" s="24" t="s">
         <v>114</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="D10" s="24" t="s">
         <v>115</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="E10" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="G10" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="H10" s="24" t="s">
         <v>116</v>
       </c>
-      <c r="E10" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="H10" s="24" t="s">
+      <c r="I10" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="J10" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="J10" s="24" t="s">
+      <c r="K10" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="K10" s="24" t="s">
+      <c r="L10" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="L10" s="24" t="s">
+      <c r="M10" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="M10" s="24" t="s">
+      <c r="N10" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="N10" s="24" t="s">
+      <c r="O10" s="24" t="s">
         <v>123</v>
       </c>
-      <c r="O10" s="24" t="s">
+      <c r="P10" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="P10" s="24" t="s">
+      <c r="Q10" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="Q10" s="24" t="s">
+      <c r="R10" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="R10" s="24" t="s">
+      <c r="S10" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="S10" s="24" t="s">
+      <c r="T10" s="24" t="s">
         <v>128</v>
       </c>
-      <c r="T10" s="24" t="s">
+      <c r="U10" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="U10" s="24" t="s">
+      <c r="V10" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="V10" s="24" t="s">
+      <c r="W10" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="W10" s="24" t="s">
+      <c r="X10" s="24" t="s">
         <v>132</v>
       </c>
-      <c r="X10" s="24" t="s">
+      <c r="Y10" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="Y10" s="24" t="s">
+      <c r="Z10" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="Z10" s="24" t="s">
+      <c r="AA10" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="AA10" s="24" t="s">
+      <c r="AB10" s="24" t="s">
         <v>136</v>
       </c>
-      <c r="AB10" s="24" t="s">
+      <c r="AC10" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="AC10" s="24" t="s">
+      <c r="AD10" s="24" t="s">
         <v>138</v>
-      </c>
-      <c r="AD10" s="24" t="s">
-        <v>139</v>
       </c>
     </row>
   </sheetData>
@@ -4279,12 +4279,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" s="3">
         <v>15</v>
@@ -4292,7 +4292,7 @@
     </row>
     <row r="3" spans="1:29" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B3" s="3">
         <v>29</v>
@@ -4300,7 +4300,7 @@
     </row>
     <row r="4" spans="1:29" s="3" customFormat="1">
       <c r="A4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -4308,7 +4308,7 @@
     </row>
     <row r="5" spans="1:29" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
@@ -4316,7 +4316,7 @@
     </row>
     <row r="6" spans="1:29" s="3" customFormat="1">
       <c r="A6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -4324,7 +4324,7 @@
     </row>
     <row r="7" spans="1:29" s="3" customFormat="1">
       <c r="A7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="3">
         <v>0</v>
@@ -4332,7 +4332,7 @@
     </row>
     <row r="8" spans="1:29" s="3" customFormat="1">
       <c r="A8" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -4340,188 +4340,188 @@
     </row>
     <row r="9" spans="1:29" s="3" customFormat="1">
       <c r="A9" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="C9" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="D9" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="34" t="s">
+      <c r="E9" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="F9" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="G9" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="G9" s="34" t="s">
+      <c r="H9" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="I9" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I9" s="34" t="s">
+      <c r="J9" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="J9" s="34" t="s">
+      <c r="K9" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="K9" s="34" t="s">
+      <c r="L9" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="L9" s="34" t="s">
+      <c r="M9" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="M9" s="34" t="s">
+      <c r="N9" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="N9" s="34" t="s">
+      <c r="O9" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="O9" s="34" t="s">
+      <c r="P9" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="P9" s="34" t="s">
+      <c r="Q9" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="Q9" s="34" t="s">
+      <c r="R9" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="R9" s="34" t="s">
+      <c r="S9" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="S9" s="34" t="s">
+      <c r="T9" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="T9" s="34" t="s">
+      <c r="U9" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="U9" s="34" t="s">
+      <c r="V9" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="V9" s="34" t="s">
+      <c r="W9" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="W9" s="34" t="s">
+      <c r="X9" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="X9" s="34" t="s">
+      <c r="Y9" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="Y9" s="34" t="s">
+      <c r="Z9" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="Z9" s="34" t="s">
+      <c r="AA9" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="AA9" s="34" t="s">
+      <c r="AB9" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="AB9" s="34" t="s">
+      <c r="AC9" s="34" t="s">
         <v>112</v>
-      </c>
-      <c r="AC9" s="34" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="10" spans="1:29" s="3" customFormat="1">
       <c r="A10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="U10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Y10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Z10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AA10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AB10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:29" s="3" customFormat="1">
       <c r="A11" s="34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C11" s="34"/>
       <c r="D11" s="34"/>
@@ -4612,12 +4612,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:23" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" s="3">
         <v>64</v>
@@ -4625,7 +4625,7 @@
     </row>
     <row r="3" spans="1:23" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B3" s="3">
         <v>23</v>
@@ -4633,7 +4633,7 @@
     </row>
     <row r="4" spans="1:23" s="3" customFormat="1">
       <c r="A4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -4641,7 +4641,7 @@
     </row>
     <row r="5" spans="1:23" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
@@ -4649,7 +4649,7 @@
     </row>
     <row r="6" spans="1:23" s="3" customFormat="1">
       <c r="A6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -4657,7 +4657,7 @@
     </row>
     <row r="7" spans="1:23" s="3" customFormat="1">
       <c r="A7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -4665,7 +4665,7 @@
     </row>
     <row r="8" spans="1:23" s="3" customFormat="1">
       <c r="A8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -4673,149 +4673,149 @@
     </row>
     <row r="9" spans="1:23" s="3" customFormat="1">
       <c r="A9" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="B9" s="34" t="s">
-        <v>144</v>
-      </c>
       <c r="C9" s="34" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D9" s="34" t="s">
         <v>6</v>
       </c>
       <c r="E9" s="34" t="s">
+        <v>144</v>
+      </c>
+      <c r="F9" s="34" t="s">
         <v>145</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="G9" s="34" t="s">
         <v>146</v>
       </c>
-      <c r="G9" s="34" t="s">
+      <c r="H9" s="34" t="s">
         <v>147</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="I9" s="34" t="s">
         <v>148</v>
       </c>
-      <c r="I9" s="34" t="s">
+      <c r="J9" s="34" t="s">
         <v>149</v>
       </c>
-      <c r="J9" s="34" t="s">
+      <c r="K9" s="34" t="s">
         <v>150</v>
       </c>
-      <c r="K9" s="34" t="s">
+      <c r="L9" s="34" t="s">
         <v>151</v>
       </c>
-      <c r="L9" s="34" t="s">
+      <c r="M9" s="34" t="s">
         <v>152</v>
       </c>
-      <c r="M9" s="34" t="s">
+      <c r="N9" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="N9" s="34" t="s">
+      <c r="O9" s="34" t="s">
         <v>154</v>
       </c>
-      <c r="O9" s="34" t="s">
+      <c r="P9" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="P9" s="34" t="s">
+      <c r="Q9" s="34" t="s">
         <v>156</v>
       </c>
-      <c r="Q9" s="34" t="s">
+      <c r="R9" s="34" t="s">
         <v>157</v>
       </c>
-      <c r="R9" s="34" t="s">
+      <c r="S9" s="34" t="s">
         <v>158</v>
       </c>
-      <c r="S9" s="34" t="s">
+      <c r="T9" s="34" t="s">
         <v>159</v>
       </c>
-      <c r="T9" s="34" t="s">
+      <c r="U9" s="34" t="s">
         <v>160</v>
       </c>
-      <c r="U9" s="34" t="s">
+      <c r="V9" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="V9" s="34" t="s">
+      <c r="W9" s="34" t="s">
         <v>162</v>
-      </c>
-      <c r="W9" s="34" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="10" spans="1:23" s="3" customFormat="1">
       <c r="A10" s="35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="D10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="34" t="s">
+        <v>40</v>
+      </c>
+      <c r="G10" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="D10" s="34" t="s">
+      <c r="H10" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="34" t="s">
+      <c r="I10" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="F10" s="34" t="s">
+      <c r="J10" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="I10" s="35" t="s">
-        <v>42</v>
-      </c>
-      <c r="J10" s="35" t="s">
-        <v>42</v>
-      </c>
       <c r="K10" s="35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L10" s="35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="M10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="U10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="V10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="W10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:23" s="3" customFormat="1">
       <c r="A11" s="34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="35"/>
       <c r="C11" s="34"/>
@@ -4844,12 +4844,12 @@
         <v>0</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="13" spans="1:23" s="3" customFormat="1">
       <c r="A13" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B13" s="3">
         <v>15</v>
@@ -4857,7 +4857,7 @@
     </row>
     <row r="14" spans="1:23" s="3" customFormat="1">
       <c r="A14" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B14" s="3">
         <v>29</v>
@@ -4865,7 +4865,7 @@
     </row>
     <row r="15" spans="1:23" s="3" customFormat="1">
       <c r="A15" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="3">
         <v>1</v>
@@ -4873,7 +4873,7 @@
     </row>
     <row r="16" spans="1:23" s="3" customFormat="1">
       <c r="A16" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -4881,7 +4881,7 @@
     </row>
     <row r="17" spans="1:29" s="3" customFormat="1">
       <c r="A17" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -4889,7 +4889,7 @@
     </row>
     <row r="18" spans="1:29" s="3" customFormat="1">
       <c r="A18" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="3">
         <v>0</v>
@@ -4897,7 +4897,7 @@
     </row>
     <row r="19" spans="1:29" s="3" customFormat="1">
       <c r="A19" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
@@ -4905,188 +4905,188 @@
     </row>
     <row r="20" spans="1:29" s="3" customFormat="1">
       <c r="A20" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="B20" s="34" t="s">
         <v>85</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="C20" s="34" t="s">
         <v>86</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="D20" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="E20" s="34" t="s">
         <v>88</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="F20" s="34" t="s">
         <v>89</v>
       </c>
-      <c r="F20" s="34" t="s">
+      <c r="G20" s="34" t="s">
         <v>90</v>
       </c>
-      <c r="G20" s="34" t="s">
+      <c r="H20" s="34" t="s">
         <v>91</v>
       </c>
-      <c r="H20" s="34" t="s">
+      <c r="I20" s="34" t="s">
         <v>92</v>
       </c>
-      <c r="I20" s="34" t="s">
+      <c r="J20" s="34" t="s">
         <v>93</v>
       </c>
-      <c r="J20" s="34" t="s">
+      <c r="K20" s="34" t="s">
         <v>94</v>
       </c>
-      <c r="K20" s="34" t="s">
+      <c r="L20" s="34" t="s">
         <v>95</v>
       </c>
-      <c r="L20" s="34" t="s">
+      <c r="M20" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="M20" s="34" t="s">
+      <c r="N20" s="34" t="s">
         <v>97</v>
       </c>
-      <c r="N20" s="34" t="s">
+      <c r="O20" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="O20" s="34" t="s">
+      <c r="P20" s="34" t="s">
         <v>99</v>
       </c>
-      <c r="P20" s="34" t="s">
+      <c r="Q20" s="34" t="s">
         <v>100</v>
       </c>
-      <c r="Q20" s="34" t="s">
+      <c r="R20" s="34" t="s">
         <v>101</v>
       </c>
-      <c r="R20" s="34" t="s">
+      <c r="S20" s="34" t="s">
         <v>102</v>
       </c>
-      <c r="S20" s="34" t="s">
+      <c r="T20" s="34" t="s">
         <v>103</v>
       </c>
-      <c r="T20" s="34" t="s">
+      <c r="U20" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="U20" s="34" t="s">
+      <c r="V20" s="34" t="s">
         <v>105</v>
       </c>
-      <c r="V20" s="34" t="s">
+      <c r="W20" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="W20" s="34" t="s">
+      <c r="X20" s="34" t="s">
         <v>107</v>
       </c>
-      <c r="X20" s="34" t="s">
+      <c r="Y20" s="34" t="s">
         <v>108</v>
       </c>
-      <c r="Y20" s="34" t="s">
+      <c r="Z20" s="34" t="s">
         <v>109</v>
       </c>
-      <c r="Z20" s="34" t="s">
+      <c r="AA20" s="34" t="s">
         <v>110</v>
       </c>
-      <c r="AA20" s="34" t="s">
+      <c r="AB20" s="34" t="s">
         <v>111</v>
       </c>
-      <c r="AB20" s="34" t="s">
+      <c r="AC20" s="34" t="s">
         <v>112</v>
-      </c>
-      <c r="AC20" s="34" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:29" s="3" customFormat="1">
       <c r="A21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="J21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="M21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="N21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="P21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Q21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="R21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="S21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="U21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="X21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Y21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="Z21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AA21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AB21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AC21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:29" s="3" customFormat="1">
       <c r="A22" s="34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C22" s="34"/>
       <c r="D22" s="34"/>
@@ -5167,7 +5167,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -5193,7 +5193,7 @@
     </row>
     <row r="2" spans="1:23" s="12" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" s="3">
         <v>256</v>
@@ -5222,7 +5222,7 @@
     </row>
     <row r="3" spans="1:23" s="12" customFormat="1">
       <c r="A3" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B3" s="3">
         <v>23</v>
@@ -5251,7 +5251,7 @@
     </row>
     <row r="4" spans="1:23" s="12" customFormat="1">
       <c r="A4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -5280,7 +5280,7 @@
     </row>
     <row r="5" spans="1:23" s="12" customFormat="1">
       <c r="A5" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
@@ -5309,7 +5309,7 @@
     </row>
     <row r="6" spans="1:23" s="12" customFormat="1">
       <c r="A6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -5338,7 +5338,7 @@
     </row>
     <row r="7" spans="1:23" s="12" customFormat="1">
       <c r="A7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -5367,7 +5367,7 @@
     </row>
     <row r="8" spans="1:23" s="12" customFormat="1">
       <c r="A8" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -5396,152 +5396,152 @@
     </row>
     <row r="9" spans="1:23" s="12" customFormat="1">
       <c r="A9" s="34" t="s">
+        <v>142</v>
+      </c>
+      <c r="B9" s="34" t="s">
+        <v>164</v>
+      </c>
+      <c r="C9" s="34" t="s">
         <v>143</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="D9" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="C9" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="D9" s="34" t="s">
+      <c r="E9" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="E9" s="34" t="s">
+      <c r="F9" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="F9" s="34" t="s">
+      <c r="G9" s="34" t="s">
         <v>168</v>
       </c>
-      <c r="G9" s="34" t="s">
+      <c r="H9" s="34" t="s">
         <v>169</v>
       </c>
-      <c r="H9" s="34" t="s">
+      <c r="I9" s="34" t="s">
         <v>170</v>
       </c>
-      <c r="I9" s="34" t="s">
+      <c r="J9" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="J9" s="34" t="s">
+      <c r="K9" s="34" t="s">
         <v>172</v>
       </c>
-      <c r="K9" s="34" t="s">
+      <c r="L9" s="34" t="s">
         <v>173</v>
       </c>
-      <c r="L9" s="34" t="s">
+      <c r="M9" s="34" t="s">
         <v>174</v>
       </c>
-      <c r="M9" s="34" t="s">
+      <c r="N9" s="34" t="s">
         <v>175</v>
       </c>
-      <c r="N9" s="34" t="s">
+      <c r="O9" s="34" t="s">
         <v>176</v>
       </c>
-      <c r="O9" s="34" t="s">
+      <c r="P9" s="34" t="s">
         <v>177</v>
       </c>
-      <c r="P9" s="34" t="s">
+      <c r="Q9" s="34" t="s">
         <v>178</v>
       </c>
-      <c r="Q9" s="34" t="s">
+      <c r="R9" s="34" t="s">
         <v>179</v>
       </c>
-      <c r="R9" s="34" t="s">
+      <c r="S9" s="34" t="s">
         <v>180</v>
       </c>
-      <c r="S9" s="34" t="s">
+      <c r="T9" s="34" t="s">
         <v>181</v>
       </c>
-      <c r="T9" s="34" t="s">
+      <c r="U9" s="34" t="s">
         <v>182</v>
       </c>
-      <c r="U9" s="34" t="s">
+      <c r="V9" s="34" t="s">
         <v>183</v>
       </c>
-      <c r="V9" s="34" t="s">
+      <c r="W9" s="34" t="s">
         <v>184</v>
-      </c>
-      <c r="W9" s="34" t="s">
-        <v>185</v>
       </c>
     </row>
     <row r="10" spans="1:23" s="12" customFormat="1">
       <c r="A10" s="34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="I10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="J10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="L10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="M10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="N10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="O10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="P10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="Q10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="S10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="T10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="U10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="V10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="W10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:23" s="12" customFormat="1">
       <c r="A11" s="34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C11" s="34"/>
       <c r="D11" s="34"/>
@@ -5570,7 +5570,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -5596,7 +5596,7 @@
     </row>
     <row r="13" spans="1:23" s="13" customFormat="1">
       <c r="A13" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B13" s="3">
         <v>128</v>
@@ -5625,7 +5625,7 @@
     </row>
     <row r="14" spans="1:23" s="13" customFormat="1">
       <c r="A14" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B14" s="3">
         <v>5</v>
@@ -5654,7 +5654,7 @@
     </row>
     <row r="15" spans="1:23" s="13" customFormat="1">
       <c r="A15" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="3">
         <v>0</v>
@@ -5683,7 +5683,7 @@
     </row>
     <row r="16" spans="1:23" s="13" customFormat="1">
       <c r="A16" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -5712,7 +5712,7 @@
     </row>
     <row r="17" spans="1:23" s="13" customFormat="1">
       <c r="A17" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -5741,7 +5741,7 @@
     </row>
     <row r="18" spans="1:23" s="13" customFormat="1">
       <c r="A18" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
@@ -5770,7 +5770,7 @@
     </row>
     <row r="19" spans="1:23" s="13" customFormat="1">
       <c r="A19" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
@@ -5799,44 +5799,44 @@
     </row>
     <row r="20" spans="1:23" s="13" customFormat="1">
       <c r="A20" s="34" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B20" s="34" t="s">
+        <v>187</v>
+      </c>
+      <c r="C20" s="34" t="s">
         <v>188</v>
       </c>
-      <c r="C20" s="34" t="s">
-        <v>189</v>
-      </c>
       <c r="D20" s="34" t="s">
+        <v>165</v>
+      </c>
+      <c r="E20" s="34" t="s">
         <v>166</v>
-      </c>
-      <c r="E20" s="34" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="21" spans="1:23" s="13" customFormat="1">
       <c r="A21" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:23" s="13" customFormat="1">
       <c r="A22" s="34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C22" s="34"/>
       <c r="D22" s="34"/>
@@ -5905,12 +5905,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="6" customFormat="1">
       <c r="A2" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" s="9">
         <v>8</v>
@@ -5918,7 +5918,7 @@
     </row>
     <row r="3" spans="1:4" s="6" customFormat="1">
       <c r="A3" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B3" s="9">
         <v>4</v>
@@ -5926,7 +5926,7 @@
     </row>
     <row r="4" spans="1:4" s="6" customFormat="1">
       <c r="A4" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="9">
         <v>0</v>
@@ -5934,7 +5934,7 @@
     </row>
     <row r="5" spans="1:4" s="6" customFormat="1">
       <c r="A5" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="9">
         <v>1</v>
@@ -5942,7 +5942,7 @@
     </row>
     <row r="6" spans="1:4" s="6" customFormat="1">
       <c r="A6" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="9">
         <v>0</v>
@@ -5950,7 +5950,7 @@
     </row>
     <row r="7" spans="1:4" s="6" customFormat="1">
       <c r="A7" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -5958,7 +5958,7 @@
     </row>
     <row r="8" spans="1:4" s="6" customFormat="1">
       <c r="A8" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B8" s="9">
         <v>0</v>
@@ -5966,38 +5966,38 @@
     </row>
     <row r="9" spans="1:4" s="6" customFormat="1">
       <c r="A9" s="36" t="s">
+        <v>192</v>
+      </c>
+      <c r="B9" s="36" t="s">
         <v>193</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="C9" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C9" s="36" t="s">
+      <c r="D9" s="36" t="s">
         <v>195</v>
-      </c>
-      <c r="D9" s="36" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:4" s="6" customFormat="1">
       <c r="A10" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C10" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:4" s="6" customFormat="1">
       <c r="A11" s="37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="38" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C11" s="36"/>
       <c r="D11" s="36"/>
@@ -6007,12 +6007,12 @@
         <v>0</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="13" spans="1:4" s="6" customFormat="1">
       <c r="A13" s="9" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B13" s="9">
         <v>512</v>
@@ -6020,7 +6020,7 @@
     </row>
     <row r="14" spans="1:4" s="6" customFormat="1">
       <c r="A14" s="9" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B14" s="9">
         <v>3</v>
@@ -6028,7 +6028,7 @@
     </row>
     <row r="15" spans="1:4" s="6" customFormat="1">
       <c r="A15" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="9">
         <v>0</v>
@@ -6036,7 +6036,7 @@
     </row>
     <row r="16" spans="1:4" s="6" customFormat="1">
       <c r="A16" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="9">
         <v>1</v>
@@ -6044,7 +6044,7 @@
     </row>
     <row r="17" spans="1:3" s="6" customFormat="1">
       <c r="A17" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="9">
         <v>0</v>
@@ -6052,7 +6052,7 @@
     </row>
     <row r="18" spans="1:3" s="6" customFormat="1">
       <c r="A18" s="9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
@@ -6060,7 +6060,7 @@
     </row>
     <row r="19" spans="1:3" s="6" customFormat="1">
       <c r="A19" s="9" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B19" s="9">
         <v>0</v>
@@ -6068,32 +6068,32 @@
     </row>
     <row r="20" spans="1:3" s="6" customFormat="1">
       <c r="A20" s="36" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B20" s="36" t="s">
+        <v>198</v>
+      </c>
+      <c r="C20" s="36" t="s">
         <v>199</v>
-      </c>
-      <c r="C20" s="36" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="21" spans="1:3" s="6" customFormat="1">
       <c r="A21" s="36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="36" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:3" s="6" customFormat="1">
       <c r="A22" s="37" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="38" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C22" s="36"/>
     </row>
@@ -6149,12 +6149,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B2" s="3">
         <v>128</v>
@@ -6162,7 +6162,7 @@
     </row>
     <row r="3" spans="1:6" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B3" s="3">
         <v>6</v>
@@ -6170,7 +6170,7 @@
     </row>
     <row r="4" spans="1:6" s="3" customFormat="1">
       <c r="A4" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -6178,7 +6178,7 @@
     </row>
     <row r="5" spans="1:6" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
@@ -6186,7 +6186,7 @@
     </row>
     <row r="6" spans="1:6" s="3" customFormat="1">
       <c r="A6" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -6194,7 +6194,7 @@
     </row>
     <row r="7" spans="1:6" s="3" customFormat="1">
       <c r="A7" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -6202,7 +6202,7 @@
     </row>
     <row r="8" spans="1:6" s="3" customFormat="1">
       <c r="A8" s="3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -6210,47 +6210,47 @@
     </row>
     <row r="9" spans="1:6" s="3" customFormat="1">
       <c r="A9" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="B9" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="C9" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="D9" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="D9" s="34" t="s">
-        <v>206</v>
-      </c>
       <c r="E9" s="34" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="F9" s="34" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="3" customFormat="1">
       <c r="A10" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" s="34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D10" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="E10" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="E10" s="34" t="s">
-        <v>228</v>
-      </c>
       <c r="F10" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="3" customFormat="1">
       <c r="A11" s="34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B11" s="34"/>
       <c r="C11" s="34"/>
@@ -6263,12 +6263,12 @@
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="3" customFormat="1">
       <c r="A13" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B13" s="3">
         <v>128</v>
@@ -6276,7 +6276,7 @@
     </row>
     <row r="14" spans="1:6" s="3" customFormat="1">
       <c r="A14" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B14" s="3">
         <v>6</v>
@@ -6284,7 +6284,7 @@
     </row>
     <row r="15" spans="1:6" s="3" customFormat="1">
       <c r="A15" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B15" s="3">
         <v>0</v>
@@ -6292,7 +6292,7 @@
     </row>
     <row r="16" spans="1:6" s="3" customFormat="1">
       <c r="A16" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="3">
         <v>1</v>
@@ -6300,7 +6300,7 @@
     </row>
     <row r="17" spans="1:6" s="3" customFormat="1">
       <c r="A17" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17" s="3">
         <v>1</v>
@@ -6308,7 +6308,7 @@
     </row>
     <row r="18" spans="1:6" s="3" customFormat="1">
       <c r="A18" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
@@ -6316,7 +6316,7 @@
     </row>
     <row r="19" spans="1:6" s="3" customFormat="1">
       <c r="A19" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
@@ -6324,47 +6324,47 @@
     </row>
     <row r="20" spans="1:6" s="3" customFormat="1">
       <c r="A20" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="B20" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="C20" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="D20" s="34" t="s">
         <v>205</v>
       </c>
-      <c r="D20" s="34" t="s">
+      <c r="E20" s="34" t="s">
         <v>206</v>
       </c>
-      <c r="E20" s="34" t="s">
+      <c r="F20" s="34" t="s">
         <v>207</v>
-      </c>
-      <c r="F20" s="34" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="3" customFormat="1">
       <c r="A21" s="34" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="F21" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="3" customFormat="1">
       <c r="A22" s="34" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B22" s="34"/>
       <c r="C22" s="34"/>
@@ -6398,7 +6398,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
@@ -6414,27 +6414,27 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>209</v>
+      </c>
+      <c r="C1" t="s">
         <v>210</v>
       </c>
-      <c r="C1" t="s">
-        <v>211</v>
-      </c>
       <c r="D1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>213</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bc for fighting hero id
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Player.xlsx
+++ b/_Out/NFDataCfg/Excel/Player.xlsx
@@ -1852,9 +1852,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AT10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP1" sqref="AP1:AP1048576"/>
+      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -2192,7 +2192,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L3" s="39">
         <v>0</v>
@@ -2471,8 +2471,8 @@
       <c r="J5" s="16">
         <v>0</v>
       </c>
-      <c r="K5" s="40">
-        <v>0</v>
+      <c r="K5" s="39">
+        <v>1</v>
       </c>
       <c r="L5" s="40">
         <v>0</v>
@@ -3278,7 +3278,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:T3 AQ5:AR6 V3:AJ3 J3 K6:Q6 AQ7:AT9 B7:AO9 B5:AP5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:T3 AQ5:AR6 V3:AJ3 J3 K6:Q6 AQ7:AT9 B7:AO9 B5:J5 L5:AP5">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>

</xml_diff>

<commit_message>
fix bug for hero module
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Player.xlsx
+++ b/_Out/NFDataCfg/Excel/Player.xlsx
@@ -421,7 +421,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="599" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="233">
   <si>
     <t>Id</t>
   </si>
@@ -1155,6 +1155,9 @@
   </si>
   <si>
     <t>Diamond</t>
+  </si>
+  <si>
+    <t>FightHeroCnfID</t>
   </si>
 </sst>
 </file>
@@ -1850,11 +1853,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AT10"/>
+  <dimension ref="A1:AU10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K9" sqref="K9"/>
+      <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -1868,19 +1871,19 @@
     <col min="8" max="8" width="17.6640625" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
     <col min="10" max="10" width="12.6640625" customWidth="1"/>
-    <col min="11" max="17" width="17.33203125" customWidth="1"/>
-    <col min="27" max="27" width="11.3984375" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="13.59765625" customWidth="1"/>
-    <col min="33" max="33" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="12.3984375" customWidth="1"/>
-    <col min="36" max="36" width="15.9296875" customWidth="1"/>
-    <col min="42" max="42" width="18.33203125" customWidth="1"/>
-    <col min="43" max="43" width="15.6640625" customWidth="1"/>
-    <col min="44" max="44" width="14.46484375" customWidth="1"/>
-    <col min="45" max="46" width="15.9296875" customWidth="1"/>
+    <col min="11" max="18" width="17.33203125" customWidth="1"/>
+    <col min="28" max="28" width="11.3984375" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="13.59765625" customWidth="1"/>
+    <col min="34" max="34" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="12.3984375" customWidth="1"/>
+    <col min="37" max="37" width="15.9296875" customWidth="1"/>
+    <col min="43" max="43" width="18.33203125" customWidth="1"/>
+    <col min="44" max="44" width="15.6640625" customWidth="1"/>
+    <col min="45" max="45" width="14.46484375" customWidth="1"/>
+    <col min="46" max="47" width="15.9296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46" s="25" customFormat="1">
+    <row r="1" spans="1:47" s="25" customFormat="1">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
@@ -1915,112 +1918,115 @@
         <v>215</v>
       </c>
       <c r="L1" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="M1" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="N1" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="O1" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="P1" s="28" t="s">
         <v>157</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="Q1" s="28" t="s">
         <v>158</v>
       </c>
-      <c r="Q1" s="28" t="s">
+      <c r="R1" s="28" t="s">
         <v>159</v>
       </c>
-      <c r="R1" s="28" t="s">
+      <c r="S1" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="S1" s="28" t="s">
+      <c r="T1" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="U1" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="28" t="s">
+      <c r="V1" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="V1" s="28" t="s">
+      <c r="W1" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="W1" s="28" t="s">
+      <c r="X1" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="X1" s="28" t="s">
+      <c r="Y1" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="Y1" s="28" t="s">
+      <c r="Z1" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="Z1" s="28" t="s">
+      <c r="AA1" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="AA1" s="28" t="s">
+      <c r="AB1" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="AB1" s="28" t="s">
+      <c r="AC1" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="AC1" s="28" t="s">
+      <c r="AD1" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="AD1" s="28" t="s">
+      <c r="AE1" s="28" t="s">
         <v>22</v>
       </c>
-      <c r="AE1" s="28" t="s">
+      <c r="AF1" s="28" t="s">
         <v>23</v>
       </c>
-      <c r="AF1" s="28" t="s">
+      <c r="AG1" s="28" t="s">
         <v>24</v>
       </c>
-      <c r="AG1" s="28" t="s">
+      <c r="AH1" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="AH1" s="28" t="s">
+      <c r="AI1" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="AI1" s="28" t="s">
+      <c r="AJ1" s="28" t="s">
         <v>27</v>
       </c>
-      <c r="AJ1" s="28" t="s">
+      <c r="AK1" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="AK1" s="28" t="s">
+      <c r="AL1" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="AL1" s="28" t="s">
+      <c r="AM1" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="AM1" s="28" t="s">
+      <c r="AN1" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="AN1" s="28" t="s">
+      <c r="AO1" s="28" t="s">
         <v>32</v>
       </c>
-      <c r="AO1" s="28" t="s">
+      <c r="AP1" s="28" t="s">
         <v>33</v>
       </c>
-      <c r="AP1" s="28" t="s">
+      <c r="AQ1" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="AQ1" s="25" t="s">
+      <c r="AR1" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="AR1" s="25" t="s">
+      <c r="AS1" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="AS1" s="25" t="s">
+      <c r="AT1" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="AT1" s="25" t="s">
+      <c r="AU1" s="25" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="2" spans="1:46" s="26" customFormat="1">
+    <row r="2" spans="1:47" s="26" customFormat="1">
       <c r="A2" s="29" t="s">
         <v>38</v>
       </c>
@@ -2055,7 +2061,7 @@
         <v>41</v>
       </c>
       <c r="L2" s="39" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="M2" s="39" t="s">
         <v>41</v>
@@ -2064,7 +2070,7 @@
         <v>41</v>
       </c>
       <c r="O2" s="39" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="P2" s="39" t="s">
         <v>39</v>
@@ -2072,8 +2078,8 @@
       <c r="Q2" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="3" t="s">
-        <v>40</v>
+      <c r="R2" s="39" t="s">
+        <v>39</v>
       </c>
       <c r="S2" s="3" t="s">
         <v>40</v>
@@ -2097,13 +2103,13 @@
         <v>40</v>
       </c>
       <c r="Z2" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AA2" s="3" t="s">
         <v>39</v>
       </c>
       <c r="AB2" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="AC2" s="3" t="s">
         <v>40</v>
@@ -2121,7 +2127,7 @@
         <v>40</v>
       </c>
       <c r="AH2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AI2" s="3" t="s">
         <v>41</v>
@@ -2130,7 +2136,7 @@
         <v>41</v>
       </c>
       <c r="AK2" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AL2" s="3" t="s">
         <v>40</v>
@@ -2139,28 +2145,31 @@
         <v>40</v>
       </c>
       <c r="AN2" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AO2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="AP2" s="30" t="s">
-        <v>40</v>
+      <c r="AP2" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="AQ2" s="30" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AR2" s="30" t="s">
         <v>41</v>
       </c>
       <c r="AS2" s="30" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="AT2" s="30" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="3" spans="1:46" s="26" customFormat="1">
+      <c r="AU2" s="30" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:47" s="26" customFormat="1">
       <c r="A3" s="29" t="s">
         <v>42</v>
       </c>
@@ -2195,7 +2204,7 @@
         <v>1</v>
       </c>
       <c r="L3" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="M3" s="39">
         <v>0</v>
@@ -2212,7 +2221,7 @@
       <c r="Q3" s="39">
         <v>0</v>
       </c>
-      <c r="R3" s="16">
+      <c r="R3" s="39">
         <v>0</v>
       </c>
       <c r="S3" s="16">
@@ -2221,11 +2230,11 @@
       <c r="T3" s="16">
         <v>0</v>
       </c>
-      <c r="U3" s="3">
-        <v>1</v>
-      </c>
-      <c r="V3" s="16">
-        <v>0</v>
+      <c r="U3" s="16">
+        <v>0</v>
+      </c>
+      <c r="V3" s="3">
+        <v>1</v>
       </c>
       <c r="W3" s="16">
         <v>0</v>
@@ -2269,11 +2278,11 @@
       <c r="AJ3" s="16">
         <v>0</v>
       </c>
-      <c r="AK3" s="3">
-        <v>1</v>
+      <c r="AK3" s="16">
+        <v>0</v>
       </c>
       <c r="AL3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM3" s="3">
         <v>0</v>
@@ -2284,10 +2293,10 @@
       <c r="AO3" s="3">
         <v>0</v>
       </c>
-      <c r="AP3" s="31">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="30">
+      <c r="AP3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="31">
         <v>0</v>
       </c>
       <c r="AR3" s="30">
@@ -2299,8 +2308,11 @@
       <c r="AT3" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:46" s="26" customFormat="1">
+      <c r="AU3" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" s="26" customFormat="1">
       <c r="A4" s="29" t="s">
         <v>43</v>
       </c>
@@ -2352,7 +2364,7 @@
       <c r="Q4" s="39">
         <v>1</v>
       </c>
-      <c r="R4" s="3">
+      <c r="R4" s="39">
         <v>1</v>
       </c>
       <c r="S4" s="3">
@@ -2413,22 +2425,22 @@
         <v>1</v>
       </c>
       <c r="AL4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM4" s="3">
         <v>0</v>
       </c>
       <c r="AN4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO4" s="3">
         <v>1</v>
       </c>
-      <c r="AP4" s="30">
+      <c r="AP4" s="3">
         <v>1</v>
       </c>
       <c r="AQ4" s="30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AR4" s="30">
         <v>0</v>
@@ -2439,8 +2451,11 @@
       <c r="AT4" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:46" s="26" customFormat="1">
+      <c r="AU4" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" s="26" customFormat="1">
       <c r="A5" s="29" t="s">
         <v>44</v>
       </c>
@@ -2474,8 +2489,8 @@
       <c r="K5" s="39">
         <v>1</v>
       </c>
-      <c r="L5" s="40">
-        <v>0</v>
+      <c r="L5" s="39">
+        <v>1</v>
       </c>
       <c r="M5" s="40">
         <v>0</v>
@@ -2492,7 +2507,7 @@
       <c r="Q5" s="40">
         <v>0</v>
       </c>
-      <c r="R5" s="16">
+      <c r="R5" s="40">
         <v>0</v>
       </c>
       <c r="S5" s="16">
@@ -2564,7 +2579,7 @@
       <c r="AO5" s="16">
         <v>0</v>
       </c>
-      <c r="AP5" s="31">
+      <c r="AP5" s="16">
         <v>0</v>
       </c>
       <c r="AQ5" s="31">
@@ -2573,14 +2588,17 @@
       <c r="AR5" s="31">
         <v>0</v>
       </c>
-      <c r="AS5" s="30">
+      <c r="AS5" s="31">
         <v>0</v>
       </c>
       <c r="AT5" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:46" s="26" customFormat="1">
+      <c r="AU5" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47" s="26" customFormat="1">
       <c r="A6" s="29" t="s">
         <v>45</v>
       </c>
@@ -2632,7 +2650,7 @@
       <c r="Q6" s="40">
         <v>1</v>
       </c>
-      <c r="R6" s="3">
+      <c r="R6" s="40">
         <v>1</v>
       </c>
       <c r="S6" s="3">
@@ -2704,23 +2722,26 @@
       <c r="AO6" s="3">
         <v>1</v>
       </c>
-      <c r="AP6" s="30">
-        <v>1</v>
-      </c>
-      <c r="AQ6" s="31">
-        <v>0</v>
+      <c r="AP6" s="3">
+        <v>1</v>
+      </c>
+      <c r="AQ6" s="30">
+        <v>1</v>
       </c>
       <c r="AR6" s="31">
         <v>0</v>
       </c>
-      <c r="AS6" s="30">
+      <c r="AS6" s="31">
         <v>0</v>
       </c>
       <c r="AT6" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:46" s="16" customFormat="1">
+      <c r="AU6" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" s="16" customFormat="1">
       <c r="A7" s="22" t="s">
         <v>46</v>
       </c>
@@ -2772,7 +2793,7 @@
       <c r="Q7" s="40">
         <v>0</v>
       </c>
-      <c r="R7" s="16">
+      <c r="R7" s="40">
         <v>0</v>
       </c>
       <c r="S7" s="16">
@@ -2844,7 +2865,7 @@
       <c r="AO7" s="16">
         <v>0</v>
       </c>
-      <c r="AP7" s="31">
+      <c r="AP7" s="16">
         <v>0</v>
       </c>
       <c r="AQ7" s="31">
@@ -2859,8 +2880,11 @@
       <c r="AT7" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:46" s="16" customFormat="1">
+      <c r="AU7" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" s="16" customFormat="1">
       <c r="A8" s="22" t="s">
         <v>229</v>
       </c>
@@ -2912,7 +2936,7 @@
       <c r="Q8" s="40">
         <v>0</v>
       </c>
-      <c r="R8" s="16">
+      <c r="R8" s="40">
         <v>0</v>
       </c>
       <c r="S8" s="16">
@@ -2984,7 +3008,7 @@
       <c r="AO8" s="16">
         <v>0</v>
       </c>
-      <c r="AP8" s="31">
+      <c r="AP8" s="16">
         <v>0</v>
       </c>
       <c r="AQ8" s="31">
@@ -2999,8 +3023,11 @@
       <c r="AT8" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:46" s="16" customFormat="1">
+      <c r="AU8" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" s="16" customFormat="1">
       <c r="A9" s="22" t="s">
         <v>47</v>
       </c>
@@ -3052,7 +3079,7 @@
       <c r="Q9" s="40">
         <v>0</v>
       </c>
-      <c r="R9" s="16">
+      <c r="R9" s="40">
         <v>0</v>
       </c>
       <c r="S9" s="16">
@@ -3124,7 +3151,7 @@
       <c r="AO9" s="16">
         <v>0</v>
       </c>
-      <c r="AP9" s="31">
+      <c r="AP9" s="16">
         <v>0</v>
       </c>
       <c r="AQ9" s="31">
@@ -3139,8 +3166,11 @@
       <c r="AT9" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:46" s="17" customFormat="1" ht="67.5">
+      <c r="AU9" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:47" s="17" customFormat="1" ht="67.5">
       <c r="A10" s="23" t="s">
         <v>48</v>
       </c>
@@ -3175,110 +3205,113 @@
         <v>216</v>
       </c>
       <c r="L10" s="41" t="s">
+        <v>216</v>
+      </c>
+      <c r="M10" s="41" t="s">
         <v>217</v>
       </c>
-      <c r="M10" s="41" t="s">
+      <c r="N10" s="41" t="s">
         <v>218</v>
       </c>
-      <c r="N10" s="41" t="s">
+      <c r="O10" s="41" t="s">
         <v>219</v>
       </c>
-      <c r="O10" s="41" t="s">
+      <c r="P10" s="41" t="s">
         <v>217</v>
       </c>
-      <c r="P10" s="41" t="s">
+      <c r="Q10" s="41" t="s">
         <v>218</v>
       </c>
-      <c r="Q10" s="41" t="s">
+      <c r="R10" s="41" t="s">
         <v>219</v>
       </c>
-      <c r="R10" s="24" t="s">
+      <c r="S10" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="S10" s="24" t="s">
+      <c r="T10" s="24" t="s">
         <v>60</v>
       </c>
-      <c r="T10" s="24" t="s">
+      <c r="U10" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="U10" s="24" t="s">
+      <c r="V10" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="V10" s="24" t="s">
+      <c r="W10" s="24" t="s">
         <v>62</v>
       </c>
-      <c r="W10" s="24" t="s">
+      <c r="X10" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="X10" s="24" t="s">
+      <c r="Y10" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="Y10" s="24" t="s">
+      <c r="Z10" s="24" t="s">
         <v>65</v>
       </c>
-      <c r="Z10" s="24" t="s">
+      <c r="AA10" s="24" t="s">
         <v>66</v>
       </c>
-      <c r="AA10" s="24" t="s">
+      <c r="AB10" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="AB10" s="24" t="s">
+      <c r="AC10" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="AC10" s="24" t="s">
+      <c r="AD10" s="24" t="s">
         <v>69</v>
       </c>
-      <c r="AD10" s="24" t="s">
+      <c r="AE10" s="24" t="s">
         <v>70</v>
       </c>
-      <c r="AE10" s="24" t="s">
+      <c r="AF10" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="AF10" s="24" t="s">
+      <c r="AG10" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="AG10" s="24" t="s">
+      <c r="AH10" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="AH10" s="24" t="s">
+      <c r="AI10" s="24" t="s">
         <v>74</v>
       </c>
-      <c r="AI10" s="24" t="s">
+      <c r="AJ10" s="24" t="s">
         <v>75</v>
       </c>
-      <c r="AJ10" s="24" t="s">
+      <c r="AK10" s="24" t="s">
         <v>76</v>
       </c>
-      <c r="AK10" s="24" t="s">
+      <c r="AL10" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="AL10" s="24" t="s">
+      <c r="AM10" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="AM10" s="24" t="s">
+      <c r="AN10" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="AN10" s="24" t="s">
+      <c r="AO10" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="AO10" s="24" t="s">
+      <c r="AP10" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="AP10" s="32" t="s">
+      <c r="AQ10" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="AQ10" s="32" t="s">
+      <c r="AR10" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="AR10" s="32" t="s">
+      <c r="AS10" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="AS10" s="33"/>
       <c r="AT10" s="33"/>
+      <c r="AU10" s="33"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="R3:T3 AQ5:AR6 V3:AJ3 J3 K6:Q6 AQ7:AT9 B7:AO9 B5:J5 L5:AP5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="S3:U3 AR5:AS6 W3:AK3 J3 AR7:AU9 M5:AQ5 B5:J5 K6:R6 B7:AP9">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>

</xml_diff>

<commit_message>
remove unused protocol file add building/remove building save building's data when player offline
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Player.xlsx
+++ b/_Out/NFDataCfg/Excel/Player.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="10343"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21495" windowHeight="10343" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
     <sheet name="Component" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Record_Building!$E$1:$E$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Record_Building!$D$1:$D$22</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="1" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="4" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
     <definedName name="LOCAL_MYSQL_DATE_FORMAT" localSheetId="3" hidden="1">REPT(LOCAL_YEAR_FORMAT,4)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_MONTH_FORMAT,2)&amp;LOCAL_DATE_SEPARATOR&amp;REPT(LOCAL_DAY_FORMAT,2)&amp;" "&amp;REPT(LOCAL_HOUR_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_MINUTE_FORMAT,2)&amp;LOCAL_TIME_SEPARATOR&amp;REPT(LOCAL_SECOND_FORMAT,2)</definedName>
@@ -421,7 +421,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="602" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="230">
   <si>
     <t>Id</t>
   </si>
@@ -1067,21 +1067,12 @@
     <t>BuildingList</t>
   </si>
   <si>
-    <t>BuildingID</t>
-  </si>
-  <si>
     <t>BuildingGUID</t>
   </si>
   <si>
     <t>State</t>
   </si>
   <si>
-    <t>PosX</t>
-  </si>
-  <si>
-    <t>PosY</t>
-  </si>
-  <si>
     <t>StateEndTime</t>
   </si>
   <si>
@@ -1139,9 +1130,6 @@
     <t>Pos</t>
   </si>
   <si>
-    <t>float</t>
-  </si>
-  <si>
     <t>vector3</t>
   </si>
   <si>
@@ -1158,6 +1146,9 @@
   </si>
   <si>
     <t>FightHeroCnfID</t>
+  </si>
+  <si>
+    <t>BuildingCnfID</t>
   </si>
 </sst>
 </file>
@@ -1855,7 +1846,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+    <sheetView topLeftCell="I1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="L3" sqref="L3"/>
     </sheetView>
@@ -1915,19 +1906,19 @@
         <v>9</v>
       </c>
       <c r="K1" s="28" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="L1" s="28" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="M1" s="28" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="N1" s="28" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="O1" s="28" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="P1" s="28" t="s">
         <v>157</v>
@@ -1960,7 +1951,7 @@
         <v>17</v>
       </c>
       <c r="Z1" s="28" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="AA1" s="28" t="s">
         <v>18</v>
@@ -2886,7 +2877,7 @@
     </row>
     <row r="8" spans="1:47" s="16" customFormat="1">
       <c r="A8" s="22" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B8" s="16">
         <v>0</v>
@@ -3202,28 +3193,28 @@
         <v>57</v>
       </c>
       <c r="K10" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="L10" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="M10" s="41" t="s">
+        <v>214</v>
+      </c>
+      <c r="N10" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="O10" s="41" t="s">
         <v>216</v>
       </c>
-      <c r="L10" s="41" t="s">
+      <c r="P10" s="41" t="s">
+        <v>214</v>
+      </c>
+      <c r="Q10" s="41" t="s">
+        <v>215</v>
+      </c>
+      <c r="R10" s="41" t="s">
         <v>216</v>
-      </c>
-      <c r="M10" s="41" t="s">
-        <v>217</v>
-      </c>
-      <c r="N10" s="41" t="s">
-        <v>218</v>
-      </c>
-      <c r="O10" s="41" t="s">
-        <v>219</v>
-      </c>
-      <c r="P10" s="41" t="s">
-        <v>217</v>
-      </c>
-      <c r="Q10" s="41" t="s">
-        <v>218</v>
-      </c>
-      <c r="R10" s="41" t="s">
-        <v>219</v>
       </c>
       <c r="S10" s="24" t="s">
         <v>59</v>
@@ -3981,7 +3972,7 @@
     </row>
     <row r="8" spans="1:30" s="16" customFormat="1">
       <c r="A8" s="22" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B8" s="16">
         <v>0</v>
@@ -4312,7 +4303,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1">
@@ -4554,7 +4545,7 @@
         <v>48</v>
       </c>
       <c r="B11" s="35" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="C11" s="34"/>
       <c r="D11" s="34"/>
@@ -4712,7 +4703,7 @@
         <v>143</v>
       </c>
       <c r="C9" s="34" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D9" s="34" t="s">
         <v>6</v>
@@ -4877,7 +4868,7 @@
         <v>0</v>
       </c>
       <c r="B12" s="10" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:23" s="3" customFormat="1">
@@ -5119,7 +5110,7 @@
         <v>48</v>
       </c>
       <c r="B22" s="35" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C22" s="34"/>
       <c r="D22" s="34"/>
@@ -6154,10 +6145,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F22"/>
+  <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -6165,19 +6156,18 @@
     <col min="1" max="1" width="16.19921875" style="4" customWidth="1"/>
     <col min="2" max="2" width="21.19921875" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.19921875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="10.46484375" style="4" customWidth="1"/>
-    <col min="5" max="5" width="11.6640625" style="4" customWidth="1"/>
-    <col min="6" max="6" width="13.59765625" style="4" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="9" style="4"/>
-    <col min="9" max="9" width="12.6640625" style="4" customWidth="1"/>
-    <col min="10" max="10" width="13.796875" style="4" customWidth="1"/>
-    <col min="11" max="11" width="9" style="4"/>
-    <col min="12" max="12" width="11.6640625" style="4" customWidth="1"/>
-    <col min="13" max="13" width="13.796875" style="4" customWidth="1"/>
-    <col min="14" max="16384" width="9" style="4"/>
+    <col min="4" max="4" width="11.6640625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="13.59765625" style="4" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="9" style="4"/>
+    <col min="8" max="8" width="12.6640625" style="4" customWidth="1"/>
+    <col min="9" max="9" width="13.796875" style="4" customWidth="1"/>
+    <col min="10" max="10" width="9" style="4"/>
+    <col min="11" max="11" width="11.6640625" style="4" customWidth="1"/>
+    <col min="12" max="12" width="13.796875" style="4" customWidth="1"/>
+    <col min="13" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="2" customFormat="1">
+    <row r="1" spans="1:5" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6185,7 +6175,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:6" s="3" customFormat="1">
+    <row r="2" spans="1:5" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>140</v>
       </c>
@@ -6193,15 +6183,15 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:6" s="3" customFormat="1">
+    <row r="3" spans="1:5" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>141</v>
       </c>
       <c r="B3" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" s="3" customFormat="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" s="3" customFormat="1">
       <c r="A4" s="3" t="s">
         <v>42</v>
       </c>
@@ -6209,7 +6199,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" s="3" customFormat="1">
+    <row r="5" spans="1:5" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>43</v>
       </c>
@@ -6217,7 +6207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" s="3" customFormat="1">
+    <row r="6" spans="1:5" s="3" customFormat="1">
       <c r="A6" s="3" t="s">
         <v>44</v>
       </c>
@@ -6225,7 +6215,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" s="3" customFormat="1">
+    <row r="7" spans="1:5" s="3" customFormat="1">
       <c r="A7" s="3" t="s">
         <v>45</v>
       </c>
@@ -6233,7 +6223,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:6" s="3" customFormat="1">
+    <row r="8" spans="1:5" s="3" customFormat="1">
       <c r="A8" s="3" t="s">
         <v>189</v>
       </c>
@@ -6241,27 +6231,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:6" s="3" customFormat="1">
+    <row r="9" spans="1:5" s="3" customFormat="1">
       <c r="A9" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="B9" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="B9" s="34" t="s">
+      <c r="C9" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="C9" s="34" t="s">
+      <c r="D9" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="E9" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="D9" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="E9" s="34" t="s">
-        <v>225</v>
-      </c>
-      <c r="F9" s="34" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" s="3" customFormat="1">
+    </row>
+    <row r="10" spans="1:5" s="3" customFormat="1">
       <c r="A10" s="34" t="s">
         <v>39</v>
       </c>
@@ -6272,16 +6259,13 @@
         <v>40</v>
       </c>
       <c r="D10" s="34" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E10" s="34" t="s">
-        <v>227</v>
-      </c>
-      <c r="F10" s="34" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" s="3" customFormat="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" s="3" customFormat="1">
       <c r="A11" s="34" t="s">
         <v>48</v>
       </c>
@@ -6289,17 +6273,16 @@
       <c r="C11" s="34"/>
       <c r="D11" s="34"/>
       <c r="E11" s="34"/>
-      <c r="F11" s="34"/>
-    </row>
-    <row r="12" spans="1:6" s="2" customFormat="1">
+    </row>
+    <row r="12" spans="1:5" s="2" customFormat="1">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>208</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" s="3" customFormat="1">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="3" customFormat="1">
       <c r="A13" s="3" t="s">
         <v>140</v>
       </c>
@@ -6307,15 +6290,15 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:6" s="3" customFormat="1">
+    <row r="14" spans="1:5" s="3" customFormat="1">
       <c r="A14" s="3" t="s">
         <v>141</v>
       </c>
       <c r="B14" s="3">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" s="3" customFormat="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" s="3" customFormat="1">
       <c r="A15" s="3" t="s">
         <v>42</v>
       </c>
@@ -6323,7 +6306,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:6" s="3" customFormat="1">
+    <row r="16" spans="1:5" s="3" customFormat="1">
       <c r="A16" s="3" t="s">
         <v>43</v>
       </c>
@@ -6331,7 +6314,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:6" s="3" customFormat="1">
+    <row r="17" spans="1:5" s="3" customFormat="1">
       <c r="A17" s="3" t="s">
         <v>44</v>
       </c>
@@ -6339,7 +6322,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:6" s="3" customFormat="1">
+    <row r="18" spans="1:5" s="3" customFormat="1">
       <c r="A18" s="3" t="s">
         <v>45</v>
       </c>
@@ -6347,7 +6330,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:6" s="3" customFormat="1">
+    <row r="19" spans="1:5" s="3" customFormat="1">
       <c r="A19" s="3" t="s">
         <v>47</v>
       </c>
@@ -6355,27 +6338,24 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:6" s="3" customFormat="1">
+    <row r="20" spans="1:5" s="3" customFormat="1">
       <c r="A20" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="B20" s="34" t="s">
         <v>202</v>
       </c>
-      <c r="B20" s="34" t="s">
+      <c r="C20" s="34" t="s">
         <v>203</v>
       </c>
-      <c r="C20" s="34" t="s">
+      <c r="D20" s="34" t="s">
+        <v>222</v>
+      </c>
+      <c r="E20" s="34" t="s">
         <v>204</v>
       </c>
-      <c r="D20" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="E20" s="34" t="s">
-        <v>206</v>
-      </c>
-      <c r="F20" s="34" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" s="3" customFormat="1">
+    </row>
+    <row r="21" spans="1:5" s="3" customFormat="1">
       <c r="A21" s="34" t="s">
         <v>39</v>
       </c>
@@ -6386,16 +6366,13 @@
         <v>40</v>
       </c>
       <c r="D21" s="34" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="E21" s="34" t="s">
-        <v>226</v>
-      </c>
-      <c r="F21" s="34" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" s="3" customFormat="1">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" s="3" customFormat="1">
       <c r="A22" s="34" t="s">
         <v>48</v>
       </c>
@@ -6403,15 +6380,14 @@
       <c r="C22" s="34"/>
       <c r="D22" s="34"/>
       <c r="E22" s="34"/>
-      <c r="F22" s="34"/>
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6:B8 B18:B19 G1:G1048576 A15:B17 A4:B5 D12:D19 D22:D1048576 F1:F8 F11:F19 F22:F1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6:B8 B18:B19 F1:F1048576 A15:B17 A4:B5 E1:E8 E11:E19 E22:E1048576">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A9:B9 A20:B20 I40:I1048576 D20 D9"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A10:B10 A21:B21 I1:I39 D21 D10">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A9:B9 H40:H1048576 A20:B20"/>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A10:B10 A21:B21 H1:H39">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C21">
@@ -6447,10 +6423,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="C1" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="D1" t="s">
         <v>48</v>
@@ -6458,16 +6434,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added property fr opponent added a new interface for co (but not implement)
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Player.xlsx
+++ b/_Out/NFDataCfg/Excel/Player.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18528"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/James/Desktop/NoahGameFrame/_Out/NFDataCfg/Excel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\James\Desktop\NoahGameFrame\_Out\NFDataCfg\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28040" windowHeight="17540"/>
+    <workbookView xWindow="0" yWindow="458" windowWidth="28043" windowHeight="17543" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -42,12 +42,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>pengbo.yang</author>
   </authors>
   <commentList>
-    <comment ref="D9" authorId="0">
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000001000000}">
       <text>
         <r>
           <rPr>
@@ -59,7 +59,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0">
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000002000000}">
       <text>
         <r>
           <rPr>
@@ -71,7 +71,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0">
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000003000000}">
       <text>
         <r>
           <rPr>
@@ -83,7 +83,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G9" authorId="0">
+    <comment ref="G9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000004000000}">
       <text>
         <r>
           <rPr>
@@ -95,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H9" authorId="0">
+    <comment ref="H9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000005000000}">
       <text>
         <r>
           <rPr>
@@ -107,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I9" authorId="0">
+    <comment ref="I9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000006000000}">
       <text>
         <r>
           <rPr>
@@ -119,7 +119,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J9" authorId="0">
+    <comment ref="J9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000007000000}">
       <text>
         <r>
           <rPr>
@@ -131,7 +131,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K9" authorId="0">
+    <comment ref="K9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0200-000008000000}">
       <text>
         <r>
           <rPr>
@@ -148,12 +148,12 @@
 </file>
 
 <file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>pengbo.yang</author>
   </authors>
   <commentList>
-    <comment ref="B9" authorId="0">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000001000000}">
       <text>
         <r>
           <rPr>
@@ -165,7 +165,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="0">
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000002000000}">
       <text>
         <r>
           <rPr>
@@ -177,7 +177,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E9" authorId="0">
+    <comment ref="E9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000003000000}">
       <text>
         <r>
           <rPr>
@@ -189,7 +189,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F9" authorId="0">
+    <comment ref="F9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000004000000}">
       <text>
         <r>
           <rPr>
@@ -201,7 +201,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D20" authorId="0">
+    <comment ref="D20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000005000000}">
       <text>
         <r>
           <rPr>
@@ -213,7 +213,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E20" authorId="0">
+    <comment ref="E20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000006000000}">
       <text>
         <r>
           <rPr>
@@ -225,7 +225,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F20" authorId="0">
+    <comment ref="F20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000007000000}">
       <text>
         <r>
           <rPr>
@@ -237,7 +237,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G20" authorId="0">
+    <comment ref="G20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000008000000}">
       <text>
         <r>
           <rPr>
@@ -249,7 +249,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H20" authorId="0">
+    <comment ref="H20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-000009000000}">
       <text>
         <r>
           <rPr>
@@ -261,7 +261,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I20" authorId="0">
+    <comment ref="I20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000A000000}">
       <text>
         <r>
           <rPr>
@@ -273,7 +273,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="J20" authorId="0">
+    <comment ref="J20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000B000000}">
       <text>
         <r>
           <rPr>
@@ -285,7 +285,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K20" authorId="0">
+    <comment ref="K20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0300-00000C000000}">
       <text>
         <r>
           <rPr>
@@ -302,12 +302,12 @@
 </file>
 
 <file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>pengbo.yang</author>
   </authors>
   <commentList>
-    <comment ref="A9" authorId="0">
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000001000000}">
       <text>
         <r>
           <rPr>
@@ -319,7 +319,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B9" authorId="0">
+    <comment ref="B9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000002000000}">
       <text>
         <r>
           <rPr>
@@ -331,7 +331,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C9" authorId="0">
+    <comment ref="C9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000003000000}">
       <text>
         <r>
           <rPr>
@@ -343,7 +343,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D9" authorId="0">
+    <comment ref="D9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000004000000}">
       <text>
         <r>
           <rPr>
@@ -355,7 +355,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0">
+    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000005000000}">
       <text>
         <r>
           <rPr>
@@ -367,7 +367,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B20" authorId="0">
+    <comment ref="B20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000006000000}">
       <text>
         <r>
           <rPr>
@@ -379,7 +379,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C20" authorId="0">
+    <comment ref="C20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0500-000007000000}">
       <text>
         <r>
           <rPr>
@@ -396,12 +396,12 @@
 </file>
 
 <file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>pengbo.yang</author>
   </authors>
   <commentList>
-    <comment ref="A9" authorId="0">
+    <comment ref="A9" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000001000000}">
       <text>
         <r>
           <rPr>
@@ -413,7 +413,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A20" authorId="0">
+    <comment ref="A20" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0600-000002000000}">
       <text>
         <r>
           <rPr>
@@ -430,7 +430,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="607" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="655" uniqueCount="248">
   <si>
     <t>Id</t>
   </si>
@@ -1165,12 +1165,60 @@
   <si>
     <t>FightOpponent</t>
   </si>
+  <si>
+    <t>OpponentHeroPos1</t>
+  </si>
+  <si>
+    <t>OpponentHeroPos2</t>
+  </si>
+  <si>
+    <t>OpponentHeroPos3</t>
+  </si>
+  <si>
+    <t>Cup</t>
+  </si>
+  <si>
+    <t>OpponentCup</t>
+  </si>
+  <si>
+    <t>OpponentName</t>
+  </si>
+  <si>
+    <t>OpponentHead</t>
+  </si>
+  <si>
+    <t>HeroPos3Star</t>
+  </si>
+  <si>
+    <t>HeroPos2Star</t>
+  </si>
+  <si>
+    <t>HeroPos1Star</t>
+  </si>
+  <si>
+    <t>EnemyHeroPos1Star</t>
+  </si>
+  <si>
+    <t>EnemyHeroPos2Star</t>
+  </si>
+  <si>
+    <t>EnemyHeroPos3Star</t>
+  </si>
+  <si>
+    <t>HeroPos1CnfID</t>
+  </si>
+  <si>
+    <t>HeroPos2CnfID</t>
+  </si>
+  <si>
+    <t>HeroPos3CnfID</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
@@ -1514,7 +1562,7 @@
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium7">
-    <tableStyle name="MySqlDefault" count="2">
+    <tableStyle name="MySqlDefault" count="2" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
       <tableStyleElement type="wholeTable" dxfId="1"/>
       <tableStyleElement type="headerRow" dxfId="0"/>
     </tableStyle>
@@ -1858,38 +1906,41 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AR10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:BH10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AQ6" sqref="AQ6"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <pane ySplit="10" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AS2" sqref="AS2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="23.83203125" customWidth="1"/>
-    <col min="2" max="2" width="8.1640625" customWidth="1"/>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="1" max="1" width="23.796875" customWidth="1"/>
+    <col min="2" max="2" width="8.1328125" customWidth="1"/>
+    <col min="3" max="3" width="10.46484375" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="6" max="6" width="8.1640625" customWidth="1"/>
+    <col min="6" max="6" width="8.1328125" customWidth="1"/>
     <col min="7" max="7" width="9.33203125" customWidth="1"/>
     <col min="8" max="8" width="17.6640625" customWidth="1"/>
     <col min="9" max="9" width="19" customWidth="1"/>
     <col min="10" max="10" width="12.6640625" customWidth="1"/>
-    <col min="11" max="15" width="17.33203125" customWidth="1"/>
-    <col min="25" max="25" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="13.6640625" customWidth="1"/>
-    <col min="31" max="31" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="12.33203125" customWidth="1"/>
-    <col min="34" max="34" width="16" customWidth="1"/>
-    <col min="40" max="40" width="18.33203125" customWidth="1"/>
-    <col min="41" max="41" width="15.6640625" customWidth="1"/>
-    <col min="42" max="42" width="14.5" customWidth="1"/>
-    <col min="43" max="44" width="16" customWidth="1"/>
+    <col min="20" max="20" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13.6640625" customWidth="1"/>
+    <col min="26" max="26" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="12.33203125" customWidth="1"/>
+    <col min="29" max="29" width="16" customWidth="1"/>
+    <col min="35" max="36" width="18.33203125" customWidth="1"/>
+    <col min="37" max="47" width="17.33203125" customWidth="1"/>
+    <col min="48" max="48" width="15.6640625" customWidth="1"/>
+    <col min="49" max="49" width="14.46484375" customWidth="1"/>
+    <col min="50" max="51" width="16" customWidth="1"/>
+    <col min="52" max="54" width="17.33203125" customWidth="1"/>
+    <col min="55" max="57" width="18.33203125" customWidth="1"/>
+    <col min="58" max="60" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44" s="25" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:60" s="25" customFormat="1">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
@@ -1921,109 +1972,157 @@
         <v>9</v>
       </c>
       <c r="K1" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="R1" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="S1" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="28" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="28" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="28" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" s="28" t="s">
+        <v>5</v>
+      </c>
+      <c r="AJ1" s="28" t="s">
+        <v>235</v>
+      </c>
+      <c r="AK1" s="28" t="s">
         <v>210</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="AL1" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="AM1" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="AN1" s="28" t="s">
         <v>216</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="AO1" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="P1" s="28" t="s">
-        <v>11</v>
-      </c>
-      <c r="Q1" s="28" t="s">
-        <v>12</v>
-      </c>
-      <c r="R1" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="S1" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="T1" s="28" t="s">
-        <v>15</v>
-      </c>
-      <c r="U1" s="28" t="s">
-        <v>16</v>
-      </c>
-      <c r="V1" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="W1" s="28" t="s">
-        <v>225</v>
-      </c>
-      <c r="X1" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="Y1" s="28" t="s">
-        <v>19</v>
-      </c>
-      <c r="Z1" s="28" t="s">
-        <v>20</v>
-      </c>
-      <c r="AA1" s="28" t="s">
-        <v>21</v>
-      </c>
-      <c r="AB1" s="28" t="s">
-        <v>22</v>
-      </c>
-      <c r="AC1" s="28" t="s">
-        <v>23</v>
-      </c>
-      <c r="AD1" s="28" t="s">
-        <v>24</v>
-      </c>
-      <c r="AE1" s="28" t="s">
-        <v>25</v>
-      </c>
-      <c r="AF1" s="28" t="s">
-        <v>26</v>
-      </c>
-      <c r="AG1" s="28" t="s">
-        <v>27</v>
-      </c>
-      <c r="AH1" s="28" t="s">
-        <v>28</v>
-      </c>
-      <c r="AI1" s="28" t="s">
-        <v>29</v>
-      </c>
-      <c r="AJ1" s="28" t="s">
-        <v>30</v>
-      </c>
-      <c r="AK1" s="28" t="s">
-        <v>31</v>
-      </c>
-      <c r="AL1" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="AM1" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="AN1" s="28" t="s">
-        <v>5</v>
-      </c>
-      <c r="AO1" s="25" t="s">
+      <c r="AP1" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="AQ1" s="28" t="s">
+        <v>246</v>
+      </c>
+      <c r="AR1" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="AS1" s="28" t="s">
+        <v>241</v>
+      </c>
+      <c r="AT1" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="AU1" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="AV1" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="AP1" s="25" t="s">
+      <c r="AW1" s="25" t="s">
         <v>231</v>
       </c>
-      <c r="AQ1" s="25" t="s">
+      <c r="AX1" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="AR1" s="25" t="s">
+      <c r="AY1" s="25" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="2" spans="1:44" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="AZ1" s="28" t="s">
+        <v>232</v>
+      </c>
+      <c r="BA1" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="BB1" s="28" t="s">
+        <v>234</v>
+      </c>
+      <c r="BC1" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="BD1" s="28" t="s">
+        <v>237</v>
+      </c>
+      <c r="BE1" s="28" t="s">
+        <v>238</v>
+      </c>
+      <c r="BF1" s="28" t="s">
+        <v>242</v>
+      </c>
+      <c r="BG1" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="BH1" s="28" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="2" spans="1:60" s="26" customFormat="1">
       <c r="A2" s="29" t="s">
         <v>36</v>
       </c>
@@ -2054,63 +2153,63 @@
       <c r="J2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="K2" s="39" t="s">
+      <c r="K2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="AA2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="39" t="s">
-        <v>37</v>
-      </c>
-      <c r="M2" s="39" t="s">
+      <c r="AB2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="39" t="s">
+      <c r="AC2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="O2" s="39" t="s">
-        <v>39</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="U2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="V2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AB2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>38</v>
-      </c>
       <c r="AD2" s="3" t="s">
         <v>38</v>
       </c>
@@ -2118,7 +2217,7 @@
         <v>38</v>
       </c>
       <c r="AF2" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="AG2" s="3" t="s">
         <v>39</v>
@@ -2132,32 +2231,80 @@
       <c r="AJ2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AK2" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="AL2" s="3" t="s">
+      <c r="AK2" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AL2" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM2" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="AN2" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="AO2" s="30" t="s">
+      <c r="AN2" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="AP2" s="30" t="s">
+      <c r="AO2" s="39" t="s">
         <v>39</v>
       </c>
-      <c r="AQ2" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="AR2" s="30" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:44" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="AP2" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AQ2" s="39" t="s">
+        <v>39</v>
+      </c>
+      <c r="AR2" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AS2" s="39" t="s">
+        <v>37</v>
+      </c>
+      <c r="AT2" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="AU2" s="39" t="s">
+        <v>38</v>
+      </c>
+      <c r="AV2" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="AW2" s="30" t="s">
+        <v>39</v>
+      </c>
+      <c r="AX2" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="AY2" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="AZ2" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="BA2" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="BB2" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="BC2" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="BD2" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="BE2" s="30" t="s">
+        <v>37</v>
+      </c>
+      <c r="BF2" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="BG2" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="BH2" s="30" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:60" s="26" customFormat="1">
       <c r="A3" s="29" t="s">
         <v>40</v>
       </c>
@@ -2188,19 +2335,19 @@
       <c r="J3" s="16">
         <v>0</v>
       </c>
-      <c r="K3" s="39">
-        <v>1</v>
-      </c>
-      <c r="L3" s="39">
-        <v>1</v>
-      </c>
-      <c r="M3" s="39">
-        <v>0</v>
-      </c>
-      <c r="N3" s="39">
-        <v>0</v>
-      </c>
-      <c r="O3" s="39">
+      <c r="K3" s="16">
+        <v>0</v>
+      </c>
+      <c r="L3" s="16">
+        <v>0</v>
+      </c>
+      <c r="M3" s="16">
+        <v>0</v>
+      </c>
+      <c r="N3" s="3">
+        <v>1</v>
+      </c>
+      <c r="O3" s="16">
         <v>0</v>
       </c>
       <c r="P3" s="16">
@@ -2212,8 +2359,8 @@
       <c r="R3" s="16">
         <v>0</v>
       </c>
-      <c r="S3" s="3">
-        <v>1</v>
+      <c r="S3" s="16">
+        <v>0</v>
       </c>
       <c r="T3" s="16">
         <v>0</v>
@@ -2245,53 +2392,101 @@
       <c r="AC3" s="16">
         <v>0</v>
       </c>
-      <c r="AD3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="16">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="3">
-        <v>1</v>
-      </c>
-      <c r="AJ3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="31">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="30">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="30">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="30">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:44" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="AD3" s="3">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="16">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="16">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="39">
+        <v>1</v>
+      </c>
+      <c r="AL3" s="39">
+        <v>1</v>
+      </c>
+      <c r="AM3" s="39">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="39">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="39">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="39">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="39">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="39">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="39">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="39">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="39">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AW3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AX3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AY3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AZ3" s="30">
+        <v>0</v>
+      </c>
+      <c r="BA3" s="30">
+        <v>0</v>
+      </c>
+      <c r="BB3" s="30">
+        <v>0</v>
+      </c>
+      <c r="BC3" s="31">
+        <v>0</v>
+      </c>
+      <c r="BD3" s="31">
+        <v>0</v>
+      </c>
+      <c r="BE3" s="31">
+        <v>0</v>
+      </c>
+      <c r="BF3" s="30">
+        <v>0</v>
+      </c>
+      <c r="BG3" s="30">
+        <v>0</v>
+      </c>
+      <c r="BH3" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:60" s="26" customFormat="1">
       <c r="A4" s="29" t="s">
         <v>41</v>
       </c>
@@ -2322,19 +2517,19 @@
       <c r="J4" s="3">
         <v>1</v>
       </c>
-      <c r="K4" s="39">
-        <v>1</v>
-      </c>
-      <c r="L4" s="39">
-        <v>1</v>
-      </c>
-      <c r="M4" s="39">
-        <v>1</v>
-      </c>
-      <c r="N4" s="39">
-        <v>1</v>
-      </c>
-      <c r="O4" s="39">
+      <c r="K4" s="3">
+        <v>1</v>
+      </c>
+      <c r="L4" s="3">
+        <v>1</v>
+      </c>
+      <c r="M4" s="3">
+        <v>1</v>
+      </c>
+      <c r="N4" s="3">
+        <v>1</v>
+      </c>
+      <c r="O4" s="3">
         <v>1</v>
       </c>
       <c r="P4" s="3">
@@ -2383,10 +2578,10 @@
         <v>1</v>
       </c>
       <c r="AE4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF4" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG4" s="3">
         <v>1</v>
@@ -2398,34 +2593,82 @@
         <v>1</v>
       </c>
       <c r="AJ4" s="3">
-        <v>0</v>
-      </c>
-      <c r="AK4" s="3">
-        <v>0</v>
-      </c>
-      <c r="AL4" s="3">
-        <v>1</v>
-      </c>
-      <c r="AM4" s="3">
-        <v>1</v>
-      </c>
-      <c r="AN4" s="30">
-        <v>1</v>
-      </c>
-      <c r="AO4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AP4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AQ4" s="30">
-        <v>0</v>
-      </c>
-      <c r="AR4" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:44" s="26" customFormat="1" x14ac:dyDescent="0.15">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="39">
+        <v>1</v>
+      </c>
+      <c r="AL4" s="39">
+        <v>1</v>
+      </c>
+      <c r="AM4" s="39">
+        <v>1</v>
+      </c>
+      <c r="AN4" s="39">
+        <v>1</v>
+      </c>
+      <c r="AO4" s="39">
+        <v>1</v>
+      </c>
+      <c r="AP4" s="39">
+        <v>1</v>
+      </c>
+      <c r="AQ4" s="39">
+        <v>1</v>
+      </c>
+      <c r="AR4" s="39">
+        <v>1</v>
+      </c>
+      <c r="AS4" s="39">
+        <v>1</v>
+      </c>
+      <c r="AT4" s="39">
+        <v>1</v>
+      </c>
+      <c r="AU4" s="39">
+        <v>1</v>
+      </c>
+      <c r="AV4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AW4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AX4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AY4" s="30">
+        <v>0</v>
+      </c>
+      <c r="AZ4" s="30">
+        <v>1</v>
+      </c>
+      <c r="BA4" s="30">
+        <v>1</v>
+      </c>
+      <c r="BB4" s="30">
+        <v>1</v>
+      </c>
+      <c r="BC4" s="30">
+        <v>1</v>
+      </c>
+      <c r="BD4" s="30">
+        <v>1</v>
+      </c>
+      <c r="BE4" s="30">
+        <v>1</v>
+      </c>
+      <c r="BF4" s="30">
+        <v>1</v>
+      </c>
+      <c r="BG4" s="30">
+        <v>1</v>
+      </c>
+      <c r="BH4" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:60" s="26" customFormat="1">
       <c r="A5" s="29" t="s">
         <v>42</v>
       </c>
@@ -2456,19 +2699,19 @@
       <c r="J5" s="16">
         <v>0</v>
       </c>
-      <c r="K5" s="39">
-        <v>1</v>
-      </c>
-      <c r="L5" s="39">
-        <v>1</v>
-      </c>
-      <c r="M5" s="40">
-        <v>0</v>
-      </c>
-      <c r="N5" s="40">
-        <v>0</v>
-      </c>
-      <c r="O5" s="40">
+      <c r="K5" s="16">
+        <v>0</v>
+      </c>
+      <c r="L5" s="16">
+        <v>0</v>
+      </c>
+      <c r="M5" s="16">
+        <v>0</v>
+      </c>
+      <c r="N5" s="16">
+        <v>0</v>
+      </c>
+      <c r="O5" s="16">
         <v>0</v>
       </c>
       <c r="P5" s="16">
@@ -2534,32 +2777,80 @@
       <c r="AJ5" s="16">
         <v>0</v>
       </c>
-      <c r="AK5" s="16">
-        <v>0</v>
-      </c>
-      <c r="AL5" s="16">
-        <v>0</v>
-      </c>
-      <c r="AM5" s="16">
-        <v>0</v>
-      </c>
-      <c r="AN5" s="31">
-        <v>0</v>
-      </c>
-      <c r="AO5" s="31">
-        <v>0</v>
-      </c>
-      <c r="AP5" s="31">
-        <v>0</v>
-      </c>
-      <c r="AQ5" s="30">
-        <v>0</v>
-      </c>
-      <c r="AR5" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:44" s="26" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="AK5" s="39">
+        <v>1</v>
+      </c>
+      <c r="AL5" s="39">
+        <v>1</v>
+      </c>
+      <c r="AM5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AN5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AT5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AU5" s="40">
+        <v>0</v>
+      </c>
+      <c r="AV5" s="31">
+        <v>0</v>
+      </c>
+      <c r="AW5" s="31">
+        <v>0</v>
+      </c>
+      <c r="AX5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AY5" s="30">
+        <v>0</v>
+      </c>
+      <c r="AZ5" s="31">
+        <v>0</v>
+      </c>
+      <c r="BA5" s="31">
+        <v>0</v>
+      </c>
+      <c r="BB5" s="31">
+        <v>0</v>
+      </c>
+      <c r="BC5" s="31">
+        <v>0</v>
+      </c>
+      <c r="BD5" s="31">
+        <v>0</v>
+      </c>
+      <c r="BE5" s="31">
+        <v>0</v>
+      </c>
+      <c r="BF5" s="31">
+        <v>0</v>
+      </c>
+      <c r="BG5" s="31">
+        <v>0</v>
+      </c>
+      <c r="BH5" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:60" s="26" customFormat="1">
       <c r="A6" s="29" t="s">
         <v>43</v>
       </c>
@@ -2590,19 +2881,19 @@
       <c r="J6" s="3">
         <v>1</v>
       </c>
-      <c r="K6" s="40">
-        <v>1</v>
-      </c>
-      <c r="L6" s="40">
-        <v>1</v>
-      </c>
-      <c r="M6" s="40">
-        <v>1</v>
-      </c>
-      <c r="N6" s="40">
-        <v>1</v>
-      </c>
-      <c r="O6" s="40">
+      <c r="K6" s="3">
+        <v>1</v>
+      </c>
+      <c r="L6" s="3">
+        <v>1</v>
+      </c>
+      <c r="M6" s="3">
+        <v>1</v>
+      </c>
+      <c r="N6" s="3">
+        <v>1</v>
+      </c>
+      <c r="O6" s="3">
         <v>1</v>
       </c>
       <c r="P6" s="3">
@@ -2668,32 +2959,80 @@
       <c r="AJ6" s="3">
         <v>1</v>
       </c>
-      <c r="AK6" s="3">
-        <v>1</v>
-      </c>
-      <c r="AL6" s="3">
-        <v>1</v>
-      </c>
-      <c r="AM6" s="3">
-        <v>1</v>
-      </c>
-      <c r="AN6" s="30">
-        <v>1</v>
-      </c>
-      <c r="AO6" s="31">
-        <v>0</v>
-      </c>
-      <c r="AP6" s="31">
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="30">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:44" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="AK6" s="40">
+        <v>1</v>
+      </c>
+      <c r="AL6" s="40">
+        <v>1</v>
+      </c>
+      <c r="AM6" s="40">
+        <v>1</v>
+      </c>
+      <c r="AN6" s="40">
+        <v>1</v>
+      </c>
+      <c r="AO6" s="40">
+        <v>1</v>
+      </c>
+      <c r="AP6" s="40">
+        <v>1</v>
+      </c>
+      <c r="AQ6" s="40">
+        <v>1</v>
+      </c>
+      <c r="AR6" s="40">
+        <v>1</v>
+      </c>
+      <c r="AS6" s="40">
+        <v>1</v>
+      </c>
+      <c r="AT6" s="40">
+        <v>1</v>
+      </c>
+      <c r="AU6" s="40">
+        <v>1</v>
+      </c>
+      <c r="AV6" s="31">
+        <v>0</v>
+      </c>
+      <c r="AW6" s="31">
+        <v>0</v>
+      </c>
+      <c r="AX6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AY6" s="30">
+        <v>0</v>
+      </c>
+      <c r="AZ6" s="31">
+        <v>1</v>
+      </c>
+      <c r="BA6" s="31">
+        <v>1</v>
+      </c>
+      <c r="BB6" s="31">
+        <v>1</v>
+      </c>
+      <c r="BC6" s="30">
+        <v>1</v>
+      </c>
+      <c r="BD6" s="30">
+        <v>1</v>
+      </c>
+      <c r="BE6" s="30">
+        <v>1</v>
+      </c>
+      <c r="BF6" s="31">
+        <v>1</v>
+      </c>
+      <c r="BG6" s="31">
+        <v>1</v>
+      </c>
+      <c r="BH6" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:60" s="16" customFormat="1">
       <c r="A7" s="22" t="s">
         <v>44</v>
       </c>
@@ -2724,19 +3063,19 @@
       <c r="J7" s="16">
         <v>0</v>
       </c>
-      <c r="K7" s="40">
-        <v>0</v>
-      </c>
-      <c r="L7" s="40">
-        <v>0</v>
-      </c>
-      <c r="M7" s="40">
-        <v>0</v>
-      </c>
-      <c r="N7" s="40">
-        <v>0</v>
-      </c>
-      <c r="O7" s="40">
+      <c r="K7" s="16">
+        <v>0</v>
+      </c>
+      <c r="L7" s="16">
+        <v>0</v>
+      </c>
+      <c r="M7" s="16">
+        <v>0</v>
+      </c>
+      <c r="N7" s="16">
+        <v>0</v>
+      </c>
+      <c r="O7" s="16">
         <v>0</v>
       </c>
       <c r="P7" s="16">
@@ -2802,32 +3141,80 @@
       <c r="AJ7" s="16">
         <v>0</v>
       </c>
-      <c r="AK7" s="16">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="16">
-        <v>0</v>
-      </c>
-      <c r="AM7" s="16">
-        <v>0</v>
-      </c>
-      <c r="AN7" s="31">
-        <v>0</v>
-      </c>
-      <c r="AO7" s="31">
-        <v>0</v>
-      </c>
-      <c r="AP7" s="31">
-        <v>0</v>
-      </c>
-      <c r="AQ7" s="31">
-        <v>0</v>
-      </c>
-      <c r="AR7" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:44" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="AK7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AL7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AM7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AN7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AT7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AU7" s="40">
+        <v>0</v>
+      </c>
+      <c r="AV7" s="31">
+        <v>0</v>
+      </c>
+      <c r="AW7" s="31">
+        <v>0</v>
+      </c>
+      <c r="AX7" s="31">
+        <v>0</v>
+      </c>
+      <c r="AY7" s="31">
+        <v>0</v>
+      </c>
+      <c r="AZ7" s="31">
+        <v>0</v>
+      </c>
+      <c r="BA7" s="31">
+        <v>0</v>
+      </c>
+      <c r="BB7" s="31">
+        <v>0</v>
+      </c>
+      <c r="BC7" s="31">
+        <v>0</v>
+      </c>
+      <c r="BD7" s="31">
+        <v>0</v>
+      </c>
+      <c r="BE7" s="31">
+        <v>0</v>
+      </c>
+      <c r="BF7" s="31">
+        <v>0</v>
+      </c>
+      <c r="BG7" s="31">
+        <v>0</v>
+      </c>
+      <c r="BH7" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:60" s="16" customFormat="1">
       <c r="A8" s="22" t="s">
         <v>223</v>
       </c>
@@ -2858,19 +3245,19 @@
       <c r="J8" s="16">
         <v>0</v>
       </c>
-      <c r="K8" s="40">
-        <v>0</v>
-      </c>
-      <c r="L8" s="40">
-        <v>0</v>
-      </c>
-      <c r="M8" s="40">
-        <v>0</v>
-      </c>
-      <c r="N8" s="40">
-        <v>0</v>
-      </c>
-      <c r="O8" s="40">
+      <c r="K8" s="16">
+        <v>0</v>
+      </c>
+      <c r="L8" s="16">
+        <v>0</v>
+      </c>
+      <c r="M8" s="16">
+        <v>0</v>
+      </c>
+      <c r="N8" s="16">
+        <v>0</v>
+      </c>
+      <c r="O8" s="16">
         <v>0</v>
       </c>
       <c r="P8" s="16">
@@ -2936,32 +3323,80 @@
       <c r="AJ8" s="16">
         <v>0</v>
       </c>
-      <c r="AK8" s="16">
-        <v>0</v>
-      </c>
-      <c r="AL8" s="16">
-        <v>0</v>
-      </c>
-      <c r="AM8" s="16">
-        <v>0</v>
-      </c>
-      <c r="AN8" s="31">
-        <v>0</v>
-      </c>
-      <c r="AO8" s="31">
-        <v>0</v>
-      </c>
-      <c r="AP8" s="31">
-        <v>0</v>
-      </c>
-      <c r="AQ8" s="31">
-        <v>0</v>
-      </c>
-      <c r="AR8" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:44" s="16" customFormat="1" x14ac:dyDescent="0.15">
+      <c r="AK8" s="40">
+        <v>0</v>
+      </c>
+      <c r="AL8" s="40">
+        <v>0</v>
+      </c>
+      <c r="AM8" s="40">
+        <v>0</v>
+      </c>
+      <c r="AN8" s="40">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="40">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="40">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="40">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="40">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="40">
+        <v>0</v>
+      </c>
+      <c r="AT8" s="40">
+        <v>0</v>
+      </c>
+      <c r="AU8" s="40">
+        <v>0</v>
+      </c>
+      <c r="AV8" s="31">
+        <v>0</v>
+      </c>
+      <c r="AW8" s="31">
+        <v>0</v>
+      </c>
+      <c r="AX8" s="31">
+        <v>0</v>
+      </c>
+      <c r="AY8" s="31">
+        <v>0</v>
+      </c>
+      <c r="AZ8" s="31">
+        <v>0</v>
+      </c>
+      <c r="BA8" s="31">
+        <v>0</v>
+      </c>
+      <c r="BB8" s="31">
+        <v>0</v>
+      </c>
+      <c r="BC8" s="31">
+        <v>0</v>
+      </c>
+      <c r="BD8" s="31">
+        <v>0</v>
+      </c>
+      <c r="BE8" s="31">
+        <v>0</v>
+      </c>
+      <c r="BF8" s="31">
+        <v>0</v>
+      </c>
+      <c r="BG8" s="31">
+        <v>0</v>
+      </c>
+      <c r="BH8" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:60" s="16" customFormat="1">
       <c r="A9" s="22" t="s">
         <v>45</v>
       </c>
@@ -2992,19 +3427,19 @@
       <c r="J9" s="16">
         <v>0</v>
       </c>
-      <c r="K9" s="40">
-        <v>0</v>
-      </c>
-      <c r="L9" s="40">
-        <v>0</v>
-      </c>
-      <c r="M9" s="40">
-        <v>0</v>
-      </c>
-      <c r="N9" s="40">
-        <v>0</v>
-      </c>
-      <c r="O9" s="40">
+      <c r="K9" s="16">
+        <v>0</v>
+      </c>
+      <c r="L9" s="16">
+        <v>0</v>
+      </c>
+      <c r="M9" s="16">
+        <v>0</v>
+      </c>
+      <c r="N9" s="16">
+        <v>0</v>
+      </c>
+      <c r="O9" s="16">
         <v>0</v>
       </c>
       <c r="P9" s="16">
@@ -3070,32 +3505,80 @@
       <c r="AJ9" s="16">
         <v>0</v>
       </c>
-      <c r="AK9" s="16">
-        <v>0</v>
-      </c>
-      <c r="AL9" s="16">
-        <v>0</v>
-      </c>
-      <c r="AM9" s="16">
-        <v>0</v>
-      </c>
-      <c r="AN9" s="31">
-        <v>0</v>
-      </c>
-      <c r="AO9" s="31">
-        <v>0</v>
-      </c>
-      <c r="AP9" s="31">
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="31">
-        <v>0</v>
-      </c>
-      <c r="AR9" s="31">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:44" s="17" customFormat="1" ht="70" x14ac:dyDescent="0.15">
+      <c r="AK9" s="40">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="40">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="40">
+        <v>0</v>
+      </c>
+      <c r="AN9" s="40">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="40">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="40">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="40">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="40">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="40">
+        <v>0</v>
+      </c>
+      <c r="AT9" s="40">
+        <v>0</v>
+      </c>
+      <c r="AU9" s="40">
+        <v>0</v>
+      </c>
+      <c r="AV9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AW9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AX9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AY9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AZ9" s="31">
+        <v>0</v>
+      </c>
+      <c r="BA9" s="31">
+        <v>0</v>
+      </c>
+      <c r="BB9" s="31">
+        <v>0</v>
+      </c>
+      <c r="BC9" s="31">
+        <v>0</v>
+      </c>
+      <c r="BD9" s="31">
+        <v>0</v>
+      </c>
+      <c r="BE9" s="31">
+        <v>0</v>
+      </c>
+      <c r="BF9" s="31">
+        <v>0</v>
+      </c>
+      <c r="BG9" s="31">
+        <v>0</v>
+      </c>
+      <c r="BH9" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:60" s="17" customFormat="1" ht="67.5">
       <c r="A10" s="23" t="s">
         <v>46</v>
       </c>
@@ -3126,132 +3609,180 @@
       <c r="J10" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="K10" s="41" t="s">
+      <c r="K10" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="L10" s="24" t="s">
+        <v>58</v>
+      </c>
+      <c r="M10" s="24" t="s">
+        <v>57</v>
+      </c>
+      <c r="N10" s="24" t="s">
+        <v>59</v>
+      </c>
+      <c r="O10" s="24" t="s">
+        <v>60</v>
+      </c>
+      <c r="P10" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="Q10" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="R10" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="S10" s="24" t="s">
+        <v>64</v>
+      </c>
+      <c r="T10" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="U10" s="24" t="s">
+        <v>66</v>
+      </c>
+      <c r="V10" s="24" t="s">
+        <v>67</v>
+      </c>
+      <c r="W10" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="X10" s="24" t="s">
+        <v>69</v>
+      </c>
+      <c r="Y10" s="24" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z10" s="24" t="s">
+        <v>71</v>
+      </c>
+      <c r="AA10" s="24" t="s">
+        <v>72</v>
+      </c>
+      <c r="AB10" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="AC10" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="AD10" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="AE10" s="24" t="s">
+        <v>76</v>
+      </c>
+      <c r="AF10" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="AG10" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="AH10" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="AI10" s="24" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ10" s="24" t="s">
+        <v>235</v>
+      </c>
+      <c r="AK10" s="41" t="s">
         <v>211</v>
       </c>
-      <c r="L10" s="41" t="s">
+      <c r="AL10" s="41" t="s">
         <v>211</v>
       </c>
-      <c r="M10" s="41" t="s">
+      <c r="AM10" s="41" t="s">
         <v>212</v>
       </c>
-      <c r="N10" s="41" t="s">
+      <c r="AN10" s="41" t="s">
         <v>213</v>
       </c>
-      <c r="O10" s="41" t="s">
+      <c r="AO10" s="41" t="s">
         <v>214</v>
       </c>
-      <c r="P10" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q10" s="24" t="s">
-        <v>58</v>
-      </c>
-      <c r="R10" s="24" t="s">
-        <v>57</v>
-      </c>
-      <c r="S10" s="24" t="s">
-        <v>59</v>
-      </c>
-      <c r="T10" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="U10" s="24" t="s">
-        <v>61</v>
-      </c>
-      <c r="V10" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="W10" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="X10" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y10" s="24" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z10" s="24" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA10" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB10" s="24" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC10" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD10" s="24" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE10" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="AF10" s="24" t="s">
-        <v>72</v>
-      </c>
-      <c r="AG10" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="AH10" s="24" t="s">
-        <v>74</v>
-      </c>
-      <c r="AI10" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="AJ10" s="24" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK10" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="AL10" s="24" t="s">
-        <v>78</v>
-      </c>
-      <c r="AM10" s="24" t="s">
-        <v>79</v>
-      </c>
-      <c r="AN10" s="32" t="s">
-        <v>51</v>
-      </c>
-      <c r="AO10" s="32" t="s">
+      <c r="AP10" s="41" t="s">
+        <v>212</v>
+      </c>
+      <c r="AQ10" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="AR10" s="41" t="s">
+        <v>214</v>
+      </c>
+      <c r="AS10" s="41" t="s">
+        <v>212</v>
+      </c>
+      <c r="AT10" s="41" t="s">
+        <v>213</v>
+      </c>
+      <c r="AU10" s="41" t="s">
+        <v>214</v>
+      </c>
+      <c r="AV10" s="32" t="s">
         <v>80</v>
       </c>
-      <c r="AP10" s="32" t="s">
+      <c r="AW10" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="AQ10" s="33"/>
-      <c r="AR10" s="33"/>
+      <c r="AX10" s="33"/>
+      <c r="AY10" s="33"/>
+      <c r="AZ10" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="BA10" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="BB10" s="32" t="s">
+        <v>214</v>
+      </c>
+      <c r="BC10" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="BD10" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="BE10" s="32" t="s">
+        <v>235</v>
+      </c>
+      <c r="BF10" s="32" t="s">
+        <v>212</v>
+      </c>
+      <c r="BG10" s="32" t="s">
+        <v>213</v>
+      </c>
+      <c r="BH10" s="32" t="s">
+        <v>214</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="P3:R3 AO5:AP6 T3:AH3 J3 AO7:AR9 B5:J5 K6:O6 B7:AM9 M5:AN5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AV5:AW6 O3:AC3 J3:M3 AZ5:BB6 B5:AJ5 BC5:BH5 B7:AH9 AV7:BB9 BF6:BH9 AM5:AU5 AK6:AU9" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9" xr:uid="{00000000-0002-0000-0000-000001000000}"/>
   </dataValidations>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <headerFooter alignWithMargins="0"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:AD10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" customWidth="1"/>
+    <col min="1" max="1" width="19.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="14" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:30" s="14" customFormat="1" ht="27">
       <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
@@ -3343,7 +3874,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:30" s="15" customFormat="1">
       <c r="A2" s="20" t="s">
         <v>36</v>
       </c>
@@ -3435,7 +3966,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:30" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:30" s="15" customFormat="1">
       <c r="A3" s="20" t="s">
         <v>40</v>
       </c>
@@ -3527,7 +4058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:30" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:30" s="15" customFormat="1">
       <c r="A4" s="20" t="s">
         <v>41</v>
       </c>
@@ -3619,7 +4150,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:30" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:30" s="15" customFormat="1">
       <c r="A5" s="20" t="s">
         <v>42</v>
       </c>
@@ -3711,7 +4242,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:30" s="15" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:30" s="15" customFormat="1">
       <c r="A6" s="20" t="s">
         <v>43</v>
       </c>
@@ -3803,7 +4334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:30" s="16" customFormat="1">
       <c r="A7" s="22" t="s">
         <v>44</v>
       </c>
@@ -3895,7 +4426,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:30" s="16" customFormat="1">
       <c r="A8" s="22" t="s">
         <v>223</v>
       </c>
@@ -3987,7 +4518,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:30" s="16" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:30" s="16" customFormat="1">
       <c r="A9" s="22" t="s">
         <v>45</v>
       </c>
@@ -4079,7 +4610,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:30" s="17" customFormat="1" ht="56" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:30" s="17" customFormat="1" ht="54">
       <c r="A10" s="23" t="s">
         <v>46</v>
       </c>
@@ -4173,8 +4704,8 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:AD9">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9" xr:uid="{00000000-0002-0000-0100-000000000000}"/>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B7:AD9" xr:uid="{00000000-0002-0000-0100-000001000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -4185,45 +4716,45 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AC11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="19.33203125" customWidth="1"/>
     <col min="2" max="2" width="21" customWidth="1"/>
-    <col min="3" max="3" width="7.1640625" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="7.1328125" customWidth="1"/>
+    <col min="4" max="4" width="10.46484375" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="8" max="9" width="9.1640625" customWidth="1"/>
+    <col min="8" max="9" width="9.1328125" customWidth="1"/>
     <col min="10" max="12" width="12.6640625" customWidth="1"/>
-    <col min="13" max="13" width="21.1640625" customWidth="1"/>
+    <col min="13" max="13" width="21.1328125" customWidth="1"/>
     <col min="14" max="14" width="10.33203125" customWidth="1"/>
     <col min="15" max="15" width="11.6640625" customWidth="1"/>
     <col min="16" max="16" width="10.33203125" customWidth="1"/>
-    <col min="17" max="17" width="9.1640625" customWidth="1"/>
-    <col min="18" max="18" width="12.83203125" customWidth="1"/>
+    <col min="17" max="17" width="9.1328125" customWidth="1"/>
+    <col min="18" max="18" width="12.796875" customWidth="1"/>
     <col min="19" max="19" width="10.33203125" customWidth="1"/>
-    <col min="20" max="20" width="15.1640625" customWidth="1"/>
+    <col min="20" max="20" width="15.1328125" customWidth="1"/>
     <col min="21" max="21" width="14" customWidth="1"/>
     <col min="22" max="22" width="12.6640625" customWidth="1"/>
     <col min="23" max="23" width="14" customWidth="1"/>
     <col min="24" max="25" width="11.6640625" customWidth="1"/>
-    <col min="26" max="26" width="15.1640625" customWidth="1"/>
+    <col min="26" max="26" width="15.1328125" customWidth="1"/>
     <col min="27" max="27" width="12.6640625" customWidth="1"/>
     <col min="28" max="29" width="14" customWidth="1"/>
     <col min="30" max="30" width="11.6640625" customWidth="1"/>
-    <col min="31" max="32" width="15.1640625" customWidth="1"/>
+    <col min="31" max="32" width="15.1328125" customWidth="1"/>
     <col min="33" max="33" width="14" customWidth="1"/>
-    <col min="34" max="34" width="15.1640625" customWidth="1"/>
+    <col min="34" max="34" width="15.1328125" customWidth="1"/>
     <col min="35" max="35" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:29" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4231,7 +4762,7 @@
         <v>222</v>
       </c>
     </row>
-    <row r="2" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:29" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>138</v>
       </c>
@@ -4239,7 +4770,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:29" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>139</v>
       </c>
@@ -4247,7 +4778,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:29" s="3" customFormat="1">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -4255,7 +4786,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:29" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>41</v>
       </c>
@@ -4263,7 +4794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:29" s="3" customFormat="1">
       <c r="A6" s="3" t="s">
         <v>42</v>
       </c>
@@ -4271,7 +4802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:29" s="3" customFormat="1">
       <c r="A7" s="3" t="s">
         <v>43</v>
       </c>
@@ -4279,7 +4810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:29" s="3" customFormat="1">
       <c r="A8" s="3" t="s">
         <v>187</v>
       </c>
@@ -4287,7 +4818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:29" s="3" customFormat="1">
       <c r="A9" s="34" t="s">
         <v>82</v>
       </c>
@@ -4376,7 +4907,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="10" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:29" s="3" customFormat="1">
       <c r="A10" s="34" t="s">
         <v>38</v>
       </c>
@@ -4465,7 +4996,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:29" s="3" customFormat="1">
       <c r="A11" s="34" t="s">
         <v>46</v>
       </c>
@@ -4502,13 +5033,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:B5 D11:G1048576 A6 D1:G8 B6:B8">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A4:B5 D11:G1048576 A6 D1:G8 B6:B8" xr:uid="{00000000-0002-0000-0200-000000000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A10:C10 U10 V9:AC10 I11:AC1048576 D9:T10 AD1:AK1048576 I1:AC8">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A10:C10 U10 V9:AC10 I11:AC1048576 D9:T10 AD1:AK1048576 I1:AC8" xr:uid="{00000000-0002-0000-0200-000001000000}">
       <formula1>"int,string,float,object"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11 B12:C1048576 A2:B3 C1:C8">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C11 B12:C1048576 A2:B3 C1:C8" xr:uid="{00000000-0002-0000-0200-000002000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -4520,19 +5051,19 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AC22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" style="4" customWidth="1"/>
+    <col min="1" max="1" width="16.1328125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="21.796875" style="4" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" style="4" customWidth="1"/>
+    <col min="4" max="4" width="10.46484375" style="4" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" style="4" customWidth="1"/>
     <col min="6" max="9" width="9" style="4"/>
     <col min="10" max="10" width="12.6640625" style="4" customWidth="1"/>
@@ -4545,7 +5076,7 @@
     <col min="17" max="19" width="9" style="4"/>
     <col min="20" max="20" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9.33203125" style="4" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.1640625" style="4" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="8.1328125" style="4" bestFit="1" customWidth="1"/>
     <col min="23" max="24" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="10.33203125" style="4" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="11.33203125" style="4" bestFit="1" customWidth="1"/>
@@ -4556,7 +5087,7 @@
     <col min="31" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -4564,7 +5095,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:23" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>138</v>
       </c>
@@ -4572,7 +5103,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:23" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>139</v>
       </c>
@@ -4580,7 +5111,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:23" s="3" customFormat="1">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -4588,7 +5119,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:23" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>41</v>
       </c>
@@ -4596,7 +5127,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:23" s="3" customFormat="1">
       <c r="A6" s="3" t="s">
         <v>42</v>
       </c>
@@ -4604,7 +5135,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:23" s="3" customFormat="1">
       <c r="A7" s="3" t="s">
         <v>43</v>
       </c>
@@ -4612,7 +5143,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:23" s="3" customFormat="1">
       <c r="A8" s="3" t="s">
         <v>45</v>
       </c>
@@ -4620,7 +5151,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:23" s="3" customFormat="1">
       <c r="A9" s="34" t="s">
         <v>140</v>
       </c>
@@ -4691,7 +5222,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:23" s="3" customFormat="1">
       <c r="A10" s="35" t="s">
         <v>39</v>
       </c>
@@ -4762,7 +5293,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:23" s="3" customFormat="1">
       <c r="A11" s="34" t="s">
         <v>46</v>
       </c>
@@ -4788,7 +5319,7 @@
       <c r="U11" s="34"/>
       <c r="V11" s="34"/>
     </row>
-    <row r="12" spans="1:23" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:23" s="2" customFormat="1">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -4796,7 +5327,7 @@
         <v>224</v>
       </c>
     </row>
-    <row r="13" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:23" s="3" customFormat="1">
       <c r="A13" s="3" t="s">
         <v>138</v>
       </c>
@@ -4804,7 +5335,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:23" s="3" customFormat="1">
       <c r="A14" s="3" t="s">
         <v>139</v>
       </c>
@@ -4812,7 +5343,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:23" s="3" customFormat="1">
       <c r="A15" s="3" t="s">
         <v>40</v>
       </c>
@@ -4820,7 +5351,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:23" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:23" s="3" customFormat="1">
       <c r="A16" s="3" t="s">
         <v>41</v>
       </c>
@@ -4828,7 +5359,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:29" s="3" customFormat="1">
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
@@ -4836,7 +5367,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:29" s="3" customFormat="1">
       <c r="A18" s="3" t="s">
         <v>43</v>
       </c>
@@ -4844,7 +5375,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:29" s="3" customFormat="1">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
@@ -4852,7 +5383,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:29" s="3" customFormat="1">
       <c r="A20" s="34" t="s">
         <v>82</v>
       </c>
@@ -4941,7 +5472,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="21" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:29" s="3" customFormat="1">
       <c r="A21" s="34" t="s">
         <v>38</v>
       </c>
@@ -5030,7 +5561,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:29" s="3" customFormat="1">
       <c r="A22" s="34" t="s">
         <v>46</v>
       </c>
@@ -5067,13 +5598,13 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6:B8 A17 C22 B17:B19 D22:G1048576 A4:B5 A15:B16 C12:G18">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6:B8 A17 C22 B17:B19 D22:G1048576 A4:B5 A15:B16 C12:G18" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A21:C21 U21 D20:T21 V20:AC21">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A21:C21 U21 D20:T21 V20:AC21" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"int,string,float,object"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A13:B14 B23:C1048576 A2:B3">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A13:B14 B23:C1048576 A2:B3" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -5085,33 +5616,33 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W33"/>
   <sheetViews>
     <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="12.6640625" customWidth="1"/>
     <col min="2" max="2" width="15.33203125" customWidth="1"/>
     <col min="3" max="3" width="10.33203125" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="14.1328125" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
-    <col min="8" max="15" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="18" width="16.5" customWidth="1"/>
+    <col min="8" max="15" width="12.46484375" bestFit="1" customWidth="1"/>
+    <col min="16" max="18" width="16.46484375" customWidth="1"/>
     <col min="19" max="19" width="20" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="21.1328125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="20" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="25" width="16.5" customWidth="1"/>
+    <col min="24" max="25" width="16.46484375" customWidth="1"/>
     <col min="26" max="26" width="19" customWidth="1"/>
-    <col min="27" max="31" width="20.1640625" customWidth="1"/>
+    <col min="27" max="31" width="20.1328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:23" s="11" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5140,7 +5671,7 @@
       <c r="V1" s="2"/>
       <c r="W1" s="2"/>
     </row>
-    <row r="2" spans="1:23" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:23" s="12" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>138</v>
       </c>
@@ -5169,7 +5700,7 @@
       <c r="V2" s="3"/>
       <c r="W2" s="3"/>
     </row>
-    <row r="3" spans="1:23" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:23" s="12" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>139</v>
       </c>
@@ -5198,7 +5729,7 @@
       <c r="V3" s="3"/>
       <c r="W3" s="3"/>
     </row>
-    <row r="4" spans="1:23" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:23" s="12" customFormat="1">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -5227,7 +5758,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="1:23" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:23" s="12" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>41</v>
       </c>
@@ -5256,7 +5787,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="1:23" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:23" s="12" customFormat="1">
       <c r="A6" s="3" t="s">
         <v>42</v>
       </c>
@@ -5285,7 +5816,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="1:23" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:23" s="12" customFormat="1">
       <c r="A7" s="3" t="s">
         <v>43</v>
       </c>
@@ -5314,7 +5845,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="8" spans="1:23" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:23" s="12" customFormat="1">
       <c r="A8" s="3" t="s">
         <v>45</v>
       </c>
@@ -5343,7 +5874,7 @@
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
     </row>
-    <row r="9" spans="1:23" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:23" s="12" customFormat="1">
       <c r="A9" s="34" t="s">
         <v>140</v>
       </c>
@@ -5414,7 +5945,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:23" s="12" customFormat="1">
       <c r="A10" s="34" t="s">
         <v>39</v>
       </c>
@@ -5485,7 +6016,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="12" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:23" s="12" customFormat="1">
       <c r="A11" s="34" t="s">
         <v>46</v>
       </c>
@@ -5514,7 +6045,7 @@
       <c r="V11" s="34"/>
       <c r="W11" s="34"/>
     </row>
-    <row r="12" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:23" s="11" customFormat="1">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -5543,7 +6074,7 @@
       <c r="V12" s="2"/>
       <c r="W12" s="2"/>
     </row>
-    <row r="13" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:23" s="13" customFormat="1">
       <c r="A13" s="3" t="s">
         <v>138</v>
       </c>
@@ -5572,7 +6103,7 @@
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
     </row>
-    <row r="14" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:23" s="13" customFormat="1">
       <c r="A14" s="3" t="s">
         <v>139</v>
       </c>
@@ -5601,7 +6132,7 @@
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
     </row>
-    <row r="15" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:23" s="13" customFormat="1">
       <c r="A15" s="3" t="s">
         <v>40</v>
       </c>
@@ -5630,7 +6161,7 @@
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
     </row>
-    <row r="16" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:23" s="13" customFormat="1">
       <c r="A16" s="3" t="s">
         <v>41</v>
       </c>
@@ -5659,7 +6190,7 @@
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
     </row>
-    <row r="17" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:23" s="13" customFormat="1">
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
@@ -5688,7 +6219,7 @@
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
     </row>
-    <row r="18" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:23" s="13" customFormat="1">
       <c r="A18" s="3" t="s">
         <v>43</v>
       </c>
@@ -5717,7 +6248,7 @@
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
     </row>
-    <row r="19" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:23" s="13" customFormat="1">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
@@ -5746,7 +6277,7 @@
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
     </row>
-    <row r="20" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:23" s="13" customFormat="1">
       <c r="A20" s="34" t="s">
         <v>141</v>
       </c>
@@ -5763,7 +6294,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="21" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:23" s="13" customFormat="1">
       <c r="A21" s="34" t="s">
         <v>37</v>
       </c>
@@ -5780,7 +6311,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:23" s="13" customFormat="1">
       <c r="A22" s="34" t="s">
         <v>46</v>
       </c>
@@ -5809,7 +6340,7 @@
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
     </row>
-    <row r="23" spans="1:23" s="11" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:23" s="11" customFormat="1">
       <c r="A23" s="2" t="s">
         <v>0</v>
       </c>
@@ -5838,7 +6369,7 @@
       <c r="V23" s="2"/>
       <c r="W23" s="2"/>
     </row>
-    <row r="24" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:23" s="13" customFormat="1">
       <c r="A24" s="3" t="s">
         <v>138</v>
       </c>
@@ -5867,7 +6398,7 @@
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
     </row>
-    <row r="25" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:23" s="13" customFormat="1">
       <c r="A25" s="3" t="s">
         <v>139</v>
       </c>
@@ -5896,7 +6427,7 @@
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
     </row>
-    <row r="26" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:23" s="13" customFormat="1">
       <c r="A26" s="3" t="s">
         <v>40</v>
       </c>
@@ -5925,7 +6456,7 @@
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
     </row>
-    <row r="27" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="27" spans="1:23" s="13" customFormat="1">
       <c r="A27" s="3" t="s">
         <v>41</v>
       </c>
@@ -5954,7 +6485,7 @@
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
     </row>
-    <row r="28" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="28" spans="1:23" s="13" customFormat="1">
       <c r="A28" s="3" t="s">
         <v>42</v>
       </c>
@@ -5983,7 +6514,7 @@
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
     </row>
-    <row r="29" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="29" spans="1:23" s="13" customFormat="1">
       <c r="A29" s="3" t="s">
         <v>43</v>
       </c>
@@ -6012,7 +6543,7 @@
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
     </row>
-    <row r="30" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="30" spans="1:23" s="13" customFormat="1">
       <c r="A30" s="3" t="s">
         <v>45</v>
       </c>
@@ -6041,7 +6572,7 @@
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
     </row>
-    <row r="31" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="31" spans="1:23" s="13" customFormat="1">
       <c r="A31" s="34" t="s">
         <v>140</v>
       </c>
@@ -6055,7 +6586,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="32" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="32" spans="1:23" s="13" customFormat="1">
       <c r="A32" s="34" t="s">
         <v>39</v>
       </c>
@@ -6069,7 +6600,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="33" spans="1:23" s="13" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="33" spans="1:23" s="13" customFormat="1">
       <c r="A33" s="34" t="s">
         <v>46</v>
       </c>
@@ -6097,16 +6628,16 @@
       <c r="W33" s="3"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:W33"/>
+  <autoFilter ref="A1:W33" xr:uid="{00000000-0009-0000-0000-000004000000}"/>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6:B8 E11:F11 A17 B17:B19 G11:G19 E1:G8 A4:B5 D12:F19 A15:B16 D22:G30 A26:B28 E33 G33:G1048576 D34:F1048576 B29:B30">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6:B8 E11:F11 A17 B17:B19 G11:G19 E1:G8 A4:B5 D12:F19 A15:B16 D22:G30 A26:B28 E33 G33:G1048576 D34:F1048576 B29:B30" xr:uid="{00000000-0002-0000-0400-000000000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B9 G9 N9:W9 F9:F10 N1:N8 N11:N19 N22:N30 N33:N1048576 A31"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B10 G10 N10:W10 A9:A10 O1:AE8 A20:E21 I11:M19 O11:AE19 O33:AE1048576 I1:M8 X9:AE10 C9:E10 H9:M10 O22:AE30 I22:M30 I33:M1048576 A32 B31:C32">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="B9 G9 N9:W9 F9:F10 N1:N8 N11:N19 N22:N30 N33:N1048576 A31" xr:uid="{00000000-0002-0000-0400-000001000000}"/>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="B10 G10 N10:W10 A9:A10 O1:AE8 A20:E21 I11:M19 O11:AE19 O33:AE1048576 I1:M8 X9:AE10 C9:E10 H9:M10 O22:AE30 I22:M30 I33:M1048576 A32 B31:C32" xr:uid="{00000000-0002-0000-0400-000002000000}">
       <formula1>"int,string,float,object"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C33:C1048576 C12:C19 A2:B3 A13:B14 C22:C30 B34:B1048576 A24:B25 D33">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C33:C1048576 C12:C19 A2:B3 A13:B14 C22:C30 B34:B1048576 A24:B25 D33" xr:uid="{00000000-0002-0000-0400-000003000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -6117,27 +6648,27 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" customWidth="1"/>
+    <col min="1" max="1" width="16.1328125" customWidth="1"/>
+    <col min="2" max="2" width="17.1328125" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" customWidth="1"/>
-    <col min="4" max="4" width="10.5" customWidth="1"/>
+    <col min="4" max="4" width="10.46484375" customWidth="1"/>
     <col min="5" max="5" width="11.6640625" customWidth="1"/>
     <col min="8" max="8" width="11" customWidth="1"/>
     <col min="9" max="9" width="12.6640625" customWidth="1"/>
     <col min="10" max="11" width="22.6640625" customWidth="1"/>
-    <col min="12" max="12" width="10.5" customWidth="1"/>
+    <col min="12" max="12" width="10.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4" s="5" customFormat="1">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -6145,7 +6676,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4" s="6" customFormat="1">
       <c r="A2" s="9" t="s">
         <v>138</v>
       </c>
@@ -6153,7 +6684,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:4" s="6" customFormat="1">
       <c r="A3" s="9" t="s">
         <v>139</v>
       </c>
@@ -6161,7 +6692,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:4" s="6" customFormat="1">
       <c r="A4" s="9" t="s">
         <v>40</v>
       </c>
@@ -6169,7 +6700,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:4" s="6" customFormat="1">
       <c r="A5" s="9" t="s">
         <v>41</v>
       </c>
@@ -6177,7 +6708,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:4" s="6" customFormat="1">
       <c r="A6" s="9" t="s">
         <v>42</v>
       </c>
@@ -6185,7 +6716,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:4" s="6" customFormat="1">
       <c r="A7" s="9" t="s">
         <v>43</v>
       </c>
@@ -6193,7 +6724,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:4" s="6" customFormat="1">
       <c r="A8" s="9" t="s">
         <v>189</v>
       </c>
@@ -6201,7 +6732,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:4" s="6" customFormat="1">
       <c r="A9" s="36" t="s">
         <v>190</v>
       </c>
@@ -6215,7 +6746,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="10" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:4" s="6" customFormat="1">
       <c r="A10" s="36" t="s">
         <v>37</v>
       </c>
@@ -6229,7 +6760,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:4" s="6" customFormat="1">
       <c r="A11" s="37" t="s">
         <v>46</v>
       </c>
@@ -6239,7 +6770,7 @@
       <c r="C11" s="36"/>
       <c r="D11" s="36"/>
     </row>
-    <row r="12" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:4" s="5" customFormat="1">
       <c r="A12" s="7" t="s">
         <v>0</v>
       </c>
@@ -6247,7 +6778,7 @@
         <v>195</v>
       </c>
     </row>
-    <row r="13" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:4" s="6" customFormat="1">
       <c r="A13" s="9" t="s">
         <v>138</v>
       </c>
@@ -6255,7 +6786,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="14" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:4" s="6" customFormat="1">
       <c r="A14" s="9" t="s">
         <v>139</v>
       </c>
@@ -6263,7 +6794,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:4" s="6" customFormat="1">
       <c r="A15" s="9" t="s">
         <v>40</v>
       </c>
@@ -6271,7 +6802,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:4" s="6" customFormat="1">
       <c r="A16" s="9" t="s">
         <v>41</v>
       </c>
@@ -6279,7 +6810,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:3" s="6" customFormat="1">
       <c r="A17" s="9" t="s">
         <v>42</v>
       </c>
@@ -6287,7 +6818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:3" s="6" customFormat="1">
       <c r="A18" s="9" t="s">
         <v>43</v>
       </c>
@@ -6295,7 +6826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:3" s="6" customFormat="1">
       <c r="A19" s="9" t="s">
         <v>189</v>
       </c>
@@ -6303,7 +6834,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:3" s="6" customFormat="1">
       <c r="A20" s="36" t="s">
         <v>193</v>
       </c>
@@ -6314,7 +6845,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:3" s="6" customFormat="1">
       <c r="A21" s="36" t="s">
         <v>37</v>
       </c>
@@ -6325,7 +6856,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:3" s="6" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:3" s="6" customFormat="1">
       <c r="A22" s="37" t="s">
         <v>46</v>
       </c>
@@ -6336,16 +6867,16 @@
     </row>
   </sheetData>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B19" xr:uid="{00000000-0002-0000-0500-000000000000}">
       <formula1>"true,false"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6 B7 B8 A17 B17 B18 G1:G21 E1:F11 D12:F21 D22:G1048576 A4:B5 A15:B16">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6 B7 B8 A17 B17 B18 G1:G21 E1:F11 D12:F21 D22:G1048576 A4:B5 A15:B16" xr:uid="{00000000-0002-0000-0500-000001000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B1048576 C12:C19 C22:C1048576 A13:B14 A2:B3">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B1048576 C12:C19 C22:C1048576 A13:B14 A2:B3" xr:uid="{00000000-0002-0000-0500-000002000000}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A9:D10 I1:L1048576 A20:B21">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A9:D10 I1:L1048576 A20:B21" xr:uid="{00000000-0002-0000-0500-000003000000}">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
   </dataValidations>
@@ -6357,30 +6888,30 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="16.1640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="21.1640625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.1640625" style="4" customWidth="1"/>
+    <col min="1" max="1" width="16.1328125" style="4" customWidth="1"/>
+    <col min="2" max="2" width="21.1328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.1328125" style="4" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" style="4" customWidth="1"/>
     <col min="5" max="5" width="13.6640625" style="4" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9" style="4"/>
     <col min="8" max="8" width="12.6640625" style="4" customWidth="1"/>
-    <col min="9" max="9" width="13.83203125" style="4" customWidth="1"/>
+    <col min="9" max="9" width="13.796875" style="4" customWidth="1"/>
     <col min="10" max="10" width="9" style="4"/>
     <col min="11" max="11" width="11.6640625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="13.83203125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="13.796875" style="4" customWidth="1"/>
     <col min="13" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -6388,7 +6919,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>138</v>
       </c>
@@ -6396,7 +6927,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:5" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>139</v>
       </c>
@@ -6404,7 +6935,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="4" spans="1:5" s="3" customFormat="1">
       <c r="A4" s="3" t="s">
         <v>40</v>
       </c>
@@ -6412,7 +6943,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="5" spans="1:5" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>41</v>
       </c>
@@ -6420,7 +6951,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="6" spans="1:5" s="3" customFormat="1">
       <c r="A6" s="3" t="s">
         <v>42</v>
       </c>
@@ -6428,7 +6959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5" s="3" customFormat="1">
       <c r="A7" s="3" t="s">
         <v>43</v>
       </c>
@@ -6436,7 +6967,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5" s="3" customFormat="1">
       <c r="A8" s="3" t="s">
         <v>187</v>
       </c>
@@ -6444,7 +6975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5" s="3" customFormat="1">
       <c r="A9" s="34" t="s">
         <v>227</v>
       </c>
@@ -6461,7 +6992,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="10" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5" s="3" customFormat="1">
       <c r="A10" s="34" t="s">
         <v>37</v>
       </c>
@@ -6478,7 +7009,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5" s="3" customFormat="1">
       <c r="A11" s="34" t="s">
         <v>46</v>
       </c>
@@ -6487,7 +7018,7 @@
       <c r="D11" s="34"/>
       <c r="E11" s="34"/>
     </row>
-    <row r="12" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" s="2" customFormat="1">
       <c r="A12" s="2" t="s">
         <v>0</v>
       </c>
@@ -6495,7 +7026,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="13" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="13" spans="1:5" s="3" customFormat="1">
       <c r="A13" s="3" t="s">
         <v>138</v>
       </c>
@@ -6503,7 +7034,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="14" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5" s="3" customFormat="1">
       <c r="A14" s="3" t="s">
         <v>139</v>
       </c>
@@ -6511,7 +7042,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="15" spans="1:5" s="3" customFormat="1">
       <c r="A15" s="3" t="s">
         <v>40</v>
       </c>
@@ -6519,7 +7050,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="16" spans="1:5" s="3" customFormat="1">
       <c r="A16" s="3" t="s">
         <v>41</v>
       </c>
@@ -6527,7 +7058,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="17" spans="1:5" s="3" customFormat="1">
       <c r="A17" s="3" t="s">
         <v>42</v>
       </c>
@@ -6535,7 +7066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5" s="3" customFormat="1">
       <c r="A18" s="3" t="s">
         <v>43</v>
       </c>
@@ -6543,7 +7074,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5" s="3" customFormat="1">
       <c r="A19" s="3" t="s">
         <v>45</v>
       </c>
@@ -6551,7 +7082,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5" s="3" customFormat="1">
       <c r="A20" s="34" t="s">
         <v>227</v>
       </c>
@@ -6568,7 +7099,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5" s="3" customFormat="1">
       <c r="A21" s="34" t="s">
         <v>37</v>
       </c>
@@ -6585,7 +7116,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5" s="3" customFormat="1">
       <c r="A22" s="34" t="s">
         <v>46</v>
       </c>
@@ -6596,18 +7127,18 @@
     </row>
   </sheetData>
   <dataValidations count="6">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6:B8 B18:B19 F1:F1048576 A15:B17 A4:B5 E1:E8 E11:E19 E22:E1048576">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 B6:B8 B18:B19 F1:F1048576 A15:B17 A4:B5 E1:E8 E11:E19 E22:E1048576" xr:uid="{00000000-0002-0000-0600-000000000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A9:B9 H40:H1048576 A20:B20"/>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A10:B10 A21:B21 H1:H39">
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="A9:B9 H40:H1048576 A20:B20" xr:uid="{00000000-0002-0000-0600-000001000000}"/>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A10:B10 A21:B21 H1:H39" xr:uid="{00000000-0002-0000-0600-000002000000}">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C21">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C10 C21" xr:uid="{00000000-0002-0000-0600-000003000000}">
       <formula1>"int,float,string,object"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8 A18:A19"/>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B1048576 C12:C19 C22:C1048576 A2:B3 A13:B14">
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A8 A18:A19" xr:uid="{00000000-0002-0000-0600-000004000000}"/>
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B23:B1048576 C12:C19 C22:C1048576 A2:B3 A13:B14" xr:uid="{00000000-0002-0000-0600-000005000000}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -6617,21 +7148,21 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="1" width="8.1640625" customWidth="1"/>
+    <col min="1" max="1" width="8.1328125" customWidth="1"/>
     <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="10.5" customWidth="1"/>
+    <col min="3" max="3" width="10.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -6645,7 +7176,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
         <v>206</v>
       </c>
@@ -6661,10 +7192,10 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2" xr:uid="{00000000-0002-0000-0700-000000000000}">
       <formula1>"lua,python,C#,js"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2" xr:uid="{00000000-0002-0000-0700-000001000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
new protocol for hero
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Player.xlsx
+++ b/_Out/NFDataCfg/Excel/Player.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="458" windowWidth="28043" windowHeight="17543" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="458" windowWidth="28043" windowHeight="17543" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -432,7 +432,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="930" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="896" uniqueCount="288">
   <si>
     <t>Id</t>
   </si>
@@ -860,39 +860,6 @@
     <t>Star</t>
   </si>
   <si>
-    <t>Equip1</t>
-  </si>
-  <si>
-    <t>Equip2</t>
-  </si>
-  <si>
-    <t>Equip3</t>
-  </si>
-  <si>
-    <t>Equip4</t>
-  </si>
-  <si>
-    <t>Equip5</t>
-  </si>
-  <si>
-    <t>Equip6</t>
-  </si>
-  <si>
-    <t>Talent1</t>
-  </si>
-  <si>
-    <t>Talent2</t>
-  </si>
-  <si>
-    <t>Talent3</t>
-  </si>
-  <si>
-    <t>Talent4</t>
-  </si>
-  <si>
-    <t>Talent5</t>
-  </si>
-  <si>
     <t>Skill1</t>
   </si>
   <si>
@@ -906,9 +873,6 @@
   </si>
   <si>
     <t>Skill5</t>
-  </si>
-  <si>
-    <t>FightSkill</t>
   </si>
   <si>
     <t>BagEquipList</t>
@@ -2110,7 +2074,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AS10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AJ6" sqref="A6:XFD6"/>
     </sheetView>
@@ -2188,7 +2152,7 @@
         <v>17</v>
       </c>
       <c r="R1" s="28" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="S1" s="28" t="s">
         <v>18</v>
@@ -2242,34 +2206,34 @@
         <v>5</v>
       </c>
       <c r="AJ1" s="28" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="AK1" s="28" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="AL1" s="28" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="AM1" s="28" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="AN1" s="28" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="AO1" s="28" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="AP1" s="28" t="s">
-        <v>258</v>
+        <v>246</v>
       </c>
       <c r="AQ1" s="28" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="AR1" s="28" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="AS1" s="28" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
     </row>
     <row r="2" spans="1:45" s="26" customFormat="1">
@@ -3096,7 +3060,7 @@
     </row>
     <row r="8" spans="1:45" s="16" customFormat="1">
       <c r="A8" s="22" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B8" s="16">
         <v>0</v>
@@ -3475,34 +3439,34 @@
         <v>49</v>
       </c>
       <c r="AJ10" s="24" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="AK10" s="41" t="s">
-        <v>153</v>
+        <v>142</v>
       </c>
       <c r="AL10" s="41" t="s">
-        <v>154</v>
+        <v>143</v>
       </c>
       <c r="AM10" s="41" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="AN10" s="41" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="AO10" s="41" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="AP10" s="41" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="AQ10" s="41" t="s">
-        <v>287</v>
+        <v>275</v>
       </c>
       <c r="AR10" s="41" t="s">
-        <v>288</v>
+        <v>276</v>
       </c>
       <c r="AS10" s="41" t="s">
-        <v>289</v>
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -3538,10 +3502,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="C1" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="D1" t="s">
         <v>44</v>
@@ -3549,16 +3513,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="1" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -4235,7 +4199,7 @@
     </row>
     <row r="8" spans="1:30" s="16" customFormat="1">
       <c r="A8" s="22" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B8" s="16">
         <v>0</v>
@@ -4551,103 +4515,103 @@
         <v>0</v>
       </c>
       <c r="B1" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="C1" s="25" t="s">
+        <v>237</v>
+      </c>
+      <c r="D1" s="25" t="s">
+        <v>238</v>
+      </c>
+      <c r="E1" s="28" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" s="28" t="s">
+        <v>212</v>
+      </c>
+      <c r="G1" s="28" t="s">
+        <v>203</v>
+      </c>
+      <c r="H1" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="I1" s="28" t="s">
+        <v>201</v>
+      </c>
+      <c r="J1" s="28" t="s">
+        <v>227</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>229</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>226</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>225</v>
+      </c>
+      <c r="O1" s="28" t="s">
+        <v>224</v>
+      </c>
+      <c r="P1" s="28" t="s">
+        <v>248</v>
+      </c>
+      <c r="Q1" s="28" t="s">
+        <v>250</v>
+      </c>
+      <c r="R1" s="28" t="s">
+        <v>243</v>
+      </c>
+      <c r="S1" s="28" t="s">
+        <v>245</v>
+      </c>
+      <c r="T1" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="U1" s="25" t="s">
+        <v>216</v>
+      </c>
+      <c r="V1" s="25" t="s">
+        <v>249</v>
+      </c>
+      <c r="W1" s="25" t="s">
+        <v>239</v>
+      </c>
+      <c r="X1" s="25" t="s">
+        <v>234</v>
+      </c>
+      <c r="Y1" s="25" t="s">
+        <v>233</v>
+      </c>
+      <c r="Z1" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="AA1" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="AB1" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="AC1" s="28" t="s">
+        <v>221</v>
+      </c>
+      <c r="AD1" s="28" t="s">
+        <v>222</v>
+      </c>
+      <c r="AE1" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="AF1" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="AG1" s="28" t="s">
+        <v>231</v>
+      </c>
+      <c r="AH1" s="28" t="s">
         <v>232</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>249</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>250</v>
-      </c>
-      <c r="E1" s="28" t="s">
-        <v>208</v>
-      </c>
-      <c r="F1" s="28" t="s">
-        <v>224</v>
-      </c>
-      <c r="G1" s="28" t="s">
-        <v>215</v>
-      </c>
-      <c r="H1" s="28" t="s">
-        <v>214</v>
-      </c>
-      <c r="I1" s="28" t="s">
-        <v>213</v>
-      </c>
-      <c r="J1" s="28" t="s">
-        <v>239</v>
-      </c>
-      <c r="K1" s="28" t="s">
-        <v>240</v>
-      </c>
-      <c r="L1" s="28" t="s">
-        <v>241</v>
-      </c>
-      <c r="M1" s="28" t="s">
-        <v>238</v>
-      </c>
-      <c r="N1" s="28" t="s">
-        <v>237</v>
-      </c>
-      <c r="O1" s="28" t="s">
-        <v>236</v>
-      </c>
-      <c r="P1" s="28" t="s">
-        <v>260</v>
-      </c>
-      <c r="Q1" s="28" t="s">
-        <v>262</v>
-      </c>
-      <c r="R1" s="28" t="s">
-        <v>255</v>
-      </c>
-      <c r="S1" s="28" t="s">
-        <v>257</v>
-      </c>
-      <c r="T1" s="28" t="s">
-        <v>259</v>
-      </c>
-      <c r="U1" s="25" t="s">
-        <v>228</v>
-      </c>
-      <c r="V1" s="25" t="s">
-        <v>261</v>
-      </c>
-      <c r="W1" s="25" t="s">
-        <v>251</v>
-      </c>
-      <c r="X1" s="25" t="s">
-        <v>246</v>
-      </c>
-      <c r="Y1" s="25" t="s">
-        <v>245</v>
-      </c>
-      <c r="Z1" s="28" t="s">
-        <v>229</v>
-      </c>
-      <c r="AA1" s="28" t="s">
-        <v>230</v>
-      </c>
-      <c r="AB1" s="28" t="s">
-        <v>231</v>
-      </c>
-      <c r="AC1" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="AD1" s="28" t="s">
-        <v>234</v>
-      </c>
-      <c r="AE1" s="28" t="s">
-        <v>235</v>
-      </c>
-      <c r="AF1" s="28" t="s">
-        <v>242</v>
-      </c>
-      <c r="AG1" s="28" t="s">
-        <v>243</v>
-      </c>
-      <c r="AH1" s="28" t="s">
-        <v>244</v>
       </c>
     </row>
     <row r="2" spans="1:34" s="26" customFormat="1">
@@ -5276,7 +5240,7 @@
     </row>
     <row r="8" spans="1:34" s="16" customFormat="1">
       <c r="A8" s="22" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B8" s="40">
         <v>0</v>
@@ -5487,57 +5451,57 @@
         <v>44</v>
       </c>
       <c r="B10" s="41" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="C10" s="42"/>
       <c r="D10" s="42"/>
       <c r="E10" s="41" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="F10" s="41" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="G10" s="41" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="H10" s="41" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="I10" s="41" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="J10" s="41" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="K10" s="41" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="L10" s="41" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="M10" s="41" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="N10" s="41" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="O10" s="41" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="P10" s="32" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="Q10" s="32" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="R10" s="32" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="S10" s="32" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="T10" s="32" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="U10" s="32" t="s">
         <v>78</v>
@@ -5549,31 +5513,31 @@
       <c r="X10" s="33"/>
       <c r="Y10" s="33"/>
       <c r="Z10" s="32" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="AA10" s="32" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="AB10" s="32" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="AC10" s="32" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="AD10" s="32" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="AE10" s="32" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="AF10" s="32" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="AG10" s="32" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="AH10" s="32" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -5631,7 +5595,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" spans="1:29" s="3" customFormat="1">
@@ -5692,7 +5656,7 @@
     </row>
     <row r="9" spans="1:29" s="3" customFormat="1">
       <c r="A9" s="3" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -5700,7 +5664,7 @@
     </row>
     <row r="10" spans="1:29" s="3" customFormat="1">
       <c r="A10" s="3" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -5889,7 +5853,7 @@
         <v>44</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="C13" s="34"/>
       <c r="D13" s="34"/>
@@ -5942,8 +5906,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:AC26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21:XFD22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -5975,7 +5939,7 @@
     <col min="31" max="16384" width="9" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="2" customFormat="1">
+    <row r="1" spans="1:22" s="2" customFormat="1">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -5983,7 +5947,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="2" spans="1:23" s="3" customFormat="1">
+    <row r="2" spans="1:22" s="3" customFormat="1">
       <c r="A2" s="3" t="s">
         <v>136</v>
       </c>
@@ -5991,15 +5955,15 @@
         <v>64</v>
       </c>
     </row>
-    <row r="3" spans="1:23" s="3" customFormat="1">
+    <row r="3" spans="1:22" s="3" customFormat="1">
       <c r="A3" s="3" t="s">
         <v>137</v>
       </c>
       <c r="B3" s="3">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" s="3" customFormat="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" s="3" customFormat="1">
       <c r="A4" s="3" t="s">
         <v>38</v>
       </c>
@@ -6007,7 +5971,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:23" s="3" customFormat="1">
+    <row r="5" spans="1:22" s="3" customFormat="1">
       <c r="A5" s="3" t="s">
         <v>39</v>
       </c>
@@ -6015,7 +5979,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:23" s="3" customFormat="1">
+    <row r="6" spans="1:22" s="3" customFormat="1">
       <c r="A6" s="3" t="s">
         <v>40</v>
       </c>
@@ -6023,7 +5987,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:23" s="3" customFormat="1">
+    <row r="7" spans="1:22" s="3" customFormat="1">
       <c r="A7" s="3" t="s">
         <v>41</v>
       </c>
@@ -6031,7 +5995,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:23" s="3" customFormat="1">
+    <row r="8" spans="1:22" s="3" customFormat="1">
       <c r="A8" s="3" t="s">
         <v>42</v>
       </c>
@@ -6039,15 +6003,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:23" s="3" customFormat="1">
+    <row r="9" spans="1:22" s="3" customFormat="1">
       <c r="A9" s="3" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:23" s="3" customFormat="1">
+    <row r="10" spans="1:22" s="3" customFormat="1">
       <c r="A10" s="3" t="s">
         <v>43</v>
       </c>
@@ -6055,7 +6019,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:23" s="3" customFormat="1">
+    <row r="11" spans="1:22" s="3" customFormat="1">
       <c r="A11" s="34" t="s">
         <v>138</v>
       </c>
@@ -6063,7 +6027,7 @@
         <v>139</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="D11" s="34" t="s">
         <v>6</v>
@@ -6074,59 +6038,8 @@
       <c r="F11" s="34" t="s">
         <v>141</v>
       </c>
-      <c r="G11" s="34" t="s">
-        <v>142</v>
-      </c>
-      <c r="H11" s="34" t="s">
-        <v>143</v>
-      </c>
-      <c r="I11" s="34" t="s">
-        <v>144</v>
-      </c>
-      <c r="J11" s="34" t="s">
-        <v>145</v>
-      </c>
-      <c r="K11" s="34" t="s">
-        <v>146</v>
-      </c>
-      <c r="L11" s="34" t="s">
-        <v>147</v>
-      </c>
-      <c r="M11" s="34" t="s">
-        <v>148</v>
-      </c>
-      <c r="N11" s="34" t="s">
-        <v>149</v>
-      </c>
-      <c r="O11" s="34" t="s">
-        <v>150</v>
-      </c>
-      <c r="P11" s="34" t="s">
-        <v>151</v>
-      </c>
-      <c r="Q11" s="34" t="s">
-        <v>152</v>
-      </c>
-      <c r="R11" s="34" t="s">
-        <v>153</v>
-      </c>
-      <c r="S11" s="34" t="s">
-        <v>154</v>
-      </c>
-      <c r="T11" s="34" t="s">
-        <v>155</v>
-      </c>
-      <c r="U11" s="34" t="s">
-        <v>156</v>
-      </c>
-      <c r="V11" s="34" t="s">
-        <v>157</v>
-      </c>
-      <c r="W11" s="34" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" s="3" customFormat="1">
+    </row>
+    <row r="12" spans="1:22" s="3" customFormat="1">
       <c r="A12" s="35" t="s">
         <v>37</v>
       </c>
@@ -6145,59 +6058,8 @@
       <c r="F12" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="G12" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="I12" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="J12" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="K12" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="L12" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="M12" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="N12" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="O12" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="P12" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="Q12" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="R12" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="S12" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="T12" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="U12" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="V12" s="34" t="s">
-        <v>35</v>
-      </c>
-      <c r="W12" s="34" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" s="3" customFormat="1">
+    </row>
+    <row r="13" spans="1:22" s="3" customFormat="1">
       <c r="A13" s="34" t="s">
         <v>44</v>
       </c>
@@ -6223,15 +6085,15 @@
       <c r="U13" s="34"/>
       <c r="V13" s="34"/>
     </row>
-    <row r="14" spans="1:23" s="2" customFormat="1">
+    <row r="14" spans="1:22" s="2" customFormat="1">
       <c r="A14" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>222</v>
-      </c>
-    </row>
-    <row r="15" spans="1:23" s="3" customFormat="1">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" s="3" customFormat="1">
       <c r="A15" s="3" t="s">
         <v>136</v>
       </c>
@@ -6239,7 +6101,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:23" s="3" customFormat="1">
+    <row r="16" spans="1:22" s="3" customFormat="1">
       <c r="A16" s="3" t="s">
         <v>137</v>
       </c>
@@ -6252,7 +6114,7 @@
         <v>38</v>
       </c>
       <c r="B17" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:29" s="3" customFormat="1">
@@ -6276,7 +6138,7 @@
         <v>41</v>
       </c>
       <c r="B20" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:29" s="3" customFormat="1">
@@ -6289,7 +6151,7 @@
     </row>
     <row r="22" spans="1:29" s="3" customFormat="1">
       <c r="A22" s="3" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B22" s="3">
         <v>0</v>
@@ -6486,7 +6348,7 @@
         <v>44</v>
       </c>
       <c r="B26" s="35" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="C26" s="34"/>
       <c r="D26" s="34"/>
@@ -6518,10 +6380,10 @@
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A19 C26 D8:G9 D26:G1048576 A4:B5 A17:B18 B6:B10 B19:B23 C14:G20 D21:G22" xr:uid="{00000000-0002-0000-0300-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A19 C26 D8:G9 D26:G1048576 A4:B5 G11 B6:B10 A17:B18 C14:G20 D21:G22 B19:B23" xr:uid="{00000000-0002-0000-0300-000000000000}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A25:C25 U25 D24:T25 V24:AC25 I8:AK9 I21:AK22" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="A25:C25 U25 D24:T25 V24:AC25 I8:AK9 I21:AK22 I11:X11" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>"int,string,float,object"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A15:B16 B27:C1048576 A2:B3 C8:C9 C21:C22" xr:uid="{00000000-0002-0000-0300-000002000000}">
@@ -6567,7 +6429,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>159</v>
+        <v>147</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
@@ -6775,7 +6637,7 @@
     </row>
     <row r="9" spans="1:23" s="3" customFormat="1">
       <c r="A9" s="3" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -6815,70 +6677,70 @@
         <v>138</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>160</v>
+        <v>148</v>
       </c>
       <c r="C11" s="34" t="s">
         <v>139</v>
       </c>
       <c r="D11" s="34" t="s">
+        <v>149</v>
+      </c>
+      <c r="E11" s="34" t="s">
+        <v>150</v>
+      </c>
+      <c r="F11" s="34" t="s">
+        <v>151</v>
+      </c>
+      <c r="G11" s="34" t="s">
+        <v>152</v>
+      </c>
+      <c r="H11" s="34" t="s">
+        <v>153</v>
+      </c>
+      <c r="I11" s="34" t="s">
+        <v>154</v>
+      </c>
+      <c r="J11" s="34" t="s">
+        <v>155</v>
+      </c>
+      <c r="K11" s="34" t="s">
+        <v>156</v>
+      </c>
+      <c r="L11" s="34" t="s">
+        <v>157</v>
+      </c>
+      <c r="M11" s="34" t="s">
+        <v>158</v>
+      </c>
+      <c r="N11" s="34" t="s">
+        <v>159</v>
+      </c>
+      <c r="O11" s="34" t="s">
+        <v>160</v>
+      </c>
+      <c r="P11" s="34" t="s">
         <v>161</v>
       </c>
-      <c r="E11" s="34" t="s">
+      <c r="Q11" s="34" t="s">
         <v>162</v>
       </c>
-      <c r="F11" s="34" t="s">
+      <c r="R11" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="G11" s="34" t="s">
+      <c r="S11" s="34" t="s">
         <v>164</v>
       </c>
-      <c r="H11" s="34" t="s">
+      <c r="T11" s="34" t="s">
         <v>165</v>
       </c>
-      <c r="I11" s="34" t="s">
+      <c r="U11" s="34" t="s">
         <v>166</v>
       </c>
-      <c r="J11" s="34" t="s">
+      <c r="V11" s="34" t="s">
         <v>167</v>
       </c>
-      <c r="K11" s="34" t="s">
+      <c r="W11" s="34" t="s">
         <v>168</v>
-      </c>
-      <c r="L11" s="34" t="s">
-        <v>169</v>
-      </c>
-      <c r="M11" s="34" t="s">
-        <v>170</v>
-      </c>
-      <c r="N11" s="34" t="s">
-        <v>171</v>
-      </c>
-      <c r="O11" s="34" t="s">
-        <v>172</v>
-      </c>
-      <c r="P11" s="34" t="s">
-        <v>173</v>
-      </c>
-      <c r="Q11" s="34" t="s">
-        <v>174</v>
-      </c>
-      <c r="R11" s="34" t="s">
-        <v>175</v>
-      </c>
-      <c r="S11" s="34" t="s">
-        <v>176</v>
-      </c>
-      <c r="T11" s="34" t="s">
-        <v>177</v>
-      </c>
-      <c r="U11" s="34" t="s">
-        <v>178</v>
-      </c>
-      <c r="V11" s="34" t="s">
-        <v>179</v>
-      </c>
-      <c r="W11" s="34" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="12" spans="1:23" s="12" customFormat="1">
@@ -6957,7 +6819,7 @@
         <v>44</v>
       </c>
       <c r="B13" s="35" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="C13" s="34"/>
       <c r="D13" s="34"/>
@@ -6986,7 +6848,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>182</v>
+        <v>170</v>
       </c>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -7194,7 +7056,7 @@
     </row>
     <row r="22" spans="1:23" s="3" customFormat="1">
       <c r="A22" s="3" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B22" s="3">
         <v>0</v>
@@ -7234,16 +7096,16 @@
         <v>139</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>184</v>
+        <v>172</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>161</v>
+        <v>149</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
     </row>
     <row r="25" spans="1:23" s="13" customFormat="1">
@@ -7268,7 +7130,7 @@
         <v>44</v>
       </c>
       <c r="B26" s="35" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="C26" s="34"/>
       <c r="D26" s="34"/>
@@ -7297,7 +7159,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -7505,7 +7367,7 @@
     </row>
     <row r="35" spans="1:23" s="3" customFormat="1">
       <c r="A35" s="3" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B35" s="3">
         <v>0</v>
@@ -7548,10 +7410,10 @@
         <v>139</v>
       </c>
       <c r="C37" s="34" t="s">
-        <v>183</v>
+        <v>171</v>
       </c>
       <c r="D37" s="35" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
     </row>
     <row r="38" spans="1:23" s="13" customFormat="1">
@@ -7565,7 +7427,7 @@
         <v>36</v>
       </c>
       <c r="D38" s="35" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
     </row>
     <row r="39" spans="1:23" s="13" customFormat="1">
@@ -7641,7 +7503,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="6" customFormat="1">
@@ -7702,7 +7564,7 @@
     </row>
     <row r="9" spans="1:4" s="3" customFormat="1">
       <c r="A9" s="3" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -7710,7 +7572,7 @@
     </row>
     <row r="10" spans="1:4" s="6" customFormat="1">
       <c r="A10" s="9" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B10" s="9">
         <v>0</v>
@@ -7718,16 +7580,16 @@
     </row>
     <row r="11" spans="1:4" s="6" customFormat="1">
       <c r="A11" s="36" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="B11" s="36" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="C11" s="36" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="D11" s="36" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
     </row>
     <row r="12" spans="1:4" s="6" customFormat="1">
@@ -7749,7 +7611,7 @@
         <v>44</v>
       </c>
       <c r="B13" s="38" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="C13" s="36"/>
       <c r="D13" s="36"/>
@@ -7759,7 +7621,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
     </row>
     <row r="15" spans="1:4" s="6" customFormat="1">
@@ -7820,7 +7682,7 @@
     </row>
     <row r="22" spans="1:3" s="3" customFormat="1">
       <c r="A22" s="3" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B22" s="3">
         <v>0</v>
@@ -7828,7 +7690,7 @@
     </row>
     <row r="23" spans="1:3" s="6" customFormat="1">
       <c r="A23" s="9" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B23" s="9">
         <v>0</v>
@@ -7836,13 +7698,13 @@
     </row>
     <row r="24" spans="1:3" s="6" customFormat="1">
       <c r="A24" s="36" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="B24" s="36" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="C24" s="36" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
     </row>
     <row r="25" spans="1:3" s="6" customFormat="1">
@@ -7861,7 +7723,7 @@
         <v>44</v>
       </c>
       <c r="B26" s="38" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="C26" s="36"/>
     </row>
@@ -7916,7 +7778,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" spans="1:43" s="6" customFormat="1">
@@ -7977,7 +7839,7 @@
     </row>
     <row r="9" spans="1:43" s="3" customFormat="1">
       <c r="A9" s="3" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -7985,7 +7847,7 @@
     </row>
     <row r="10" spans="1:43" s="6" customFormat="1" ht="13.9" thickBot="1">
       <c r="A10" s="9" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B10" s="9">
         <v>0</v>
@@ -7993,133 +7855,133 @@
     </row>
     <row r="11" spans="1:43" s="6" customFormat="1" ht="42.75">
       <c r="A11" s="43" t="s">
+        <v>248</v>
+      </c>
+      <c r="B11" s="44" t="s">
+        <v>252</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="D11" s="44" t="s">
+        <v>254</v>
+      </c>
+      <c r="E11" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="F11" s="44" t="s">
+        <v>256</v>
+      </c>
+      <c r="G11" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="H11" s="45" t="s">
+        <v>258</v>
+      </c>
+      <c r="I11" s="45" t="s">
+        <v>259</v>
+      </c>
+      <c r="J11" s="44" t="s">
         <v>260</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="K11" s="44" t="s">
+        <v>261</v>
+      </c>
+      <c r="L11" s="44" t="s">
+        <v>262</v>
+      </c>
+      <c r="M11" s="44" t="s">
+        <v>263</v>
+      </c>
+      <c r="N11" s="44" t="s">
         <v>264</v>
       </c>
-      <c r="C11" s="44" t="s">
+      <c r="O11" s="44" t="s">
         <v>265</v>
       </c>
-      <c r="D11" s="44" t="s">
+      <c r="P11" s="44" t="s">
         <v>266</v>
       </c>
-      <c r="E11" s="44" t="s">
+      <c r="Q11" s="44" t="s">
         <v>267</v>
       </c>
-      <c r="F11" s="44" t="s">
+      <c r="R11" s="44" t="s">
         <v>268</v>
       </c>
-      <c r="G11" s="44" t="s">
+      <c r="S11" s="44" t="s">
         <v>269</v>
       </c>
-      <c r="H11" s="45" t="s">
+      <c r="T11" s="44" t="s">
         <v>270</v>
       </c>
-      <c r="I11" s="45" t="s">
+      <c r="U11" s="44" t="s">
         <v>271</v>
-      </c>
-      <c r="J11" s="44" t="s">
-        <v>272</v>
-      </c>
-      <c r="K11" s="44" t="s">
-        <v>273</v>
-      </c>
-      <c r="L11" s="44" t="s">
-        <v>274</v>
-      </c>
-      <c r="M11" s="44" t="s">
-        <v>275</v>
-      </c>
-      <c r="N11" s="44" t="s">
-        <v>276</v>
-      </c>
-      <c r="O11" s="44" t="s">
-        <v>277</v>
-      </c>
-      <c r="P11" s="44" t="s">
-        <v>278</v>
-      </c>
-      <c r="Q11" s="44" t="s">
-        <v>279</v>
-      </c>
-      <c r="R11" s="44" t="s">
-        <v>280</v>
-      </c>
-      <c r="S11" s="44" t="s">
-        <v>281</v>
-      </c>
-      <c r="T11" s="44" t="s">
-        <v>282</v>
-      </c>
-      <c r="U11" s="44" t="s">
-        <v>283</v>
       </c>
       <c r="V11" s="44" t="s">
         <v>17</v>
       </c>
       <c r="W11" s="44" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="X11" s="44" t="s">
+        <v>272</v>
+      </c>
+      <c r="Y11" s="45" t="s">
+        <v>273</v>
+      </c>
+      <c r="Z11" s="44" t="s">
+        <v>251</v>
+      </c>
+      <c r="AA11" s="44" t="s">
+        <v>274</v>
+      </c>
+      <c r="AB11" s="44" t="s">
+        <v>242</v>
+      </c>
+      <c r="AC11" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="AD11" s="44" t="s">
+        <v>244</v>
+      </c>
+      <c r="AE11" s="44" t="s">
+        <v>276</v>
+      </c>
+      <c r="AF11" s="44" t="s">
+        <v>246</v>
+      </c>
+      <c r="AG11" s="44" t="s">
+        <v>277</v>
+      </c>
+      <c r="AH11" s="44" t="s">
+        <v>278</v>
+      </c>
+      <c r="AI11" s="44" t="s">
+        <v>279</v>
+      </c>
+      <c r="AJ11" s="44" t="s">
+        <v>280</v>
+      </c>
+      <c r="AK11" s="44" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL11" s="45" t="s">
+        <v>282</v>
+      </c>
+      <c r="AM11" s="45" t="s">
+        <v>283</v>
+      </c>
+      <c r="AN11" s="45" t="s">
         <v>284</v>
       </c>
-      <c r="Y11" s="45" t="s">
+      <c r="AO11" s="45" t="s">
         <v>285</v>
       </c>
-      <c r="Z11" s="44" t="s">
-        <v>263</v>
-      </c>
-      <c r="AA11" s="44" t="s">
+      <c r="AP11" s="45" t="s">
         <v>286</v>
       </c>
-      <c r="AB11" s="44" t="s">
-        <v>254</v>
-      </c>
-      <c r="AC11" s="44" t="s">
+      <c r="AQ11" s="45" t="s">
         <v>287</v>
-      </c>
-      <c r="AD11" s="44" t="s">
-        <v>256</v>
-      </c>
-      <c r="AE11" s="44" t="s">
-        <v>288</v>
-      </c>
-      <c r="AF11" s="44" t="s">
-        <v>258</v>
-      </c>
-      <c r="AG11" s="44" t="s">
-        <v>289</v>
-      </c>
-      <c r="AH11" s="44" t="s">
-        <v>290</v>
-      </c>
-      <c r="AI11" s="44" t="s">
-        <v>291</v>
-      </c>
-      <c r="AJ11" s="44" t="s">
-        <v>292</v>
-      </c>
-      <c r="AK11" s="44" t="s">
-        <v>293</v>
-      </c>
-      <c r="AL11" s="45" t="s">
-        <v>294</v>
-      </c>
-      <c r="AM11" s="45" t="s">
-        <v>295</v>
-      </c>
-      <c r="AN11" s="45" t="s">
-        <v>296</v>
-      </c>
-      <c r="AO11" s="45" t="s">
-        <v>297</v>
-      </c>
-      <c r="AP11" s="45" t="s">
-        <v>298</v>
-      </c>
-      <c r="AQ11" s="45" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="12" spans="1:43" s="6" customFormat="1" ht="14.25">
@@ -8389,7 +8251,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="8" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
     </row>
     <row r="15" spans="1:43" s="6" customFormat="1">
@@ -8450,7 +8312,7 @@
     </row>
     <row r="22" spans="1:43" s="3" customFormat="1">
       <c r="A22" s="3" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B22" s="3">
         <v>0</v>
@@ -8458,7 +8320,7 @@
     </row>
     <row r="23" spans="1:43" s="6" customFormat="1" ht="13.9" thickBot="1">
       <c r="A23" s="9" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="B23" s="9">
         <v>0</v>
@@ -8466,133 +8328,133 @@
     </row>
     <row r="24" spans="1:43" s="6" customFormat="1" ht="42.75">
       <c r="A24" s="43" t="s">
+        <v>248</v>
+      </c>
+      <c r="B24" s="44" t="s">
+        <v>252</v>
+      </c>
+      <c r="C24" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="D24" s="44" t="s">
+        <v>254</v>
+      </c>
+      <c r="E24" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="F24" s="44" t="s">
+        <v>256</v>
+      </c>
+      <c r="G24" s="44" t="s">
+        <v>257</v>
+      </c>
+      <c r="H24" s="45" t="s">
+        <v>258</v>
+      </c>
+      <c r="I24" s="45" t="s">
+        <v>259</v>
+      </c>
+      <c r="J24" s="44" t="s">
         <v>260</v>
       </c>
-      <c r="B24" s="44" t="s">
+      <c r="K24" s="44" t="s">
+        <v>261</v>
+      </c>
+      <c r="L24" s="44" t="s">
+        <v>262</v>
+      </c>
+      <c r="M24" s="44" t="s">
+        <v>263</v>
+      </c>
+      <c r="N24" s="44" t="s">
         <v>264</v>
       </c>
-      <c r="C24" s="44" t="s">
+      <c r="O24" s="44" t="s">
         <v>265</v>
       </c>
-      <c r="D24" s="44" t="s">
+      <c r="P24" s="44" t="s">
         <v>266</v>
       </c>
-      <c r="E24" s="44" t="s">
+      <c r="Q24" s="44" t="s">
         <v>267</v>
       </c>
-      <c r="F24" s="44" t="s">
+      <c r="R24" s="44" t="s">
         <v>268</v>
       </c>
-      <c r="G24" s="44" t="s">
+      <c r="S24" s="44" t="s">
         <v>269</v>
       </c>
-      <c r="H24" s="45" t="s">
+      <c r="T24" s="44" t="s">
         <v>270</v>
       </c>
-      <c r="I24" s="45" t="s">
+      <c r="U24" s="44" t="s">
         <v>271</v>
-      </c>
-      <c r="J24" s="44" t="s">
-        <v>272</v>
-      </c>
-      <c r="K24" s="44" t="s">
-        <v>273</v>
-      </c>
-      <c r="L24" s="44" t="s">
-        <v>274</v>
-      </c>
-      <c r="M24" s="44" t="s">
-        <v>275</v>
-      </c>
-      <c r="N24" s="44" t="s">
-        <v>276</v>
-      </c>
-      <c r="O24" s="44" t="s">
-        <v>277</v>
-      </c>
-      <c r="P24" s="44" t="s">
-        <v>278</v>
-      </c>
-      <c r="Q24" s="44" t="s">
-        <v>279</v>
-      </c>
-      <c r="R24" s="44" t="s">
-        <v>280</v>
-      </c>
-      <c r="S24" s="44" t="s">
-        <v>281</v>
-      </c>
-      <c r="T24" s="44" t="s">
-        <v>282</v>
-      </c>
-      <c r="U24" s="44" t="s">
-        <v>283</v>
       </c>
       <c r="V24" s="44" t="s">
         <v>17</v>
       </c>
       <c r="W24" s="44" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="X24" s="44" t="s">
+        <v>272</v>
+      </c>
+      <c r="Y24" s="45" t="s">
+        <v>273</v>
+      </c>
+      <c r="Z24" s="44" t="s">
+        <v>251</v>
+      </c>
+      <c r="AA24" s="44" t="s">
+        <v>274</v>
+      </c>
+      <c r="AB24" s="44" t="s">
+        <v>242</v>
+      </c>
+      <c r="AC24" s="44" t="s">
+        <v>275</v>
+      </c>
+      <c r="AD24" s="44" t="s">
+        <v>244</v>
+      </c>
+      <c r="AE24" s="44" t="s">
+        <v>276</v>
+      </c>
+      <c r="AF24" s="44" t="s">
+        <v>246</v>
+      </c>
+      <c r="AG24" s="44" t="s">
+        <v>277</v>
+      </c>
+      <c r="AH24" s="44" t="s">
+        <v>278</v>
+      </c>
+      <c r="AI24" s="44" t="s">
+        <v>279</v>
+      </c>
+      <c r="AJ24" s="44" t="s">
+        <v>280</v>
+      </c>
+      <c r="AK24" s="44" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL24" s="45" t="s">
+        <v>282</v>
+      </c>
+      <c r="AM24" s="45" t="s">
+        <v>283</v>
+      </c>
+      <c r="AN24" s="45" t="s">
         <v>284</v>
       </c>
-      <c r="Y24" s="45" t="s">
+      <c r="AO24" s="45" t="s">
         <v>285</v>
       </c>
-      <c r="Z24" s="44" t="s">
-        <v>263</v>
-      </c>
-      <c r="AA24" s="44" t="s">
+      <c r="AP24" s="45" t="s">
         <v>286</v>
       </c>
-      <c r="AB24" s="44" t="s">
-        <v>254</v>
-      </c>
-      <c r="AC24" s="44" t="s">
+      <c r="AQ24" s="45" t="s">
         <v>287</v>
-      </c>
-      <c r="AD24" s="44" t="s">
-        <v>256</v>
-      </c>
-      <c r="AE24" s="44" t="s">
-        <v>288</v>
-      </c>
-      <c r="AF24" s="44" t="s">
-        <v>258</v>
-      </c>
-      <c r="AG24" s="44" t="s">
-        <v>289</v>
-      </c>
-      <c r="AH24" s="44" t="s">
-        <v>290</v>
-      </c>
-      <c r="AI24" s="44" t="s">
-        <v>291</v>
-      </c>
-      <c r="AJ24" s="44" t="s">
-        <v>292</v>
-      </c>
-      <c r="AK24" s="44" t="s">
-        <v>293</v>
-      </c>
-      <c r="AL24" s="45" t="s">
-        <v>294</v>
-      </c>
-      <c r="AM24" s="45" t="s">
-        <v>295</v>
-      </c>
-      <c r="AN24" s="45" t="s">
-        <v>296</v>
-      </c>
-      <c r="AO24" s="45" t="s">
-        <v>297</v>
-      </c>
-      <c r="AP24" s="45" t="s">
-        <v>298</v>
-      </c>
-      <c r="AQ24" s="45" t="s">
-        <v>299</v>
       </c>
     </row>
     <row r="25" spans="1:43" s="6" customFormat="1" ht="14.25">
@@ -8908,7 +8770,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" spans="1:5" s="3" customFormat="1">
@@ -8969,7 +8831,7 @@
     </row>
     <row r="9" spans="1:5" s="3" customFormat="1">
       <c r="A9" s="3" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -8977,7 +8839,7 @@
     </row>
     <row r="10" spans="1:5" s="3" customFormat="1">
       <c r="A10" s="3" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -8985,19 +8847,19 @@
     </row>
     <row r="11" spans="1:5" s="3" customFormat="1">
       <c r="A11" s="34" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="B11" s="34" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="C11" s="34" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="D11" s="34" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="E11" s="34" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="3" customFormat="1">
@@ -9011,7 +8873,7 @@
         <v>36</v>
       </c>
       <c r="D12" s="34" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="E12" s="34" t="s">
         <v>36</v>
@@ -9031,7 +8893,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="3" customFormat="1">
@@ -9092,7 +8954,7 @@
     </row>
     <row r="22" spans="1:5" s="3" customFormat="1">
       <c r="A22" s="3" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="B22" s="3">
         <v>0</v>
@@ -9108,19 +8970,19 @@
     </row>
     <row r="24" spans="1:5" s="3" customFormat="1">
       <c r="A24" s="34" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="B24" s="34" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="C24" s="34" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="D24" s="34" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="E24" s="34" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
     </row>
     <row r="25" spans="1:5" s="3" customFormat="1">
@@ -9134,7 +8996,7 @@
         <v>36</v>
       </c>
       <c r="D25" s="34" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="E25" s="34" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
opponent's buildings, tiles and heros
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Player.xlsx
+++ b/_Out/NFDataCfg/Excel/Player.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18730"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="458" windowWidth="28043" windowHeight="17543" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="458" windowWidth="28043" windowHeight="17543" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1077" uniqueCount="349">
   <si>
     <t>Id</t>
   </si>
@@ -1507,6 +1507,18 @@
   </si>
   <si>
     <t>Guild_WarList</t>
+  </si>
+  <si>
+    <t>HeroID1</t>
+  </si>
+  <si>
+    <t>HeroID2</t>
+  </si>
+  <si>
+    <t>HeroID3</t>
+  </si>
+  <si>
+    <t>vector</t>
   </si>
 </sst>
 </file>
@@ -6167,10 +6179,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972B7153-9DF5-4ED6-8C38-DB6612A94CE8}">
-  <dimension ref="A1:AH10"/>
+  <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -6178,18 +6190,20 @@
     <col min="1" max="1" width="23.796875" customWidth="1"/>
     <col min="2" max="2" width="18.33203125" customWidth="1"/>
     <col min="3" max="4" width="16" customWidth="1"/>
-    <col min="5" max="15" width="17.33203125" customWidth="1"/>
-    <col min="16" max="17" width="18.33203125" customWidth="1"/>
-    <col min="18" max="20" width="17.33203125" customWidth="1"/>
-    <col min="21" max="21" width="15.6640625" customWidth="1"/>
-    <col min="22" max="22" width="14.46484375" customWidth="1"/>
-    <col min="23" max="25" width="16" customWidth="1"/>
-    <col min="26" max="28" width="17.33203125" customWidth="1"/>
-    <col min="29" max="31" width="18.33203125" customWidth="1"/>
-    <col min="32" max="34" width="17.33203125" customWidth="1"/>
+    <col min="5" max="18" width="17.33203125" customWidth="1"/>
+    <col min="19" max="20" width="18.33203125" customWidth="1"/>
+    <col min="21" max="23" width="17.33203125" customWidth="1"/>
+    <col min="24" max="24" width="15.6640625" customWidth="1"/>
+    <col min="25" max="25" width="14.46484375" customWidth="1"/>
+    <col min="26" max="28" width="16" customWidth="1"/>
+    <col min="29" max="29" width="17.33203125" customWidth="1"/>
+    <col min="30" max="30" width="20" customWidth="1"/>
+    <col min="31" max="31" width="17.33203125" customWidth="1"/>
+    <col min="32" max="34" width="18.33203125" customWidth="1"/>
+    <col min="35" max="37" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" s="25" customFormat="1">
+    <row r="1" spans="1:37" s="25" customFormat="1">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
@@ -6218,82 +6232,91 @@
         <v>201</v>
       </c>
       <c r="J1" s="28" t="s">
+        <v>345</v>
+      </c>
+      <c r="K1" s="28" t="s">
+        <v>346</v>
+      </c>
+      <c r="L1" s="28" t="s">
+        <v>347</v>
+      </c>
+      <c r="M1" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="K1" s="28" t="s">
+      <c r="N1" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="L1" s="28" t="s">
+      <c r="O1" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="P1" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="Q1" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="R1" s="28" t="s">
         <v>224</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="S1" s="28" t="s">
         <v>248</v>
       </c>
-      <c r="Q1" s="28" t="s">
+      <c r="T1" s="28" t="s">
         <v>250</v>
       </c>
-      <c r="R1" s="28" t="s">
+      <c r="U1" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="S1" s="28" t="s">
+      <c r="V1" s="28" t="s">
         <v>245</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="W1" s="28" t="s">
         <v>247</v>
       </c>
-      <c r="U1" s="25" t="s">
+      <c r="X1" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="V1" s="25" t="s">
+      <c r="Y1" s="25" t="s">
         <v>249</v>
       </c>
-      <c r="W1" s="25" t="s">
+      <c r="Z1" s="25" t="s">
         <v>239</v>
       </c>
-      <c r="X1" s="25" t="s">
+      <c r="AA1" s="25" t="s">
         <v>234</v>
       </c>
-      <c r="Y1" s="25" t="s">
+      <c r="AB1" s="25" t="s">
         <v>233</v>
       </c>
-      <c r="Z1" s="28" t="s">
+      <c r="AC1" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="AA1" s="28" t="s">
+      <c r="AD1" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="AB1" s="28" t="s">
+      <c r="AE1" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="AC1" s="28" t="s">
+      <c r="AF1" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="AD1" s="28" t="s">
+      <c r="AG1" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="AE1" s="28" t="s">
+      <c r="AH1" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="AF1" s="28" t="s">
+      <c r="AI1" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="AG1" s="28" t="s">
+      <c r="AJ1" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="AH1" s="28" t="s">
+      <c r="AK1" s="28" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="2" spans="1:34" s="26" customFormat="1">
+    <row r="2" spans="1:37" s="26" customFormat="1">
       <c r="A2" s="29" t="s">
         <v>34</v>
       </c>
@@ -6313,73 +6336,73 @@
         <v>35</v>
       </c>
       <c r="G2" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="H2" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>348</v>
+      </c>
+      <c r="J2" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="H2" s="39" t="s">
+      <c r="K2" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="I2" s="39" t="s">
+      <c r="L2" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="39" t="s">
+      <c r="M2" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="39" t="s">
+      <c r="N2" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="L2" s="39" t="s">
+      <c r="O2" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="N2" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="O2" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="P2" s="30" t="s">
+      <c r="P2" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="Q2" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="R2" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" s="30" t="s">
-        <v>36</v>
-      </c>
       <c r="T2" s="30" t="s">
         <v>36</v>
       </c>
       <c r="U2" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="V2" s="30" t="s">
+      <c r="Y2" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="W2" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="Y2" s="30" t="s">
-        <v>36</v>
-      </c>
       <c r="Z2" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2" s="30" t="s">
         <v>35</v>
-      </c>
-      <c r="AA2" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="AB2" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="AC2" s="30" t="s">
-        <v>36</v>
       </c>
       <c r="AD2" s="30" t="s">
         <v>35</v>
@@ -6391,13 +6414,22 @@
         <v>36</v>
       </c>
       <c r="AG2" s="30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="AH2" s="30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:34" s="26" customFormat="1">
+        <v>35</v>
+      </c>
+      <c r="AI2" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AJ2" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AK2" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:37" s="26" customFormat="1">
       <c r="A3" s="29" t="s">
         <v>38</v>
       </c>
@@ -6443,19 +6475,19 @@
       <c r="O3" s="39">
         <v>0</v>
       </c>
-      <c r="P3" s="31">
-        <v>0</v>
-      </c>
-      <c r="Q3" s="31">
-        <v>0</v>
-      </c>
-      <c r="R3" s="30">
-        <v>0</v>
-      </c>
-      <c r="S3" s="30">
-        <v>0</v>
-      </c>
-      <c r="T3" s="30">
+      <c r="P3" s="39">
+        <v>0</v>
+      </c>
+      <c r="Q3" s="39">
+        <v>0</v>
+      </c>
+      <c r="R3" s="39">
+        <v>0</v>
+      </c>
+      <c r="S3" s="31">
+        <v>0</v>
+      </c>
+      <c r="T3" s="31">
         <v>0</v>
       </c>
       <c r="U3" s="30">
@@ -6482,26 +6514,35 @@
       <c r="AB3" s="30">
         <v>0</v>
       </c>
-      <c r="AC3" s="31">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="31">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="31">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="30">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="30">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="30">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:34" s="26" customFormat="1">
+      <c r="AC3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="31">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="31">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:37" s="26" customFormat="1">
       <c r="A4" s="29" t="s">
         <v>39</v>
       </c>
@@ -6547,13 +6588,13 @@
       <c r="O4" s="39">
         <v>1</v>
       </c>
-      <c r="P4" s="30">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="30">
-        <v>1</v>
-      </c>
-      <c r="R4" s="30">
+      <c r="P4" s="39">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="39">
+        <v>1</v>
+      </c>
+      <c r="R4" s="39">
         <v>1</v>
       </c>
       <c r="S4" s="30">
@@ -6604,8 +6645,17 @@
       <c r="AH4" s="30">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:34" s="26" customFormat="1">
+      <c r="AI4" s="30">
+        <v>1</v>
+      </c>
+      <c r="AJ4" s="30">
+        <v>1</v>
+      </c>
+      <c r="AK4" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" s="26" customFormat="1">
       <c r="A5" s="29" t="s">
         <v>40</v>
       </c>
@@ -6651,13 +6701,13 @@
       <c r="O5" s="40">
         <v>0</v>
       </c>
-      <c r="P5" s="31">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="31">
-        <v>0</v>
-      </c>
-      <c r="R5" s="31">
+      <c r="P5" s="40">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="40">
+        <v>0</v>
+      </c>
+      <c r="R5" s="40">
         <v>0</v>
       </c>
       <c r="S5" s="31">
@@ -6708,8 +6758,17 @@
       <c r="AH5" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:34" s="26" customFormat="1">
+      <c r="AI5" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ5" s="31">
+        <v>0</v>
+      </c>
+      <c r="AK5" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" s="26" customFormat="1">
       <c r="A6" s="29" t="s">
         <v>41</v>
       </c>
@@ -6755,19 +6814,19 @@
       <c r="O6" s="40">
         <v>1</v>
       </c>
-      <c r="P6" s="30">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="30">
-        <v>1</v>
-      </c>
-      <c r="R6" s="31">
-        <v>1</v>
-      </c>
-      <c r="S6" s="31">
-        <v>1</v>
-      </c>
-      <c r="T6" s="31">
+      <c r="P6" s="40">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="40">
+        <v>1</v>
+      </c>
+      <c r="R6" s="40">
+        <v>1</v>
+      </c>
+      <c r="S6" s="30">
+        <v>1</v>
+      </c>
+      <c r="T6" s="30">
         <v>1</v>
       </c>
       <c r="U6" s="31">
@@ -6794,26 +6853,35 @@
       <c r="AB6" s="31">
         <v>1</v>
       </c>
-      <c r="AC6" s="30">
-        <v>1</v>
-      </c>
-      <c r="AD6" s="30">
-        <v>1</v>
-      </c>
-      <c r="AE6" s="30">
-        <v>1</v>
-      </c>
-      <c r="AF6" s="31">
-        <v>1</v>
-      </c>
-      <c r="AG6" s="31">
-        <v>1</v>
-      </c>
-      <c r="AH6" s="31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="1:34" s="16" customFormat="1">
+      <c r="AC6" s="31">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="31">
+        <v>1</v>
+      </c>
+      <c r="AE6" s="31">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="30">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="30">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="30">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="31">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="31">
+        <v>1</v>
+      </c>
+      <c r="AK6" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" s="16" customFormat="1">
       <c r="A7" s="22" t="s">
         <v>42</v>
       </c>
@@ -6859,13 +6927,13 @@
       <c r="O7" s="40">
         <v>0</v>
       </c>
-      <c r="P7" s="31">
-        <v>0</v>
-      </c>
-      <c r="Q7" s="31">
-        <v>0</v>
-      </c>
-      <c r="R7" s="31">
+      <c r="P7" s="40">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="40">
+        <v>0</v>
+      </c>
+      <c r="R7" s="40">
         <v>0</v>
       </c>
       <c r="S7" s="31">
@@ -6916,8 +6984,17 @@
       <c r="AH7" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:34" s="16" customFormat="1">
+      <c r="AI7" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ7" s="31">
+        <v>0</v>
+      </c>
+      <c r="AK7" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" s="16" customFormat="1">
       <c r="A8" s="22" t="s">
         <v>209</v>
       </c>
@@ -6963,13 +7040,13 @@
       <c r="O8" s="40">
         <v>0</v>
       </c>
-      <c r="P8" s="31">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="31">
-        <v>0</v>
-      </c>
-      <c r="R8" s="31">
+      <c r="P8" s="40">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="40">
+        <v>0</v>
+      </c>
+      <c r="R8" s="40">
         <v>0</v>
       </c>
       <c r="S8" s="31">
@@ -7020,8 +7097,17 @@
       <c r="AH8" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:34" s="16" customFormat="1">
+      <c r="AI8" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ8" s="31">
+        <v>0</v>
+      </c>
+      <c r="AK8" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" s="16" customFormat="1">
       <c r="A9" s="22" t="s">
         <v>43</v>
       </c>
@@ -7067,13 +7153,13 @@
       <c r="O9" s="40">
         <v>0</v>
       </c>
-      <c r="P9" s="31">
-        <v>0</v>
-      </c>
-      <c r="Q9" s="31">
-        <v>0</v>
-      </c>
-      <c r="R9" s="31">
+      <c r="P9" s="40">
+        <v>0</v>
+      </c>
+      <c r="Q9" s="40">
+        <v>0</v>
+      </c>
+      <c r="R9" s="40">
         <v>0</v>
       </c>
       <c r="S9" s="31">
@@ -7124,8 +7210,17 @@
       <c r="AH9" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:34" s="17" customFormat="1" ht="27.4" thickBot="1">
+      <c r="AI9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" s="17" customFormat="1" ht="27.4" thickBot="1">
       <c r="A10" s="23" t="s">
         <v>44</v>
       </c>
@@ -7167,62 +7262,71 @@
       <c r="O10" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="P10" s="32" t="s">
+      <c r="P10" s="41" t="s">
+        <v>198</v>
+      </c>
+      <c r="Q10" s="41" t="s">
+        <v>199</v>
+      </c>
+      <c r="R10" s="41" t="s">
+        <v>200</v>
+      </c>
+      <c r="S10" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="Q10" s="32" t="s">
+      <c r="T10" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="R10" s="32" t="s">
+      <c r="U10" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="S10" s="32" t="s">
+      <c r="V10" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="T10" s="32" t="s">
+      <c r="W10" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="U10" s="32" t="s">
+      <c r="X10" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="V10" s="32" t="s">
+      <c r="Y10" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="W10" s="33"/>
-      <c r="X10" s="33"/>
-      <c r="Y10" s="33"/>
-      <c r="Z10" s="32" t="s">
+      <c r="Z10" s="33"/>
+      <c r="AA10" s="33"/>
+      <c r="AB10" s="33"/>
+      <c r="AC10" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="AA10" s="32" t="s">
+      <c r="AD10" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="AB10" s="32" t="s">
+      <c r="AE10" s="32" t="s">
         <v>200</v>
       </c>
-      <c r="AC10" s="32" t="s">
+      <c r="AF10" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="AD10" s="32" t="s">
+      <c r="AG10" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="AE10" s="32" t="s">
+      <c r="AH10" s="32" t="s">
         <v>220</v>
       </c>
-      <c r="AF10" s="32" t="s">
+      <c r="AI10" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="AG10" s="32" t="s">
+      <c r="AJ10" s="32" t="s">
         <v>199</v>
       </c>
-      <c r="AH10" s="32" t="s">
+      <c r="AK10" s="32" t="s">
         <v>200</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9" xr:uid="{C5B45FAA-DDA2-4923-883B-BDBA94013D24}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AC5:AH5 C7:D9 AF6:AH9 B5 E6:F9 G5:AB9" xr:uid="{9492378F-A71A-4DF6-9127-6F1B0B990504}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="AF5:AK5 C7:D9 AI6:AK9 B5 E6:F9 G5:AE9" xr:uid="{9492378F-A71A-4DF6-9127-6F1B0B990504}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -7235,7 +7339,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA8B9599-45C4-4EAA-B7BD-89CEB0CA8449}">
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
+    <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="Q1" sqref="Q1:Q1048576"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add born position for heroes
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Player.xlsx
+++ b/_Out/NFDataCfg/Excel/Player.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="458" windowWidth="28043" windowHeight="17543" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="458" windowWidth="28043" windowHeight="17543" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -434,7 +434,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1099" uniqueCount="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="359">
   <si>
     <t>Id</t>
   </si>
@@ -1531,6 +1531,24 @@
   </si>
   <si>
     <t>hero等级</t>
+  </si>
+  <si>
+    <t>Hero1BornPos</t>
+  </si>
+  <si>
+    <t>Hero3BornPos</t>
+  </si>
+  <si>
+    <t>Hero2BornPos</t>
+  </si>
+  <si>
+    <t>OpponentHero1BornPos</t>
+  </si>
+  <si>
+    <t>OpponentHero2BornPos</t>
+  </si>
+  <si>
+    <t>OpponentHero3BornPos</t>
   </si>
 </sst>
 </file>
@@ -6222,10 +6240,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{972B7153-9DF5-4ED6-8C38-DB6612A94CE8}">
-  <dimension ref="A1:AM10"/>
+  <dimension ref="A1:AS10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" topLeftCell="AI1" workbookViewId="0">
+      <selection activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -6234,23 +6252,26 @@
     <col min="2" max="4" width="18.33203125" customWidth="1"/>
     <col min="5" max="7" width="16" customWidth="1"/>
     <col min="8" max="9" width="21.59765625" customWidth="1"/>
-    <col min="10" max="20" width="17.33203125" customWidth="1"/>
-    <col min="21" max="22" width="18.33203125" customWidth="1"/>
-    <col min="23" max="25" width="17.33203125" customWidth="1"/>
-    <col min="26" max="26" width="15.6640625" customWidth="1"/>
-    <col min="27" max="27" width="19.6640625" customWidth="1"/>
-    <col min="28" max="29" width="16" customWidth="1"/>
-    <col min="30" max="30" width="21.59765625" customWidth="1"/>
-    <col min="31" max="33" width="18.33203125" customWidth="1"/>
-    <col min="34" max="34" width="26.3984375" customWidth="1"/>
-    <col min="35" max="35" width="26.6640625" customWidth="1"/>
-    <col min="36" max="36" width="17.33203125" customWidth="1"/>
+    <col min="10" max="23" width="17.33203125" customWidth="1"/>
+    <col min="24" max="25" width="18.33203125" customWidth="1"/>
+    <col min="26" max="28" width="17.33203125" customWidth="1"/>
+    <col min="29" max="29" width="15.6640625" customWidth="1"/>
+    <col min="30" max="30" width="19.6640625" customWidth="1"/>
+    <col min="31" max="32" width="16" customWidth="1"/>
+    <col min="33" max="33" width="21.59765625" customWidth="1"/>
+    <col min="34" max="36" width="18.33203125" customWidth="1"/>
     <col min="37" max="37" width="26.3984375" customWidth="1"/>
     <col min="38" max="38" width="26.6640625" customWidth="1"/>
-    <col min="39" max="39" width="17.33203125" customWidth="1"/>
+    <col min="39" max="39" width="23.33203125" customWidth="1"/>
+    <col min="40" max="40" width="26.3984375" customWidth="1"/>
+    <col min="41" max="41" width="26.6640625" customWidth="1"/>
+    <col min="42" max="42" width="17.33203125" customWidth="1"/>
+    <col min="43" max="43" width="26.3984375" customWidth="1"/>
+    <col min="44" max="44" width="26.6640625" customWidth="1"/>
+    <col min="45" max="45" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:39" s="25" customFormat="1">
+    <row r="1" spans="1:45" s="25" customFormat="1">
       <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
@@ -6285,91 +6306,109 @@
         <v>209</v>
       </c>
       <c r="L1" s="28" t="s">
+        <v>353</v>
+      </c>
+      <c r="M1" s="28" t="s">
+        <v>355</v>
+      </c>
+      <c r="N1" s="28" t="s">
+        <v>354</v>
+      </c>
+      <c r="O1" s="28" t="s">
         <v>336</v>
       </c>
-      <c r="M1" s="28" t="s">
+      <c r="P1" s="28" t="s">
         <v>337</v>
       </c>
-      <c r="N1" s="28" t="s">
+      <c r="Q1" s="28" t="s">
         <v>338</v>
       </c>
-      <c r="O1" s="28" t="s">
+      <c r="R1" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="P1" s="28" t="s">
+      <c r="S1" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="Q1" s="28" t="s">
+      <c r="T1" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="R1" s="28" t="s">
+      <c r="U1" s="28" t="s">
         <v>220</v>
       </c>
-      <c r="S1" s="28" t="s">
+      <c r="V1" s="28" t="s">
         <v>219</v>
       </c>
-      <c r="T1" s="28" t="s">
+      <c r="W1" s="28" t="s">
         <v>218</v>
       </c>
-      <c r="U1" s="28" t="s">
+      <c r="X1" s="28" t="s">
         <v>239</v>
       </c>
-      <c r="V1" s="28" t="s">
+      <c r="Y1" s="28" t="s">
         <v>241</v>
       </c>
-      <c r="W1" s="28" t="s">
+      <c r="Z1" s="28" t="s">
         <v>234</v>
       </c>
-      <c r="X1" s="28" t="s">
+      <c r="AA1" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="Y1" s="28" t="s">
+      <c r="AB1" s="28" t="s">
         <v>238</v>
       </c>
-      <c r="Z1" s="25" t="s">
+      <c r="AC1" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="AA1" s="25" t="s">
+      <c r="AD1" s="25" t="s">
         <v>240</v>
       </c>
-      <c r="AB1" s="25" t="s">
+      <c r="AE1" s="25" t="s">
         <v>230</v>
       </c>
-      <c r="AC1" s="25" t="s">
+      <c r="AF1" s="25" t="s">
         <v>225</v>
       </c>
-      <c r="AD1" s="25" t="s">
+      <c r="AG1" s="25" t="s">
         <v>224</v>
       </c>
-      <c r="AE1" s="28" t="s">
+      <c r="AH1" s="28" t="s">
         <v>215</v>
       </c>
-      <c r="AF1" s="28" t="s">
+      <c r="AI1" s="28" t="s">
         <v>216</v>
       </c>
-      <c r="AG1" s="28" t="s">
+      <c r="AJ1" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="AH1" s="28" t="s">
+      <c r="AK1" s="28" t="s">
+        <v>356</v>
+      </c>
+      <c r="AL1" s="28" t="s">
+        <v>357</v>
+      </c>
+      <c r="AM1" s="28" t="s">
+        <v>358</v>
+      </c>
+      <c r="AN1" s="28" t="s">
         <v>342</v>
       </c>
-      <c r="AI1" s="28" t="s">
+      <c r="AO1" s="28" t="s">
         <v>341</v>
       </c>
-      <c r="AJ1" s="28" t="s">
+      <c r="AP1" s="28" t="s">
         <v>340</v>
       </c>
-      <c r="AK1" s="28" t="s">
+      <c r="AQ1" s="28" t="s">
         <v>344</v>
       </c>
-      <c r="AL1" s="28" t="s">
+      <c r="AR1" s="28" t="s">
         <v>343</v>
       </c>
-      <c r="AM1" s="28" t="s">
+      <c r="AS1" s="28" t="s">
         <v>345</v>
       </c>
     </row>
-    <row r="2" spans="1:39" s="26" customFormat="1">
+    <row r="2" spans="1:45" s="26" customFormat="1">
       <c r="A2" s="29" t="s">
         <v>34</v>
       </c>
@@ -6404,73 +6443,73 @@
         <v>35</v>
       </c>
       <c r="L2" s="39" t="s">
+        <v>204</v>
+      </c>
+      <c r="M2" s="39" t="s">
+        <v>204</v>
+      </c>
+      <c r="N2" s="39" t="s">
+        <v>204</v>
+      </c>
+      <c r="O2" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="39" t="s">
+      <c r="P2" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="39" t="s">
+      <c r="Q2" s="39" t="s">
         <v>37</v>
       </c>
-      <c r="O2" s="39" t="s">
+      <c r="R2" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="P2" s="39" t="s">
+      <c r="S2" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="Q2" s="39" t="s">
+      <c r="T2" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="R2" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="S2" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="T2" s="39" t="s">
-        <v>36</v>
-      </c>
-      <c r="U2" s="30" t="s">
+      <c r="U2" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="V2" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="W2" s="39" t="s">
+        <v>36</v>
+      </c>
+      <c r="X2" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="V2" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="W2" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="X2" s="30" t="s">
-        <v>36</v>
-      </c>
       <c r="Y2" s="30" t="s">
         <v>36</v>
       </c>
       <c r="Z2" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AA2" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AB2" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AC2" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="AA2" s="30" t="s">
+      <c r="AD2" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="AB2" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="AC2" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="AD2" s="30" t="s">
-        <v>36</v>
-      </c>
       <c r="AE2" s="30" t="s">
         <v>36</v>
       </c>
       <c r="AF2" s="30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AG2" s="30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AH2" s="30" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AI2" s="30" t="s">
         <v>35</v>
@@ -6479,16 +6518,34 @@
         <v>35</v>
       </c>
       <c r="AK2" s="30" t="s">
-        <v>36</v>
+        <v>204</v>
       </c>
       <c r="AL2" s="30" t="s">
-        <v>36</v>
+        <v>204</v>
       </c>
       <c r="AM2" s="30" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:39" s="26" customFormat="1">
+        <v>204</v>
+      </c>
+      <c r="AN2" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="AO2" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="AP2" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="AQ2" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AR2" s="30" t="s">
+        <v>36</v>
+      </c>
+      <c r="AS2" s="30" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:45" s="26" customFormat="1">
       <c r="A3" s="29" t="s">
         <v>38</v>
       </c>
@@ -6549,19 +6606,19 @@
       <c r="T3" s="39">
         <v>0</v>
       </c>
-      <c r="U3" s="31">
-        <v>0</v>
-      </c>
-      <c r="V3" s="31">
-        <v>0</v>
-      </c>
-      <c r="W3" s="30">
-        <v>0</v>
-      </c>
-      <c r="X3" s="30">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="30">
+      <c r="U3" s="39">
+        <v>0</v>
+      </c>
+      <c r="V3" s="39">
+        <v>0</v>
+      </c>
+      <c r="W3" s="39">
+        <v>0</v>
+      </c>
+      <c r="X3" s="31">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="31">
         <v>0</v>
       </c>
       <c r="Z3" s="30">
@@ -6579,22 +6636,22 @@
       <c r="AD3" s="30">
         <v>0</v>
       </c>
-      <c r="AE3" s="31">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="31">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="31">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="30">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="30">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="30">
+      <c r="AE3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="31">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="31">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="31">
         <v>0</v>
       </c>
       <c r="AK3" s="30">
@@ -6606,8 +6663,26 @@
       <c r="AM3" s="30">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:39" s="26" customFormat="1">
+      <c r="AN3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="30">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:45" s="26" customFormat="1">
       <c r="A4" s="29" t="s">
         <v>39</v>
       </c>
@@ -6668,13 +6743,13 @@
       <c r="T4" s="39">
         <v>1</v>
       </c>
-      <c r="U4" s="30">
-        <v>1</v>
-      </c>
-      <c r="V4" s="30">
-        <v>1</v>
-      </c>
-      <c r="W4" s="30">
+      <c r="U4" s="39">
+        <v>1</v>
+      </c>
+      <c r="V4" s="39">
+        <v>1</v>
+      </c>
+      <c r="W4" s="39">
         <v>1</v>
       </c>
       <c r="X4" s="30">
@@ -6725,8 +6800,26 @@
       <c r="AM4" s="30">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:39" s="26" customFormat="1">
+      <c r="AN4" s="30">
+        <v>1</v>
+      </c>
+      <c r="AO4" s="30">
+        <v>1</v>
+      </c>
+      <c r="AP4" s="30">
+        <v>1</v>
+      </c>
+      <c r="AQ4" s="30">
+        <v>1</v>
+      </c>
+      <c r="AR4" s="30">
+        <v>1</v>
+      </c>
+      <c r="AS4" s="30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:45" s="26" customFormat="1">
       <c r="A5" s="29" t="s">
         <v>40</v>
       </c>
@@ -6787,13 +6880,13 @@
       <c r="T5" s="40">
         <v>0</v>
       </c>
-      <c r="U5" s="31">
-        <v>0</v>
-      </c>
-      <c r="V5" s="31">
-        <v>0</v>
-      </c>
-      <c r="W5" s="31">
+      <c r="U5" s="40">
+        <v>0</v>
+      </c>
+      <c r="V5" s="40">
+        <v>0</v>
+      </c>
+      <c r="W5" s="40">
         <v>0</v>
       </c>
       <c r="X5" s="31">
@@ -6844,8 +6937,26 @@
       <c r="AM5" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:39" s="26" customFormat="1">
+      <c r="AN5" s="31">
+        <v>0</v>
+      </c>
+      <c r="AO5" s="31">
+        <v>0</v>
+      </c>
+      <c r="AP5" s="31">
+        <v>0</v>
+      </c>
+      <c r="AQ5" s="31">
+        <v>0</v>
+      </c>
+      <c r="AR5" s="31">
+        <v>0</v>
+      </c>
+      <c r="AS5" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:45" s="26" customFormat="1">
       <c r="A6" s="29" t="s">
         <v>41</v>
       </c>
@@ -6906,19 +7017,19 @@
       <c r="T6" s="40">
         <v>1</v>
       </c>
-      <c r="U6" s="30">
-        <v>1</v>
-      </c>
-      <c r="V6" s="30">
-        <v>1</v>
-      </c>
-      <c r="W6" s="31">
-        <v>1</v>
-      </c>
-      <c r="X6" s="31">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="31">
+      <c r="U6" s="40">
+        <v>1</v>
+      </c>
+      <c r="V6" s="40">
+        <v>1</v>
+      </c>
+      <c r="W6" s="40">
+        <v>1</v>
+      </c>
+      <c r="X6" s="30">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="30">
         <v>1</v>
       </c>
       <c r="Z6" s="31">
@@ -6936,22 +7047,22 @@
       <c r="AD6" s="31">
         <v>1</v>
       </c>
-      <c r="AE6" s="30">
-        <v>1</v>
-      </c>
-      <c r="AF6" s="30">
-        <v>1</v>
-      </c>
-      <c r="AG6" s="30">
-        <v>1</v>
-      </c>
-      <c r="AH6" s="31">
-        <v>1</v>
-      </c>
-      <c r="AI6" s="31">
-        <v>1</v>
-      </c>
-      <c r="AJ6" s="31">
+      <c r="AE6" s="31">
+        <v>1</v>
+      </c>
+      <c r="AF6" s="31">
+        <v>1</v>
+      </c>
+      <c r="AG6" s="31">
+        <v>1</v>
+      </c>
+      <c r="AH6" s="30">
+        <v>1</v>
+      </c>
+      <c r="AI6" s="30">
+        <v>1</v>
+      </c>
+      <c r="AJ6" s="30">
         <v>1</v>
       </c>
       <c r="AK6" s="31">
@@ -6963,8 +7074,26 @@
       <c r="AM6" s="31">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:39" s="16" customFormat="1">
+      <c r="AN6" s="31">
+        <v>1</v>
+      </c>
+      <c r="AO6" s="31">
+        <v>1</v>
+      </c>
+      <c r="AP6" s="31">
+        <v>1</v>
+      </c>
+      <c r="AQ6" s="31">
+        <v>1</v>
+      </c>
+      <c r="AR6" s="31">
+        <v>1</v>
+      </c>
+      <c r="AS6" s="31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:45" s="16" customFormat="1">
       <c r="A7" s="22" t="s">
         <v>42</v>
       </c>
@@ -7025,13 +7154,13 @@
       <c r="T7" s="40">
         <v>0</v>
       </c>
-      <c r="U7" s="31">
-        <v>0</v>
-      </c>
-      <c r="V7" s="31">
-        <v>0</v>
-      </c>
-      <c r="W7" s="31">
+      <c r="U7" s="40">
+        <v>0</v>
+      </c>
+      <c r="V7" s="40">
+        <v>0</v>
+      </c>
+      <c r="W7" s="40">
         <v>0</v>
       </c>
       <c r="X7" s="31">
@@ -7082,8 +7211,26 @@
       <c r="AM7" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:39" s="16" customFormat="1">
+      <c r="AN7" s="31">
+        <v>0</v>
+      </c>
+      <c r="AO7" s="31">
+        <v>0</v>
+      </c>
+      <c r="AP7" s="31">
+        <v>0</v>
+      </c>
+      <c r="AQ7" s="31">
+        <v>0</v>
+      </c>
+      <c r="AR7" s="31">
+        <v>0</v>
+      </c>
+      <c r="AS7" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:45" s="16" customFormat="1">
       <c r="A8" s="22" t="s">
         <v>206</v>
       </c>
@@ -7144,13 +7291,13 @@
       <c r="T8" s="40">
         <v>0</v>
       </c>
-      <c r="U8" s="31">
-        <v>0</v>
-      </c>
-      <c r="V8" s="31">
-        <v>0</v>
-      </c>
-      <c r="W8" s="31">
+      <c r="U8" s="40">
+        <v>0</v>
+      </c>
+      <c r="V8" s="40">
+        <v>0</v>
+      </c>
+      <c r="W8" s="40">
         <v>0</v>
       </c>
       <c r="X8" s="31">
@@ -7201,8 +7348,26 @@
       <c r="AM8" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:39" s="16" customFormat="1">
+      <c r="AN8" s="31">
+        <v>0</v>
+      </c>
+      <c r="AO8" s="31">
+        <v>0</v>
+      </c>
+      <c r="AP8" s="31">
+        <v>0</v>
+      </c>
+      <c r="AQ8" s="31">
+        <v>0</v>
+      </c>
+      <c r="AR8" s="31">
+        <v>0</v>
+      </c>
+      <c r="AS8" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:45" s="16" customFormat="1">
       <c r="A9" s="22" t="s">
         <v>43</v>
       </c>
@@ -7263,13 +7428,13 @@
       <c r="T9" s="40">
         <v>0</v>
       </c>
-      <c r="U9" s="31">
-        <v>0</v>
-      </c>
-      <c r="V9" s="31">
-        <v>0</v>
-      </c>
-      <c r="W9" s="31">
+      <c r="U9" s="40">
+        <v>0</v>
+      </c>
+      <c r="V9" s="40">
+        <v>0</v>
+      </c>
+      <c r="W9" s="40">
         <v>0</v>
       </c>
       <c r="X9" s="31">
@@ -7320,8 +7485,26 @@
       <c r="AM9" s="31">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:39" s="17" customFormat="1" ht="27.4" thickBot="1">
+      <c r="AN9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AP9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AQ9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AR9" s="31">
+        <v>0</v>
+      </c>
+      <c r="AS9" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:45" s="17" customFormat="1" ht="27.4" thickBot="1">
       <c r="A10" s="23" t="s">
         <v>44</v>
       </c>
@@ -7370,47 +7553,47 @@
       <c r="T10" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="U10" s="32" t="s">
+      <c r="U10" s="41" t="s">
+        <v>198</v>
+      </c>
+      <c r="V10" s="41" t="s">
+        <v>199</v>
+      </c>
+      <c r="W10" s="41" t="s">
+        <v>200</v>
+      </c>
+      <c r="X10" s="32" t="s">
         <v>214</v>
       </c>
-      <c r="V10" s="32" t="s">
+      <c r="Y10" s="32" t="s">
         <v>214</v>
       </c>
-      <c r="W10" s="32" t="s">
+      <c r="Z10" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="X10" s="32" t="s">
+      <c r="AA10" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="Y10" s="32" t="s">
+      <c r="AB10" s="32" t="s">
         <v>198</v>
       </c>
-      <c r="Z10" s="32" t="s">
+      <c r="AC10" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="AA10" s="32" t="s">
+      <c r="AD10" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="AB10" s="33"/>
-      <c r="AC10" s="33"/>
-      <c r="AD10" s="33"/>
-      <c r="AE10" s="32" t="s">
+      <c r="AE10" s="33"/>
+      <c r="AF10" s="33"/>
+      <c r="AG10" s="33"/>
+      <c r="AH10" s="32" t="s">
         <v>214</v>
       </c>
-      <c r="AF10" s="32" t="s">
+      <c r="AI10" s="32" t="s">
         <v>214</v>
       </c>
-      <c r="AG10" s="32" t="s">
+      <c r="AJ10" s="32" t="s">
         <v>214</v>
-      </c>
-      <c r="AH10" s="32" t="s">
-        <v>198</v>
-      </c>
-      <c r="AI10" s="32" t="s">
-        <v>199</v>
-      </c>
-      <c r="AJ10" s="32" t="s">
-        <v>200</v>
       </c>
       <c r="AK10" s="32" t="s">
         <v>198</v>
@@ -7419,13 +7602,31 @@
         <v>199</v>
       </c>
       <c r="AM10" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="AN10" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="AO10" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="AP10" s="32" t="s">
+        <v>200</v>
+      </c>
+      <c r="AQ10" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="AR10" s="32" t="s">
+        <v>199</v>
+      </c>
+      <c r="AS10" s="32" t="s">
         <v>200</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9" xr:uid="{C5B45FAA-DDA2-4923-883B-BDBA94013D24}"/>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:I9 AE5:AM5 AH6:AM9 L5:AD9 J6:K9 B5:C5" xr:uid="{9492378F-A71A-4DF6-9127-6F1B0B990504}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D7:I9 J6:K9 AK6:AS9 L5:AG9 B5:C5 AH5:AS5" xr:uid="{9492378F-A71A-4DF6-9127-6F1B0B990504}">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
   </dataValidations>
@@ -9007,7 +9208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:W52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fixed bug for property's type
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Player.xlsx
+++ b/_Out/NFDataCfg/Excel/Player.xlsx
@@ -506,7 +506,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352">
   <si>
     <t>Id</t>
   </si>
@@ -1090,7 +1090,7 @@
     <t>HeroPos3</t>
   </si>
   <si>
-    <t>vector</t>
+    <t>vector3</t>
   </si>
   <si>
     <t>Hero1</t>
@@ -1397,9 +1397,6 @@
     <t>Postion</t>
   </si>
   <si>
-    <t>vector3</t>
-  </si>
-  <si>
     <t>TaskMonsterList</t>
   </si>
   <si>
@@ -1610,10 +1607,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -1645,11 +1642,31 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1669,37 +1686,8 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1714,8 +1702,70 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1724,29 +1774,6 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1761,36 +1788,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1847,13 +1844,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1871,7 +1892,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1883,7 +1916,61 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1895,7 +1982,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1907,127 +2018,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2181,17 +2178,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2213,18 +2204,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2246,11 +2245,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2259,148 +2256,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="19" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2978,7 +2975,7 @@
   <sheetPr/>
   <dimension ref="A1:AS10"/>
   <sheetViews>
-    <sheetView topLeftCell="AG1" workbookViewId="0">
+    <sheetView topLeftCell="AM1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
       <selection pane="bottomLeft" activeCell="H1" sqref="H$1:H$1048576"/>
@@ -4417,7 +4414,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="1" spans="1:2">
@@ -4494,19 +4491,19 @@
     </row>
     <row r="11" s="3" customFormat="1" spans="1:5">
       <c r="A11" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="B11" s="4" t="s">
+      <c r="C11" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="C11" s="4" t="s">
+      <c r="D11" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="E11" s="4" t="s">
         <v>327</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="12" s="3" customFormat="1" spans="1:5">
@@ -4520,7 +4517,7 @@
         <v>47</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>290</v>
+        <v>194</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>47</v>
@@ -4540,7 +4537,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" spans="1:2">
@@ -4617,19 +4614,19 @@
     </row>
     <row r="24" s="3" customFormat="1" spans="1:5">
       <c r="A24" s="4" t="s">
+        <v>323</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>324</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="C24" s="4" t="s">
         <v>325</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="D24" s="4" t="s">
         <v>326</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>327</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>328</v>
       </c>
     </row>
     <row r="25" s="3" customFormat="1" spans="1:5">
@@ -4643,7 +4640,7 @@
         <v>47</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>290</v>
+        <v>194</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>47</v>
@@ -4700,7 +4697,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -4919,37 +4916,37 @@
         <v>3</v>
       </c>
       <c r="E11" s="8" t="s">
+        <v>330</v>
+      </c>
+      <c r="F11" s="8" t="s">
         <v>331</v>
       </c>
-      <c r="F11" s="8" t="s">
+      <c r="G11" s="8" t="s">
         <v>332</v>
       </c>
-      <c r="G11" s="8" t="s">
+      <c r="H11" s="8" t="s">
         <v>333</v>
       </c>
-      <c r="H11" s="8" t="s">
+      <c r="I11" s="8" t="s">
         <v>334</v>
       </c>
-      <c r="I11" s="8" t="s">
+      <c r="J11" s="8" t="s">
         <v>335</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>336</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>30</v>
       </c>
       <c r="L11" s="8" t="s">
+        <v>336</v>
+      </c>
+      <c r="M11" s="8" t="s">
         <v>337</v>
       </c>
-      <c r="M11" s="8" t="s">
+      <c r="N11" s="8" t="s">
         <v>338</v>
       </c>
-      <c r="N11" s="8" t="s">
+      <c r="O11" s="8" t="s">
         <v>339</v>
-      </c>
-      <c r="O11" s="8" t="s">
-        <v>340</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:15">
@@ -5004,7 +5001,7 @@
         <v>56</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -5025,7 +5022,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -5241,7 +5238,7 @@
         <v>6</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -5285,7 +5282,7 @@
         <v>56</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -5306,7 +5303,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -5562,7 +5559,7 @@
         <v>56</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="7"/>
@@ -5583,7 +5580,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
@@ -5888,10 +5885,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>344</v>
+      </c>
+      <c r="C1" t="s">
         <v>345</v>
-      </c>
-      <c r="C1" t="s">
-        <v>346</v>
       </c>
       <c r="D1" t="s">
         <v>56</v>
@@ -5899,16 +5896,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="B2" s="5" t="s">
         <v>347</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="C2">
+        <v>1</v>
+      </c>
+      <c r="D2" s="5" t="s">
         <v>348</v>
-      </c>
-      <c r="C2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>349</v>
       </c>
     </row>
   </sheetData>
@@ -5942,7 +5939,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="2" spans="1:2">
@@ -6019,10 +6016,10 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="4" t="s">
+        <v>350</v>
+      </c>
+      <c r="B11" s="4" t="s">
         <v>351</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>352</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -7126,7 +7123,7 @@
   <dimension ref="A1:AT10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="AR5" sqref="AR5"/>
+      <selection activeCell="AS13" sqref="AS13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -8553,7 +8550,7 @@
   <sheetPr/>
   <dimension ref="A1:V10"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U5" sqref="U5"/>
     </sheetView>
   </sheetViews>
@@ -11499,7 +11496,7 @@
         <v>47</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>290</v>
+        <v>194</v>
       </c>
     </row>
     <row r="52" s="24" customFormat="1" spans="1:23">
@@ -11578,7 +11575,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="2" s="11" customFormat="1" spans="1:2">
@@ -11647,7 +11644,7 @@
     </row>
     <row r="10" s="11" customFormat="1" spans="1:2">
       <c r="A10" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B10" s="14">
         <v>0</v>
@@ -11655,16 +11652,16 @@
     </row>
     <row r="11" s="11" customFormat="1" spans="1:4">
       <c r="A11" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>293</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="C11" s="19" t="s">
         <v>294</v>
       </c>
-      <c r="C11" s="19" t="s">
+      <c r="D11" s="19" t="s">
         <v>295</v>
-      </c>
-      <c r="D11" s="19" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="12" s="11" customFormat="1" spans="1:4">
@@ -11686,7 +11683,7 @@
         <v>56</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
@@ -11696,7 +11693,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="15" s="11" customFormat="1" spans="1:2">
@@ -11765,7 +11762,7 @@
     </row>
     <row r="23" s="11" customFormat="1" spans="1:2">
       <c r="A23" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B23" s="14">
         <v>0</v>
@@ -11773,13 +11770,13 @@
     </row>
     <row r="24" s="11" customFormat="1" spans="1:3">
       <c r="A24" s="19" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="B24" s="19" t="s">
+        <v>298</v>
+      </c>
+      <c r="C24" s="19" t="s">
         <v>299</v>
-      </c>
-      <c r="C24" s="19" t="s">
-        <v>300</v>
       </c>
     </row>
     <row r="25" s="11" customFormat="1" spans="1:3">
@@ -11798,7 +11795,7 @@
         <v>56</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C26" s="19"/>
     </row>
@@ -11857,7 +11854,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="2" s="11" customFormat="1" spans="1:2">
@@ -11926,7 +11923,7 @@
     </row>
     <row r="10" s="11" customFormat="1" ht="14.25" spans="1:2">
       <c r="A10" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B10" s="14">
         <v>0</v>
@@ -11937,40 +11934,40 @@
         <v>168</v>
       </c>
       <c r="B11" s="16" t="s">
+        <v>302</v>
+      </c>
+      <c r="C11" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="D11" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="E11" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="F11" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="G11" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="H11" s="16" t="s">
         <v>308</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="I11" s="16" t="s">
         <v>309</v>
       </c>
-      <c r="I11" s="16" t="s">
+      <c r="J11" s="16" t="s">
         <v>310</v>
       </c>
-      <c r="J11" s="16" t="s">
+      <c r="K11" s="16" t="s">
         <v>311</v>
       </c>
-      <c r="K11" s="16" t="s">
+      <c r="L11" s="16" t="s">
         <v>312</v>
       </c>
-      <c r="L11" s="16" t="s">
+      <c r="M11" s="16" t="s">
         <v>313</v>
-      </c>
-      <c r="M11" s="16" t="s">
-        <v>314</v>
       </c>
       <c r="N11" s="16" t="s">
         <v>16</v>
@@ -11979,19 +11976,19 @@
         <v>17</v>
       </c>
       <c r="P11" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="Q11" s="16" t="s">
         <v>315</v>
       </c>
-      <c r="Q11" s="16" t="s">
+      <c r="R11" s="16" t="s">
         <v>316</v>
       </c>
-      <c r="R11" s="16" t="s">
+      <c r="S11" s="16" t="s">
         <v>317</v>
       </c>
-      <c r="S11" s="16" t="s">
+      <c r="T11" s="16" t="s">
         <v>318</v>
-      </c>
-      <c r="T11" s="16" t="s">
-        <v>319</v>
       </c>
     </row>
     <row r="12" s="11" customFormat="1" ht="15" spans="1:20">
@@ -12123,7 +12120,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="15" s="11" customFormat="1" spans="1:2">
@@ -12192,7 +12189,7 @@
     </row>
     <row r="23" s="11" customFormat="1" ht="14.25" spans="1:2">
       <c r="A23" s="14" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B23" s="14">
         <v>0</v>
@@ -12200,10 +12197,10 @@
     </row>
     <row r="24" s="11" customFormat="1" ht="15" spans="1:3">
       <c r="A24" s="15" t="s">
+        <v>320</v>
+      </c>
+      <c r="B24" s="16" t="s">
         <v>321</v>
-      </c>
-      <c r="B24" s="16" t="s">
-        <v>322</v>
       </c>
       <c r="C24" s="3"/>
     </row>

</xml_diff>

<commit_message>
enter scene 1 when the player on line.
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Player.xlsx
+++ b/_Out/NFDataCfg/Excel/Player.xlsx
@@ -1608,8 +1608,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="24">
@@ -1643,9 +1643,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1657,24 +1657,9 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1694,6 +1679,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -1704,14 +1697,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1734,29 +1720,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -1765,7 +1728,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1780,6 +1743,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1788,6 +1773,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1844,19 +1844,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1868,13 +1856,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1886,25 +1868,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1916,19 +1892,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1940,79 +1934,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2025,6 +1953,78 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2154,17 +2154,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2187,6 +2187,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -2198,32 +2213,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2251,153 +2240,164 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="19" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -7123,7 +7123,7 @@
   <dimension ref="A1:AT10"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="AS13" sqref="AS13"/>
+      <selection activeCell="AQ6" sqref="AQ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -7864,19 +7864,19 @@
         <v>1</v>
       </c>
       <c r="E6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J6" s="40">
         <v>1</v>
@@ -7911,41 +7911,41 @@
       <c r="T6" s="40">
         <v>1</v>
       </c>
-      <c r="U6" s="44">
-        <v>1</v>
+      <c r="U6" s="45">
+        <v>0</v>
       </c>
       <c r="V6" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="W6" s="45">
-        <v>1</v>
-      </c>
-      <c r="X6" s="44">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="X6" s="45">
+        <v>0</v>
       </c>
       <c r="Y6" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z6" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AB6" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AD6" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AE6" s="45">
         <v>1</v>
       </c>
-      <c r="AF6" s="44">
-        <v>1</v>
+      <c r="AF6" s="45">
+        <v>0</v>
       </c>
       <c r="AG6" s="44">
         <v>1</v>
@@ -7954,31 +7954,31 @@
         <v>1</v>
       </c>
       <c r="AI6" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ6" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK6" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL6" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AM6" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN6" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AO6" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AP6" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AQ6" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AR6" s="45">
         <v>1</v>
@@ -8534,7 +8534,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:C5 AF5:AH5 J5:AE9 D7:I9 AI5:AQ9 AR5:AT9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:C5 J5:AE5 AF5:AH5 AI5:AQ5 J6:T6 AE6 D7:I9 AR5:AT9 J7:AE9 AI7:AQ9">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>

</xml_diff>

<commit_message>
added name for creating a role
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Player.xlsx
+++ b/_Out/NFDataCfg/Excel/Player.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="17100" windowHeight="9915" activeTab="2"/>
+    <workbookView windowWidth="21495" windowHeight="10335" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -1015,10 +1015,7 @@
     <t>WarID</t>
   </si>
   <si>
-    <t>ViewOpponent</t>
-  </si>
-  <si>
-    <t>FightingOpponent</t>
+    <t>OpponentFighting</t>
   </si>
   <si>
     <t>WarEventTime</t>
@@ -1036,6 +1033,9 @@
     <t>FightHeroLevel</t>
   </si>
   <si>
+    <t>OpponentID</t>
+  </si>
+  <si>
     <t>OpponentLevel</t>
   </si>
   <si>
@@ -1102,10 +1102,10 @@
     <t>Hero3</t>
   </si>
   <si>
+    <t>pvp_oppnent</t>
+  </si>
+  <si>
     <t>when searching</t>
-  </si>
-  <si>
-    <t>pvp_oppnent</t>
   </si>
   <si>
     <t>Guild_Name</t>
@@ -1643,7 +1643,29 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1673,9 +1695,47 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1697,23 +1757,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1728,44 +1772,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1781,13 +1788,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1844,7 +1844,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1856,43 +1892,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1904,43 +1904,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1958,7 +1952,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1970,19 +2000,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1994,31 +2012,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2178,15 +2178,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -2197,6 +2188,30 @@
         <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -2213,21 +2228,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2256,148 +2256,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -7122,8 +7122,8 @@
   <sheetPr/>
   <dimension ref="A1:AT10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="AQ6" sqref="AQ6"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="V2" sqref="V2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -7132,7 +7132,9 @@
     <col min="2" max="4" width="18.375" customWidth="1"/>
     <col min="5" max="7" width="16" customWidth="1"/>
     <col min="8" max="9" width="21.625" customWidth="1"/>
-    <col min="10" max="32" width="17.375" customWidth="1"/>
+    <col min="10" max="21" width="17.375" customWidth="1"/>
+    <col min="22" max="22" width="25.125" customWidth="1"/>
+    <col min="23" max="32" width="17.375" customWidth="1"/>
     <col min="33" max="34" width="18.375" customWidth="1"/>
     <col min="35" max="37" width="17.375" customWidth="1"/>
     <col min="38" max="38" width="15.625" customWidth="1"/>
@@ -7217,7 +7219,7 @@
       <c r="V1" s="33" t="s">
         <v>169</v>
       </c>
-      <c r="W1" s="33" t="s">
+      <c r="W1" s="37" t="s">
         <v>170</v>
       </c>
       <c r="X1" s="37" t="s">
@@ -7229,7 +7231,7 @@
       <c r="Z1" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="AA1" s="37" t="s">
+      <c r="AA1" s="33" t="s">
         <v>174</v>
       </c>
       <c r="AB1" s="33" t="s">
@@ -7358,22 +7360,22 @@
         <v>48</v>
       </c>
       <c r="W2" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="X2" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y2" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z2" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA2" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB2" s="44" t="s">
         <v>48</v>
-      </c>
-      <c r="X2" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y2" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z2" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA2" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB2" s="44" t="s">
-        <v>47</v>
       </c>
       <c r="AC2" s="44" t="s">
         <v>47</v>
@@ -7497,10 +7499,10 @@
       <c r="V3" s="44">
         <v>0</v>
       </c>
-      <c r="W3" s="44">
-        <v>0</v>
-      </c>
-      <c r="X3" s="45">
+      <c r="W3" s="45">
+        <v>0</v>
+      </c>
+      <c r="X3" s="44">
         <v>0</v>
       </c>
       <c r="Y3" s="44">
@@ -7942,16 +7944,16 @@
         <v>0</v>
       </c>
       <c r="AE6" s="45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AF6" s="45">
         <v>0</v>
       </c>
-      <c r="AG6" s="44">
-        <v>1</v>
-      </c>
-      <c r="AH6" s="44">
-        <v>1</v>
+      <c r="AG6" s="45">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="45">
+        <v>0</v>
       </c>
       <c r="AI6" s="45">
         <v>0</v>
@@ -8466,10 +8468,10 @@
         <v>198</v>
       </c>
       <c r="W10" s="46" t="s">
-        <v>199</v>
+        <v>149</v>
       </c>
       <c r="X10" s="46" t="s">
-        <v>149</v>
+        <v>195</v>
       </c>
       <c r="Y10" s="46" t="s">
         <v>195</v>
@@ -8477,11 +8479,11 @@
       <c r="Z10" s="46" t="s">
         <v>195</v>
       </c>
-      <c r="AA10" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="AB10" s="47" t="s">
-        <v>175</v>
+      <c r="AA10" s="47" t="s">
+        <v>174</v>
+      </c>
+      <c r="AB10" s="46" t="s">
+        <v>199</v>
       </c>
       <c r="AC10" s="47"/>
       <c r="AD10" s="47"/>
@@ -8534,7 +8536,7 @@
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:C5 J5:AE5 AF5:AH5 AI5:AQ5 J6:T6 AE6 D7:I9 AR5:AT9 J7:AE9 AI7:AQ9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:C5 J5:U5 V5:AA5 AB5 AC5:AE5 AF5:AH5 AI5:AQ5 J6:T6 AE6 AG6 AH6 AB7:AB9 D7:I9 V7:AA9 AR5:AT9 AI7:AQ9 AC7:AE9 J7:U9">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>

</xml_diff>

<commit_message>
added hp for heroes added tostring interface for datalist, property manager and record manager
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Player.xlsx
+++ b/_Out/NFDataCfg/Excel/Player.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="21495" windowHeight="10335" activeTab="2"/>
+    <workbookView windowWidth="21495" windowHeight="10335"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -277,6 +277,30 @@
         </r>
       </text>
     </comment>
+    <comment ref="N11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="SimSun"/>
+            <charset val="134"/>
+          </rPr>
+          <t>星级</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="O11" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <rFont val="SimSun"/>
+            <charset val="134"/>
+          </rPr>
+          <t>星级</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="D24" authorId="0">
       <text>
         <r>
@@ -506,7 +530,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347">
   <si>
     <t>Id</t>
   </si>
@@ -610,7 +634,7 @@
     <t>TeamID</t>
   </si>
   <si>
-    <t>HomeSceneID</t>
+    <t>HomeCellID</t>
   </si>
   <si>
     <t>Head</t>
@@ -958,9 +982,6 @@
     <t>Cup</t>
   </si>
   <si>
-    <t>PVPType</t>
-  </si>
-  <si>
     <t>FightingStar</t>
   </si>
   <si>
@@ -1072,27 +1093,6 @@
     <t>OpponentHeroStar3</t>
   </si>
   <si>
-    <t>FightHeroHP1</t>
-  </si>
-  <si>
-    <t>FightHeroHP2</t>
-  </si>
-  <si>
-    <t>FightHeroHP3</t>
-  </si>
-  <si>
-    <t>HeroPos1</t>
-  </si>
-  <si>
-    <t>HeroPos2</t>
-  </si>
-  <si>
-    <t>HeroPos3</t>
-  </si>
-  <si>
-    <t>vector3</t>
-  </si>
-  <si>
     <t>Hero1</t>
   </si>
   <si>
@@ -1100,6 +1100,9 @@
   </si>
   <si>
     <t>Hero3</t>
+  </si>
+  <si>
+    <t>主要是给离线玩家看</t>
   </si>
   <si>
     <t>pvp_oppnent</t>
@@ -1286,6 +1289,9 @@
     <t>Star</t>
   </si>
   <si>
+    <t>ReliveTime</t>
+  </si>
+  <si>
     <t>Ice_Talent</t>
   </si>
   <si>
@@ -1395,6 +1401,9 @@
   </si>
   <si>
     <t>Postion</t>
+  </si>
+  <si>
+    <t>vector3</t>
   </si>
   <si>
     <t>TaskMonsterList</t>
@@ -1607,9 +1616,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="24">
@@ -1656,8 +1665,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1687,14 +1697,6 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -1703,7 +1705,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1717,24 +1719,45 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1757,37 +1780,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1844,25 +1853,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1874,13 +1883,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1892,13 +1895,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1916,13 +1925,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1934,43 +1973,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1988,43 +2033,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2154,17 +2163,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color theme="4"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2173,17 +2178,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -2204,11 +2198,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2216,8 +2216,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2238,16 +2238,25 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2256,7 +2265,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2274,22 +2283,22 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="15" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="29" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="26" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2298,106 +2307,106 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="29" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="19" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="19" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -2975,10 +2984,10 @@
   <sheetPr/>
   <dimension ref="A1:AS10"/>
   <sheetViews>
-    <sheetView topLeftCell="AM1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H$1:H$1048576"/>
+      <selection pane="bottomLeft" activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -3242,7 +3251,7 @@
         <v>48</v>
       </c>
       <c r="AI2" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AJ2" s="3" t="s">
         <v>46</v>
@@ -3727,13 +3736,13 @@
         <v>1</v>
       </c>
       <c r="N6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P6" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q6" s="3">
         <v>1</v>
@@ -4414,12 +4423,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>322</v>
+        <v>317</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B2" s="3">
         <v>128</v>
@@ -4427,7 +4436,7 @@
     </row>
     <row r="3" s="3" customFormat="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B3" s="3">
         <v>5</v>
@@ -4483,7 +4492,7 @@
     </row>
     <row r="10" s="3" customFormat="1" spans="1:2">
       <c r="A10" s="3" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -4491,19 +4500,19 @@
     </row>
     <row r="11" s="3" customFormat="1" spans="1:5">
       <c r="A11" s="4" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="12" s="3" customFormat="1" spans="1:5">
@@ -4517,7 +4526,7 @@
         <v>47</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>194</v>
+        <v>284</v>
       </c>
       <c r="E12" s="4" t="s">
         <v>47</v>
@@ -4537,12 +4546,12 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>328</v>
+        <v>323</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B15" s="3">
         <v>128</v>
@@ -4550,7 +4559,7 @@
     </row>
     <row r="16" s="3" customFormat="1" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B16" s="3">
         <v>5</v>
@@ -4614,19 +4623,19 @@
     </row>
     <row r="24" s="3" customFormat="1" spans="1:5">
       <c r="A24" s="4" t="s">
-        <v>323</v>
+        <v>318</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>324</v>
+        <v>319</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>325</v>
+        <v>320</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>326</v>
+        <v>321</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>327</v>
+        <v>322</v>
       </c>
     </row>
     <row r="25" s="3" customFormat="1" spans="1:5">
@@ -4640,7 +4649,7 @@
         <v>47</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>194</v>
+        <v>284</v>
       </c>
       <c r="E25" s="4" t="s">
         <v>47</v>
@@ -4697,7 +4706,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>329</v>
+        <v>324</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -4715,7 +4724,7 @@
     </row>
     <row r="2" ht="15" spans="1:15">
       <c r="A2" s="7" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B2" s="7">
         <v>50</v>
@@ -4736,7 +4745,7 @@
     </row>
     <row r="3" ht="15" spans="1:15">
       <c r="A3" s="7" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B3" s="7">
         <v>15</v>
@@ -4904,7 +4913,7 @@
     </row>
     <row r="11" ht="15" spans="1:15">
       <c r="A11" s="8" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>1</v>
@@ -4916,37 +4925,37 @@
         <v>3</v>
       </c>
       <c r="E11" s="8" t="s">
+        <v>325</v>
+      </c>
+      <c r="F11" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>327</v>
+      </c>
+      <c r="H11" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="I11" s="8" t="s">
+        <v>329</v>
+      </c>
+      <c r="J11" s="8" t="s">
         <v>330</v>
-      </c>
-      <c r="F11" s="8" t="s">
-        <v>331</v>
-      </c>
-      <c r="G11" s="8" t="s">
-        <v>332</v>
-      </c>
-      <c r="H11" s="8" t="s">
-        <v>333</v>
-      </c>
-      <c r="I11" s="8" t="s">
-        <v>334</v>
-      </c>
-      <c r="J11" s="8" t="s">
-        <v>335</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>30</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>336</v>
+        <v>331</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>337</v>
+        <v>332</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>338</v>
+        <v>333</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>339</v>
+        <v>334</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:15">
@@ -5001,7 +5010,7 @@
         <v>56</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -5022,7 +5031,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>341</v>
+        <v>336</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -5040,7 +5049,7 @@
     </row>
     <row r="15" ht="15" spans="1:15">
       <c r="A15" s="7" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B15" s="7">
         <v>50</v>
@@ -5061,7 +5070,7 @@
     </row>
     <row r="16" ht="15" spans="1:15">
       <c r="A16" s="7" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B16" s="7">
         <v>4</v>
@@ -5229,7 +5238,7 @@
     </row>
     <row r="24" ht="15" spans="1:15">
       <c r="A24" s="8" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>1</v>
@@ -5238,7 +5247,7 @@
         <v>6</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -5282,7 +5291,7 @@
         <v>56</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -5303,7 +5312,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>342</v>
+        <v>337</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -5321,7 +5330,7 @@
     </row>
     <row r="28" ht="15" spans="1:15">
       <c r="A28" s="7" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B28" s="7">
         <v>50</v>
@@ -5342,7 +5351,7 @@
     </row>
     <row r="29" ht="15" spans="1:15">
       <c r="A29" s="7" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B29" s="7">
         <v>3</v>
@@ -5510,7 +5519,7 @@
     </row>
     <row r="37" ht="15" spans="1:15">
       <c r="A37" s="8" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>1</v>
@@ -5559,7 +5568,7 @@
         <v>56</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>340</v>
+        <v>335</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="7"/>
@@ -5580,7 +5589,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>343</v>
+        <v>338</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
@@ -5598,7 +5607,7 @@
     </row>
     <row r="41" ht="15" spans="1:15">
       <c r="A41" s="7" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B41" s="7">
         <v>50</v>
@@ -5619,7 +5628,7 @@
     </row>
     <row r="42" ht="15" spans="1:15">
       <c r="A42" s="7" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B42" s="7">
         <v>2</v>
@@ -5787,7 +5796,7 @@
     </row>
     <row r="50" ht="15" spans="1:15">
       <c r="A50" s="8" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>6</v>
@@ -5885,10 +5894,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>344</v>
+        <v>339</v>
       </c>
       <c r="C1" t="s">
-        <v>345</v>
+        <v>340</v>
       </c>
       <c r="D1" t="s">
         <v>56</v>
@@ -5896,16 +5905,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>346</v>
+        <v>341</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>347</v>
+        <v>342</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>348</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>
@@ -5939,12 +5948,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>349</v>
+        <v>344</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B2" s="3">
         <v>8</v>
@@ -5952,7 +5961,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -6016,10 +6025,10 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="4" t="s">
-        <v>350</v>
+        <v>345</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>351</v>
+        <v>346</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -6061,7 +6070,7 @@
   <sheetPr/>
   <dimension ref="A1:AF30"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
@@ -7120,46 +7129,46 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AT10"/>
+  <dimension ref="A1:AM10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="23.75" customWidth="1"/>
-    <col min="2" max="4" width="18.375" customWidth="1"/>
-    <col min="5" max="7" width="16" customWidth="1"/>
-    <col min="8" max="9" width="21.625" customWidth="1"/>
-    <col min="10" max="21" width="17.375" customWidth="1"/>
-    <col min="22" max="22" width="25.125" customWidth="1"/>
-    <col min="23" max="32" width="17.375" customWidth="1"/>
-    <col min="33" max="34" width="18.375" customWidth="1"/>
-    <col min="35" max="37" width="17.375" customWidth="1"/>
-    <col min="38" max="38" width="15.625" customWidth="1"/>
-    <col min="39" max="39" width="19.625" customWidth="1"/>
-    <col min="40" max="46" width="16" customWidth="1"/>
-    <col min="47" max="48" width="18.375" customWidth="1"/>
-    <col min="49" max="49" width="26.375" customWidth="1"/>
-    <col min="50" max="50" width="26.625" customWidth="1"/>
-    <col min="51" max="51" width="23.375" customWidth="1"/>
-    <col min="52" max="52" width="26.375" customWidth="1"/>
-    <col min="53" max="53" width="26.625" customWidth="1"/>
-    <col min="54" max="54" width="17.375" customWidth="1"/>
-    <col min="55" max="55" width="26.375" customWidth="1"/>
-    <col min="56" max="56" width="26.625" customWidth="1"/>
-    <col min="57" max="57" width="17.375" customWidth="1"/>
+    <col min="2" max="3" width="18.375" customWidth="1"/>
+    <col min="4" max="6" width="16" customWidth="1"/>
+    <col min="7" max="8" width="21.625" customWidth="1"/>
+    <col min="9" max="20" width="17.375" customWidth="1"/>
+    <col min="21" max="21" width="25.125" customWidth="1"/>
+    <col min="22" max="31" width="17.375" customWidth="1"/>
+    <col min="32" max="33" width="18.375" customWidth="1"/>
+    <col min="34" max="36" width="17.375" customWidth="1"/>
+    <col min="37" max="37" width="15.625" customWidth="1"/>
+    <col min="38" max="38" width="19.625" customWidth="1"/>
+    <col min="39" max="39" width="16" customWidth="1"/>
+    <col min="40" max="41" width="18.375" customWidth="1"/>
+    <col min="42" max="42" width="26.375" customWidth="1"/>
+    <col min="43" max="43" width="26.625" customWidth="1"/>
+    <col min="44" max="44" width="23.375" customWidth="1"/>
+    <col min="45" max="45" width="26.375" customWidth="1"/>
+    <col min="46" max="46" width="26.625" customWidth="1"/>
+    <col min="47" max="47" width="17.375" customWidth="1"/>
+    <col min="48" max="48" width="26.375" customWidth="1"/>
+    <col min="49" max="49" width="26.625" customWidth="1"/>
+    <col min="50" max="50" width="17.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="33" customFormat="1" spans="1:46">
+    <row r="1" s="33" customFormat="1" spans="1:39">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="37" t="s">
         <v>149</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="33" t="s">
         <v>150</v>
       </c>
       <c r="D1" s="33" t="s">
@@ -7177,7 +7186,7 @@
       <c r="H1" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="37" t="s">
         <v>156</v>
       </c>
       <c r="J1" s="37" t="s">
@@ -7213,10 +7222,10 @@
       <c r="T1" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="U1" s="37" t="s">
+      <c r="U1" s="33" t="s">
         <v>168</v>
       </c>
-      <c r="V1" s="33" t="s">
+      <c r="V1" s="37" t="s">
         <v>169</v>
       </c>
       <c r="W1" s="37" t="s">
@@ -7228,7 +7237,7 @@
       <c r="Y1" s="37" t="s">
         <v>172</v>
       </c>
-      <c r="Z1" s="37" t="s">
+      <c r="Z1" s="33" t="s">
         <v>173</v>
       </c>
       <c r="AA1" s="33" t="s">
@@ -7243,7 +7252,7 @@
       <c r="AD1" s="33" t="s">
         <v>177</v>
       </c>
-      <c r="AE1" s="33" t="s">
+      <c r="AE1" s="37" t="s">
         <v>178</v>
       </c>
       <c r="AF1" s="37" t="s">
@@ -7270,29 +7279,8 @@
       <c r="AM1" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="AN1" s="37" t="s">
-        <v>187</v>
-      </c>
-      <c r="AO1" s="37" t="s">
-        <v>188</v>
-      </c>
-      <c r="AP1" s="37" t="s">
-        <v>189</v>
-      </c>
-      <c r="AQ1" s="37" t="s">
-        <v>190</v>
-      </c>
-      <c r="AR1" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="AS1" s="37" t="s">
-        <v>192</v>
-      </c>
-      <c r="AT1" s="37" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" s="34" customFormat="1" spans="1:46">
+    </row>
+    <row r="2" s="34" customFormat="1" spans="1:39">
       <c r="A2" s="38" t="s">
         <v>45</v>
       </c>
@@ -7318,7 +7306,7 @@
         <v>47</v>
       </c>
       <c r="I2" s="39" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J2" s="39" t="s">
         <v>48</v>
@@ -7330,7 +7318,7 @@
         <v>48</v>
       </c>
       <c r="M2" s="39" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N2" s="39" t="s">
         <v>46</v>
@@ -7342,7 +7330,7 @@
         <v>46</v>
       </c>
       <c r="Q2" s="39" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R2" s="39" t="s">
         <v>47</v>
@@ -7350,32 +7338,32 @@
       <c r="S2" s="39" t="s">
         <v>47</v>
       </c>
-      <c r="T2" s="39" t="s">
-        <v>47</v>
+      <c r="T2" s="44" t="s">
+        <v>48</v>
       </c>
       <c r="U2" s="44" t="s">
         <v>48</v>
       </c>
       <c r="V2" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="W2" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="X2" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="Y2" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z2" s="44" t="s">
+        <v>47</v>
+      </c>
+      <c r="AA2" s="44" t="s">
         <v>48</v>
       </c>
-      <c r="W2" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="X2" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y2" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z2" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="AA2" s="44" t="s">
-        <v>47</v>
-      </c>
       <c r="AB2" s="44" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="AC2" s="44" t="s">
         <v>47</v>
@@ -7387,7 +7375,7 @@
         <v>47</v>
       </c>
       <c r="AF2" s="44" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="AG2" s="44" t="s">
         <v>46</v>
@@ -7402,7 +7390,7 @@
         <v>46</v>
       </c>
       <c r="AK2" s="44" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="AL2" s="44" t="s">
         <v>47</v>
@@ -7410,40 +7398,19 @@
       <c r="AM2" s="44" t="s">
         <v>47</v>
       </c>
-      <c r="AN2" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="AO2" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="AP2" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="AQ2" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="AR2" s="44" t="s">
-        <v>194</v>
-      </c>
-      <c r="AS2" s="44" t="s">
-        <v>194</v>
-      </c>
-      <c r="AT2" s="44" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="3" s="34" customFormat="1" spans="1:46">
+    </row>
+    <row r="3" s="34" customFormat="1" spans="1:39">
       <c r="A3" s="38" t="s">
         <v>49</v>
       </c>
       <c r="B3" s="40">
         <v>0</v>
       </c>
-      <c r="C3" s="40">
-        <v>0</v>
+      <c r="C3" s="39">
+        <v>1</v>
       </c>
       <c r="D3" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" s="39">
         <v>0</v>
@@ -7458,10 +7425,10 @@
         <v>0</v>
       </c>
       <c r="I3" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J3" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" s="39">
         <v>0</v>
@@ -7470,10 +7437,10 @@
         <v>0</v>
       </c>
       <c r="M3" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N3" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O3" s="39">
         <v>0</v>
@@ -7490,16 +7457,16 @@
       <c r="S3" s="39">
         <v>0</v>
       </c>
-      <c r="T3" s="39">
-        <v>0</v>
-      </c>
-      <c r="U3" s="45">
-        <v>0</v>
-      </c>
-      <c r="V3" s="44">
-        <v>0</v>
-      </c>
-      <c r="W3" s="45">
+      <c r="T3" s="45">
+        <v>0</v>
+      </c>
+      <c r="U3" s="44">
+        <v>0</v>
+      </c>
+      <c r="V3" s="45">
+        <v>0</v>
+      </c>
+      <c r="W3" s="44">
         <v>0</v>
       </c>
       <c r="X3" s="44">
@@ -7523,7 +7490,7 @@
       <c r="AD3" s="44">
         <v>0</v>
       </c>
-      <c r="AE3" s="44">
+      <c r="AE3" s="45">
         <v>0</v>
       </c>
       <c r="AF3" s="45">
@@ -7532,7 +7499,7 @@
       <c r="AG3" s="45">
         <v>0</v>
       </c>
-      <c r="AH3" s="45">
+      <c r="AH3" s="44">
         <v>0</v>
       </c>
       <c r="AI3" s="44">
@@ -7550,29 +7517,8 @@
       <c r="AM3" s="44">
         <v>0</v>
       </c>
-      <c r="AN3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AT3" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" s="34" customFormat="1" spans="1:46">
+    </row>
+    <row r="4" s="34" customFormat="1" spans="1:39">
       <c r="A4" s="38" t="s">
         <v>50</v>
       </c>
@@ -7630,7 +7576,7 @@
       <c r="S4" s="39">
         <v>1</v>
       </c>
-      <c r="T4" s="39">
+      <c r="T4" s="44">
         <v>1</v>
       </c>
       <c r="U4" s="44">
@@ -7690,36 +7636,15 @@
       <c r="AM4" s="44">
         <v>1</v>
       </c>
-      <c r="AN4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AO4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AP4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AQ4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AR4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AS4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AT4" s="44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" s="34" customFormat="1" spans="1:46">
+    </row>
+    <row r="5" s="34" customFormat="1" spans="1:39">
       <c r="A5" s="38" t="s">
         <v>51</v>
       </c>
       <c r="B5" s="40">
         <v>0</v>
       </c>
-      <c r="C5" s="40">
+      <c r="C5" s="39">
         <v>0</v>
       </c>
       <c r="D5" s="39">
@@ -7737,7 +7662,7 @@
       <c r="H5" s="39">
         <v>0</v>
       </c>
-      <c r="I5" s="39">
+      <c r="I5" s="40">
         <v>0</v>
       </c>
       <c r="J5" s="40">
@@ -7770,7 +7695,7 @@
       <c r="S5" s="40">
         <v>0</v>
       </c>
-      <c r="T5" s="40">
+      <c r="T5" s="45">
         <v>0</v>
       </c>
       <c r="U5" s="45">
@@ -7830,29 +7755,8 @@
       <c r="AM5" s="45">
         <v>0</v>
       </c>
-      <c r="AN5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AO5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AP5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AQ5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AR5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AS5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AT5" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" s="34" customFormat="1" spans="1:46">
+    </row>
+    <row r="6" s="34" customFormat="1" spans="1:39">
       <c r="A6" s="38" t="s">
         <v>52</v>
       </c>
@@ -7860,10 +7764,10 @@
         <v>1</v>
       </c>
       <c r="C6" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D6" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E6" s="39">
         <v>0</v>
@@ -7877,8 +7781,8 @@
       <c r="H6" s="39">
         <v>0</v>
       </c>
-      <c r="I6" s="39">
-        <v>0</v>
+      <c r="I6" s="40">
+        <v>1</v>
       </c>
       <c r="J6" s="40">
         <v>1</v>
@@ -7910,8 +7814,8 @@
       <c r="S6" s="40">
         <v>1</v>
       </c>
-      <c r="T6" s="40">
-        <v>1</v>
+      <c r="T6" s="45">
+        <v>0</v>
       </c>
       <c r="U6" s="45">
         <v>0</v>
@@ -7970,29 +7874,8 @@
       <c r="AM6" s="45">
         <v>0</v>
       </c>
-      <c r="AN6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AO6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AP6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AR6" s="45">
-        <v>1</v>
-      </c>
-      <c r="AS6" s="45">
-        <v>1</v>
-      </c>
-      <c r="AT6" s="45">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" s="27" customFormat="1" spans="1:46">
+    </row>
+    <row r="7" s="27" customFormat="1" spans="1:39">
       <c r="A7" s="31" t="s">
         <v>53</v>
       </c>
@@ -8050,7 +7933,7 @@
       <c r="S7" s="40">
         <v>0</v>
       </c>
-      <c r="T7" s="40">
+      <c r="T7" s="45">
         <v>0</v>
       </c>
       <c r="U7" s="45">
@@ -8110,29 +7993,8 @@
       <c r="AM7" s="45">
         <v>0</v>
       </c>
-      <c r="AN7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AO7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AP7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AQ7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AR7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AS7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AT7" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" s="27" customFormat="1" spans="1:46">
+    </row>
+    <row r="8" s="27" customFormat="1" spans="1:39">
       <c r="A8" s="31" t="s">
         <v>54</v>
       </c>
@@ -8190,7 +8052,7 @@
       <c r="S8" s="40">
         <v>0</v>
       </c>
-      <c r="T8" s="40">
+      <c r="T8" s="45">
         <v>0</v>
       </c>
       <c r="U8" s="45">
@@ -8250,29 +8112,8 @@
       <c r="AM8" s="45">
         <v>0</v>
       </c>
-      <c r="AN8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AO8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AP8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AQ8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AR8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AS8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AT8" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" s="27" customFormat="1" spans="1:46">
+    </row>
+    <row r="9" s="27" customFormat="1" spans="1:39">
       <c r="A9" s="31" t="s">
         <v>55</v>
       </c>
@@ -8330,7 +8171,7 @@
       <c r="S9" s="40">
         <v>0</v>
       </c>
-      <c r="T9" s="40">
+      <c r="T9" s="45">
         <v>0</v>
       </c>
       <c r="U9" s="45">
@@ -8390,104 +8231,83 @@
       <c r="AM9" s="45">
         <v>0</v>
       </c>
-      <c r="AN9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AO9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AP9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AR9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AS9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AT9" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" s="35" customFormat="1" ht="14.25" spans="1:46">
+    </row>
+    <row r="10" s="35" customFormat="1" ht="27.75" spans="1:39">
       <c r="A10" s="41" t="s">
         <v>56</v>
       </c>
       <c r="B10" s="42" t="s">
         <v>149</v>
       </c>
-      <c r="C10" s="42" t="s">
-        <v>149</v>
-      </c>
+      <c r="C10" s="43"/>
       <c r="D10" s="43"/>
       <c r="E10" s="43"/>
       <c r="F10" s="43"/>
       <c r="G10" s="43"/>
       <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
+      <c r="I10" s="42" t="s">
+        <v>156</v>
+      </c>
       <c r="J10" s="42" t="s">
-        <v>157</v>
+        <v>187</v>
       </c>
       <c r="K10" s="42" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="L10" s="42" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="M10" s="42" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="N10" s="42" t="s">
-        <v>161</v>
+        <v>190</v>
       </c>
       <c r="O10" s="42" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="P10" s="42" t="s">
-        <v>196</v>
+        <v>190</v>
       </c>
       <c r="Q10" s="42" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="R10" s="42" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="S10" s="42" t="s">
-        <v>196</v>
-      </c>
-      <c r="T10" s="42" t="s">
-        <v>197</v>
+        <v>190</v>
+      </c>
+      <c r="T10" s="46" t="s">
+        <v>149</v>
       </c>
       <c r="U10" s="46" t="s">
+        <v>191</v>
+      </c>
+      <c r="V10" s="46" t="s">
         <v>149</v>
       </c>
-      <c r="V10" s="46" t="s">
-        <v>198</v>
-      </c>
       <c r="W10" s="46" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="X10" s="46" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="Y10" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="Z10" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="AA10" s="47" t="s">
-        <v>174</v>
-      </c>
-      <c r="AB10" s="46" t="s">
-        <v>199</v>
-      </c>
+        <v>187</v>
+      </c>
+      <c r="Z10" s="47" t="s">
+        <v>173</v>
+      </c>
+      <c r="AA10" s="46" t="s">
+        <v>192</v>
+      </c>
+      <c r="AB10" s="47"/>
       <c r="AC10" s="47"/>
       <c r="AD10" s="47"/>
-      <c r="AE10" s="47"/>
+      <c r="AE10" s="46" t="s">
+        <v>149</v>
+      </c>
       <c r="AF10" s="46" t="s">
         <v>149</v>
       </c>
@@ -8495,48 +8315,27 @@
         <v>149</v>
       </c>
       <c r="AH10" s="46" t="s">
-        <v>149</v>
+        <v>187</v>
       </c>
       <c r="AI10" s="46" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="AJ10" s="46" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="AK10" s="46" t="s">
-        <v>197</v>
+        <v>187</v>
       </c>
       <c r="AL10" s="46" t="s">
-        <v>195</v>
+        <v>188</v>
       </c>
       <c r="AM10" s="46" t="s">
-        <v>196</v>
-      </c>
-      <c r="AN10" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="AO10" s="46" t="s">
-        <v>188</v>
-      </c>
-      <c r="AP10" s="46" t="s">
         <v>189</v>
-      </c>
-      <c r="AQ10" s="46" t="s">
-        <v>190</v>
-      </c>
-      <c r="AR10" s="46" t="s">
-        <v>188</v>
-      </c>
-      <c r="AS10" s="46" t="s">
-        <v>189</v>
-      </c>
-      <c r="AT10" s="46" t="s">
-        <v>190</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5:C5 J5:U5 V5:AA5 AB5 AC5:AE5 AF5:AH5 AI5:AQ5 J6:T6 AE6 AG6 AH6 AB7:AB9 D7:I9 V7:AA9 AR5:AT9 AI7:AQ9 AC7:AE9 J7:U9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5 I5:T5 U5:Z5 AA5 AB5:AD5 AE5:AG5 AH5:AM5 I6:S6 AD6 AF6 AG6 AA7:AA9 AH7:AM9 C7:H9 U7:Z9 AB7:AD9 I7:T9">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>
@@ -8584,67 +8383,67 @@
         <v>0</v>
       </c>
       <c r="B1" s="26" t="s">
+        <v>193</v>
+      </c>
+      <c r="C1" s="26" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>195</v>
+      </c>
+      <c r="E1" s="26" t="s">
+        <v>196</v>
+      </c>
+      <c r="F1" s="26" t="s">
+        <v>197</v>
+      </c>
+      <c r="G1" s="26" t="s">
+        <v>198</v>
+      </c>
+      <c r="H1" s="26" t="s">
+        <v>199</v>
+      </c>
+      <c r="I1" s="26" t="s">
         <v>200</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="J1" s="26" t="s">
         <v>201</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="K1" s="26" t="s">
         <v>202</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="L1" s="26" t="s">
         <v>203</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="M1" s="26" t="s">
         <v>204</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="N1" s="26" t="s">
         <v>205</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="O1" s="26" t="s">
         <v>206</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="P1" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="Q1" s="26" t="s">
         <v>208</v>
       </c>
-      <c r="K1" s="26" t="s">
+      <c r="R1" s="26" t="s">
         <v>209</v>
       </c>
-      <c r="L1" s="26" t="s">
+      <c r="S1" s="26" t="s">
         <v>210</v>
       </c>
-      <c r="M1" s="26" t="s">
+      <c r="T1" s="26" t="s">
         <v>211</v>
       </c>
-      <c r="N1" s="26" t="s">
+      <c r="U1" s="26" t="s">
         <v>212</v>
       </c>
-      <c r="O1" s="26" t="s">
+      <c r="V1" s="26" t="s">
         <v>213</v>
-      </c>
-      <c r="P1" s="26" t="s">
-        <v>214</v>
-      </c>
-      <c r="Q1" s="26" t="s">
-        <v>215</v>
-      </c>
-      <c r="R1" s="26" t="s">
-        <v>216</v>
-      </c>
-      <c r="S1" s="26" t="s">
-        <v>217</v>
-      </c>
-      <c r="T1" s="26" t="s">
-        <v>218</v>
-      </c>
-      <c r="U1" s="26" t="s">
-        <v>219</v>
-      </c>
-      <c r="V1" s="26" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="2" s="7" customFormat="1" ht="15" spans="1:22">
@@ -9196,67 +8995,67 @@
         <v>56</v>
       </c>
       <c r="B10" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="C10" s="28" t="s">
+        <v>215</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>216</v>
+      </c>
+      <c r="E10" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>218</v>
+      </c>
+      <c r="G10" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="H10" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="I10" s="28" t="s">
         <v>221</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="J10" s="28" t="s">
         <v>222</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="K10" s="28" t="s">
         <v>223</v>
       </c>
-      <c r="E10" s="28" t="s">
+      <c r="L10" s="28" t="s">
         <v>224</v>
       </c>
-      <c r="F10" s="28" t="s">
+      <c r="M10" s="28" t="s">
         <v>225</v>
       </c>
-      <c r="G10" s="28" t="s">
+      <c r="N10" s="28" t="s">
         <v>226</v>
       </c>
-      <c r="H10" s="28" t="s">
+      <c r="O10" s="28" t="s">
         <v>227</v>
       </c>
-      <c r="I10" s="28" t="s">
+      <c r="P10" s="28" t="s">
         <v>228</v>
       </c>
-      <c r="J10" s="28" t="s">
+      <c r="Q10" s="28" t="s">
         <v>229</v>
       </c>
-      <c r="K10" s="28" t="s">
+      <c r="R10" s="28" t="s">
         <v>230</v>
       </c>
-      <c r="L10" s="28" t="s">
+      <c r="S10" s="28" t="s">
         <v>231</v>
       </c>
-      <c r="M10" s="28" t="s">
+      <c r="T10" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="N10" s="28" t="s">
+      <c r="U10" s="28" t="s">
         <v>233</v>
       </c>
-      <c r="O10" s="28" t="s">
+      <c r="V10" s="28" t="s">
         <v>234</v>
-      </c>
-      <c r="P10" s="28" t="s">
-        <v>235</v>
-      </c>
-      <c r="Q10" s="28" t="s">
-        <v>236</v>
-      </c>
-      <c r="R10" s="28" t="s">
-        <v>237</v>
-      </c>
-      <c r="S10" s="28" t="s">
-        <v>238</v>
-      </c>
-      <c r="T10" s="28" t="s">
-        <v>239</v>
-      </c>
-      <c r="U10" s="28" t="s">
-        <v>240</v>
-      </c>
-      <c r="V10" s="28" t="s">
-        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -9317,12 +9116,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>242</v>
+        <v>235</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B2" s="3">
         <v>15</v>
@@ -9330,7 +9129,7 @@
     </row>
     <row r="3" s="3" customFormat="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B3" s="3">
         <v>31</v>
@@ -9386,7 +9185,7 @@
     </row>
     <row r="10" s="3" customFormat="1" spans="1:2">
       <c r="A10" s="3" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -9587,7 +9386,7 @@
         <v>56</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -9653,7 +9452,7 @@
   <dimension ref="A1:AE26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -9663,7 +9462,8 @@
     <col min="3" max="3" width="10.375" style="9" customWidth="1"/>
     <col min="4" max="4" width="10.5" style="9" customWidth="1"/>
     <col min="5" max="5" width="11.625" style="9" customWidth="1"/>
-    <col min="6" max="7" width="9" style="9"/>
+    <col min="6" max="6" width="9" style="9"/>
+    <col min="7" max="7" width="12.875" style="9" customWidth="1"/>
     <col min="8" max="8" width="14.125" style="9" customWidth="1"/>
     <col min="9" max="9" width="15.375" style="9" customWidth="1"/>
     <col min="10" max="10" width="14.125" style="9" customWidth="1"/>
@@ -9671,7 +9471,7 @@
     <col min="12" max="12" width="14.125" style="9" customWidth="1"/>
     <col min="13" max="13" width="12.875" style="9" customWidth="1"/>
     <col min="14" max="14" width="9.375" style="9" customWidth="1"/>
-    <col min="15" max="15" width="10.375" style="9" customWidth="1"/>
+    <col min="15" max="15" width="12.875" style="9" customWidth="1"/>
     <col min="16" max="16" width="9.375" style="9" customWidth="1"/>
     <col min="17" max="19" width="9" style="9"/>
     <col min="20" max="20" width="10.375" style="9" customWidth="1"/>
@@ -9692,12 +9492,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B2" s="3">
         <v>64</v>
@@ -9705,10 +9505,10 @@
     </row>
     <row r="3" s="3" customFormat="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B3" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" s="3" customFormat="1" spans="1:2">
@@ -9767,48 +9567,52 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" s="3" customFormat="1" spans="1:13">
+    <row r="11" s="3" customFormat="1" spans="1:15">
       <c r="A11" s="4" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>248</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>250</v>
+      </c>
+      <c r="M11" s="4" t="s">
         <v>251</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="N11" s="4" t="s">
         <v>252</v>
       </c>
-      <c r="G11" s="4" t="s">
-        <v>253</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>254</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="12" s="3" customFormat="1" spans="1:13">
+      <c r="O11" s="4"/>
+    </row>
+    <row r="12" s="3" customFormat="1" spans="1:15">
       <c r="A12" s="25" t="s">
         <v>48</v>
       </c>
@@ -9848,6 +9652,10 @@
       <c r="M12" s="4" t="s">
         <v>47</v>
       </c>
+      <c r="N12" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="O12" s="4"/>
     </row>
     <row r="13" s="3" customFormat="1" spans="1:22">
       <c r="A13" s="4" t="s">
@@ -9880,12 +9688,12 @@
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B15" s="3">
         <v>15</v>
@@ -9893,7 +9701,7 @@
     </row>
     <row r="16" s="3" customFormat="1" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B16" s="3">
         <v>31</v>
@@ -10150,7 +9958,7 @@
         <v>56</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -10187,7 +9995,7 @@
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A6 A19 C26 B6:B10 B19:B23 D8:G9 D26:G1048576 A4:B5 A17:B18 C14:G20 D21:G22">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="N11:X11 A25:C25 P25 V25 W25 I8:AK9 I21:AK22 D24:O25 Q24:U25 X24:AE25">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="P11:X11 A25:C25 P25 V25 W25 I8:AK9 I21:AK22 D24:O25 Q24:U25 X24:AE25">
       <formula1>"int,string,float,object"</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C8:C9 C21:C22 A15:B16 B27:C1048576 A2:B3">
@@ -10234,7 +10042,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -10260,7 +10068,7 @@
     </row>
     <row r="2" s="23" customFormat="1" spans="1:23">
       <c r="A2" s="3" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B2" s="3">
         <v>256</v>
@@ -10289,7 +10097,7 @@
     </row>
     <row r="3" s="23" customFormat="1" spans="1:23">
       <c r="A3" s="3" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B3" s="3">
         <v>23</v>
@@ -10479,73 +10287,73 @@
     </row>
     <row r="11" s="23" customFormat="1" spans="1:23">
       <c r="A11" s="4" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B11" s="4" t="s">
+        <v>256</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>242</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>257</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>258</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>259</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>260</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>261</v>
+      </c>
+      <c r="I11" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="C11" s="4" t="s">
-        <v>249</v>
-      </c>
-      <c r="D11" s="4" t="s">
+      <c r="J11" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="E11" s="4" t="s">
+      <c r="K11" s="4" t="s">
         <v>264</v>
       </c>
-      <c r="F11" s="4" t="s">
+      <c r="L11" s="4" t="s">
         <v>265</v>
       </c>
-      <c r="G11" s="4" t="s">
+      <c r="M11" s="4" t="s">
         <v>266</v>
       </c>
-      <c r="H11" s="4" t="s">
+      <c r="N11" s="4" t="s">
         <v>267</v>
       </c>
-      <c r="I11" s="4" t="s">
+      <c r="O11" s="4" t="s">
         <v>268</v>
       </c>
-      <c r="J11" s="4" t="s">
+      <c r="P11" s="4" t="s">
         <v>269</v>
       </c>
-      <c r="K11" s="4" t="s">
+      <c r="Q11" s="4" t="s">
         <v>270</v>
       </c>
-      <c r="L11" s="4" t="s">
+      <c r="R11" s="4" t="s">
         <v>271</v>
       </c>
-      <c r="M11" s="4" t="s">
+      <c r="S11" s="4" t="s">
         <v>272</v>
       </c>
-      <c r="N11" s="4" t="s">
+      <c r="T11" s="4" t="s">
         <v>273</v>
       </c>
-      <c r="O11" s="4" t="s">
+      <c r="U11" s="4" t="s">
         <v>274</v>
       </c>
-      <c r="P11" s="4" t="s">
+      <c r="V11" s="4" t="s">
         <v>275</v>
       </c>
-      <c r="Q11" s="4" t="s">
+      <c r="W11" s="4" t="s">
         <v>276</v>
-      </c>
-      <c r="R11" s="4" t="s">
-        <v>277</v>
-      </c>
-      <c r="S11" s="4" t="s">
-        <v>278</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>279</v>
-      </c>
-      <c r="U11" s="4" t="s">
-        <v>280</v>
-      </c>
-      <c r="V11" s="4" t="s">
-        <v>281</v>
-      </c>
-      <c r="W11" s="4" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="12" s="23" customFormat="1" spans="1:23">
@@ -10624,7 +10432,7 @@
         <v>56</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -10653,7 +10461,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>284</v>
+        <v>278</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -10679,7 +10487,7 @@
     </row>
     <row r="15" s="24" customFormat="1" spans="1:23">
       <c r="A15" s="3" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B15" s="3">
         <v>128</v>
@@ -10708,7 +10516,7 @@
     </row>
     <row r="16" s="24" customFormat="1" spans="1:23">
       <c r="A16" s="3" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B16" s="3">
         <v>5</v>
@@ -10898,19 +10706,19 @@
     </row>
     <row r="24" s="24" customFormat="1" spans="1:5">
       <c r="A24" s="4" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>286</v>
+        <v>280</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
     </row>
     <row r="25" s="24" customFormat="1" spans="1:5">
@@ -10935,7 +10743,7 @@
         <v>56</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -10964,7 +10772,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -10987,7 +10795,7 @@
     </row>
     <row r="28" s="24" customFormat="1" spans="1:20">
       <c r="A28" s="3" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B28" s="3">
         <v>8</v>
@@ -11013,7 +10821,7 @@
     </row>
     <row r="29" s="24" customFormat="1" spans="1:20">
       <c r="A29" s="3" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B29" s="3">
         <v>2</v>
@@ -11185,10 +10993,10 @@
     </row>
     <row r="37" s="24" customFormat="1" spans="1:2">
       <c r="A37" s="4" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
     </row>
     <row r="38" s="24" customFormat="1" spans="1:2">
@@ -11204,7 +11012,7 @@
         <v>56</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -11230,7 +11038,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>288</v>
+        <v>282</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -11256,7 +11064,7 @@
     </row>
     <row r="41" s="24" customFormat="1" spans="1:23">
       <c r="A41" s="3" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B41" s="3">
         <v>128</v>
@@ -11285,7 +11093,7 @@
     </row>
     <row r="42" s="24" customFormat="1" spans="1:23">
       <c r="A42" s="3" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B42" s="3">
         <v>4</v>
@@ -11475,16 +11283,16 @@
     </row>
     <row r="50" s="24" customFormat="1" spans="1:4">
       <c r="A50" s="4" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>285</v>
+        <v>279</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>289</v>
+        <v>283</v>
       </c>
     </row>
     <row r="51" s="24" customFormat="1" spans="1:4">
@@ -11498,7 +11306,7 @@
         <v>47</v>
       </c>
       <c r="D51" s="25" t="s">
-        <v>194</v>
+        <v>284</v>
       </c>
     </row>
     <row r="52" s="24" customFormat="1" spans="1:23">
@@ -11577,12 +11385,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>290</v>
+        <v>285</v>
       </c>
     </row>
     <row r="2" s="11" customFormat="1" spans="1:2">
       <c r="A2" s="14" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B2" s="14">
         <v>8</v>
@@ -11590,7 +11398,7 @@
     </row>
     <row r="3" s="11" customFormat="1" spans="1:2">
       <c r="A3" s="14" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B3" s="14">
         <v>4</v>
@@ -11646,7 +11454,7 @@
     </row>
     <row r="10" s="11" customFormat="1" spans="1:2">
       <c r="A10" s="14" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B10" s="14">
         <v>0</v>
@@ -11654,16 +11462,16 @@
     </row>
     <row r="11" s="11" customFormat="1" spans="1:4">
       <c r="A11" s="19" t="s">
-        <v>292</v>
+        <v>287</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>293</v>
+        <v>288</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>294</v>
+        <v>289</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
     </row>
     <row r="12" s="11" customFormat="1" spans="1:4">
@@ -11685,7 +11493,7 @@
         <v>56</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="C13" s="19"/>
       <c r="D13" s="19"/>
@@ -11695,12 +11503,12 @@
         <v>0</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="15" s="11" customFormat="1" spans="1:2">
       <c r="A15" s="14" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B15" s="14">
         <v>512</v>
@@ -11708,7 +11516,7 @@
     </row>
     <row r="16" s="11" customFormat="1" spans="1:2">
       <c r="A16" s="14" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B16" s="14">
         <v>3</v>
@@ -11764,7 +11572,7 @@
     </row>
     <row r="23" s="11" customFormat="1" spans="1:2">
       <c r="A23" s="14" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B23" s="14">
         <v>0</v>
@@ -11772,13 +11580,13 @@
     </row>
     <row r="24" s="11" customFormat="1" spans="1:3">
       <c r="A24" s="19" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
     </row>
     <row r="25" s="11" customFormat="1" spans="1:3">
@@ -11797,7 +11605,7 @@
         <v>56</v>
       </c>
       <c r="B26" s="21" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="C26" s="19"/>
     </row>
@@ -11856,12 +11664,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
     </row>
     <row r="2" s="11" customFormat="1" spans="1:2">
       <c r="A2" s="14" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B2" s="14">
         <v>10</v>
@@ -11869,7 +11677,7 @@
     </row>
     <row r="3" s="11" customFormat="1" spans="1:2">
       <c r="A3" s="14" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B3" s="14">
         <v>20</v>
@@ -11925,7 +11733,7 @@
     </row>
     <row r="10" s="11" customFormat="1" ht="14.25" spans="1:2">
       <c r="A10" s="14" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B10" s="14">
         <v>0</v>
@@ -11933,43 +11741,43 @@
     </row>
     <row r="11" s="11" customFormat="1" ht="30" spans="1:20">
       <c r="A11" s="15" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B11" s="16" t="s">
+        <v>297</v>
+      </c>
+      <c r="C11" s="16" t="s">
+        <v>298</v>
+      </c>
+      <c r="D11" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="E11" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="F11" s="16" t="s">
+        <v>301</v>
+      </c>
+      <c r="G11" s="16" t="s">
         <v>302</v>
       </c>
-      <c r="C11" s="16" t="s">
+      <c r="H11" s="16" t="s">
         <v>303</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="I11" s="16" t="s">
         <v>304</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="J11" s="16" t="s">
         <v>305</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="K11" s="16" t="s">
         <v>306</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="L11" s="16" t="s">
         <v>307</v>
       </c>
-      <c r="H11" s="16" t="s">
+      <c r="M11" s="16" t="s">
         <v>308</v>
-      </c>
-      <c r="I11" s="16" t="s">
-        <v>309</v>
-      </c>
-      <c r="J11" s="16" t="s">
-        <v>310</v>
-      </c>
-      <c r="K11" s="16" t="s">
-        <v>311</v>
-      </c>
-      <c r="L11" s="16" t="s">
-        <v>312</v>
-      </c>
-      <c r="M11" s="16" t="s">
-        <v>313</v>
       </c>
       <c r="N11" s="16" t="s">
         <v>16</v>
@@ -11978,19 +11786,19 @@
         <v>17</v>
       </c>
       <c r="P11" s="16" t="s">
-        <v>314</v>
+        <v>309</v>
       </c>
       <c r="Q11" s="16" t="s">
-        <v>315</v>
+        <v>310</v>
       </c>
       <c r="R11" s="16" t="s">
-        <v>316</v>
+        <v>311</v>
       </c>
       <c r="S11" s="16" t="s">
-        <v>317</v>
+        <v>312</v>
       </c>
       <c r="T11" s="16" t="s">
-        <v>318</v>
+        <v>313</v>
       </c>
     </row>
     <row r="12" s="11" customFormat="1" ht="15" spans="1:20">
@@ -12122,12 +11930,12 @@
         <v>0</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>319</v>
+        <v>314</v>
       </c>
     </row>
     <row r="15" s="11" customFormat="1" spans="1:2">
       <c r="A15" s="14" t="s">
-        <v>243</v>
+        <v>236</v>
       </c>
       <c r="B15" s="14">
         <v>100</v>
@@ -12135,7 +11943,7 @@
     </row>
     <row r="16" s="11" customFormat="1" spans="1:2">
       <c r="A16" s="14" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="B16" s="14">
         <v>2</v>
@@ -12191,7 +11999,7 @@
     </row>
     <row r="23" s="11" customFormat="1" ht="14.25" spans="1:2">
       <c r="A23" s="14" t="s">
-        <v>291</v>
+        <v>286</v>
       </c>
       <c r="B23" s="14">
         <v>0</v>
@@ -12199,10 +12007,10 @@
     </row>
     <row r="24" s="11" customFormat="1" ht="15" spans="1:3">
       <c r="A24" s="15" t="s">
-        <v>320</v>
+        <v>315</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>321</v>
+        <v>316</v>
       </c>
       <c r="C24" s="3"/>
     </row>

</xml_diff>

<commit_message>
the broadcast system for scene property management system && scene record management system
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Player.xlsx
+++ b/_Out/NFDataCfg/Excel/Player.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="21495" windowHeight="10335" activeTab="5"/>
+    <workbookView windowWidth="21495" windowHeight="10335" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -458,7 +458,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="341">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="309">
   <si>
     <t>Id</t>
   </si>
@@ -928,24 +928,12 @@
     <t>Streak</t>
   </si>
   <si>
-    <t>MatchStar</t>
-  </si>
-  <si>
-    <t>GambleDiamond</t>
-  </si>
-  <si>
-    <t>WinGold</t>
-  </si>
-  <si>
-    <t>WinCup</t>
-  </si>
-  <si>
-    <t>WinDiamond</t>
-  </si>
-  <si>
     <t>FightHeroID</t>
   </si>
   <si>
+    <t>FightHeroCnfID</t>
+  </si>
+  <si>
     <t>HeroID1</t>
   </si>
   <si>
@@ -955,9 +943,6 @@
     <t>HeroID3</t>
   </si>
   <si>
-    <t>FightHeroCnfID</t>
-  </si>
-  <si>
     <t>HeroCnfID1</t>
   </si>
   <si>
@@ -976,91 +961,10 @@
     <t>HeroStar3</t>
   </si>
   <si>
-    <t>MatchTeamID</t>
-  </si>
-  <si>
-    <t>MatchID</t>
-  </si>
-  <si>
-    <t>MatchPlayers</t>
-  </si>
-  <si>
-    <t>OpponentFighting</t>
-  </si>
-  <si>
-    <t>WarEventTime</t>
-  </si>
-  <si>
-    <t>Item1UsedCount</t>
-  </si>
-  <si>
-    <t>Item2UsedCount</t>
-  </si>
-  <si>
-    <t>Item3UsedCount</t>
-  </si>
-  <si>
-    <t>FightHeroLevel</t>
-  </si>
-  <si>
-    <t>OpponentID</t>
-  </si>
-  <si>
-    <t>OpponentLevel</t>
-  </si>
-  <si>
-    <t>OpponentGold</t>
-  </si>
-  <si>
-    <t>OpponentDiamond</t>
-  </si>
-  <si>
-    <t>OpponentCup</t>
-  </si>
-  <si>
-    <t>OpponentName</t>
-  </si>
-  <si>
-    <t>OpponentHead</t>
-  </si>
-  <si>
-    <t>OpponentHero1</t>
-  </si>
-  <si>
-    <t>OpponentHero2</t>
-  </si>
-  <si>
-    <t>OpponentHero3</t>
-  </si>
-  <si>
-    <t>OpponentHeroStar1</t>
-  </si>
-  <si>
-    <t>OpponentHeroStar2</t>
-  </si>
-  <si>
-    <t>OpponentHeroStar3</t>
-  </si>
-  <si>
     <t>streak win count</t>
   </si>
   <si>
-    <t>Hero1</t>
-  </si>
-  <si>
-    <t>Hero2</t>
-  </si>
-  <si>
-    <t>Hero3</t>
-  </si>
-  <si>
     <t>主要是给离线玩家看</t>
-  </si>
-  <si>
-    <t>pvp_oppnent</t>
-  </si>
-  <si>
-    <t>when searching</t>
   </si>
   <si>
     <t>Clan_Name</t>
@@ -1527,9 +1431,9 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -1564,12 +1468,19 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1582,22 +1493,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -1611,9 +1509,30 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1627,8 +1546,38 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -1645,14 +1594,15 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1665,54 +1615,8 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="40">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1757,7 +1661,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1769,61 +1829,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1835,115 +1841,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2073,17 +1971,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2092,7 +1984,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2114,6 +2006,15 @@
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -2123,20 +2024,17 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -2175,152 +2073,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="16" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="15" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="21" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="24" borderId="16" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="13" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2449,21 +2347,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -4184,112 +4067,112 @@
       <c r="A10" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="45" t="s">
         <v>59</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="45" t="s">
         <v>60</v>
       </c>
-      <c r="D10" s="50" t="s">
+      <c r="D10" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="E10" s="50" t="s">
+      <c r="E10" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="50" t="s">
+      <c r="F10" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="G10" s="50" t="s">
+      <c r="G10" s="45" t="s">
         <v>64</v>
       </c>
-      <c r="H10" s="50" t="s">
+      <c r="H10" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="I10" s="50" t="s">
+      <c r="I10" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="J10" s="50" t="s">
+      <c r="J10" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="K10" s="50" t="s">
+      <c r="K10" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="L10" s="50" t="s">
+      <c r="L10" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="M10" s="50" t="s">
+      <c r="M10" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="N10" s="50" t="s">
+      <c r="N10" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="O10" s="50" t="s">
+      <c r="O10" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="P10" s="50" t="s">
+      <c r="P10" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="Q10" s="50" t="s">
+      <c r="Q10" s="45" t="s">
         <v>73</v>
       </c>
-      <c r="R10" s="50" t="s">
+      <c r="R10" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="S10" s="50" t="s">
+      <c r="S10" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="T10" s="50" t="s">
+      <c r="T10" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="U10" s="50" t="s">
+      <c r="U10" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="V10" s="50" t="s">
+      <c r="V10" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="W10" s="50" t="s">
+      <c r="W10" s="45" t="s">
         <v>79</v>
       </c>
-      <c r="X10" s="50" t="s">
+      <c r="X10" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="Y10" s="50" t="s">
+      <c r="Y10" s="45" t="s">
         <v>81</v>
       </c>
-      <c r="Z10" s="50" t="s">
+      <c r="Z10" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="AA10" s="50" t="s">
+      <c r="AA10" s="45" t="s">
         <v>83</v>
       </c>
-      <c r="AB10" s="50" t="s">
+      <c r="AB10" s="45" t="s">
         <v>84</v>
       </c>
-      <c r="AC10" s="50" t="s">
+      <c r="AC10" s="45" t="s">
         <v>85</v>
       </c>
-      <c r="AD10" s="50" t="s">
+      <c r="AD10" s="45" t="s">
         <v>86</v>
       </c>
-      <c r="AE10" s="50" t="s">
+      <c r="AE10" s="45" t="s">
         <v>87</v>
       </c>
-      <c r="AF10" s="50" t="s">
+      <c r="AF10" s="45" t="s">
         <v>88</v>
       </c>
-      <c r="AG10" s="50" t="s">
+      <c r="AG10" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="AH10" s="50" t="s">
+      <c r="AH10" s="45" t="s">
         <v>90</v>
       </c>
-      <c r="AI10" s="50" t="s">
+      <c r="AI10" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="AJ10" s="50" t="s">
+      <c r="AJ10" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="AK10" s="50" t="s">
+      <c r="AK10" s="45" t="s">
         <v>92</v>
       </c>
       <c r="AL10" s="42" t="s">
@@ -4363,12 +4246,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>311</v>
+        <v>279</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B2" s="3">
         <v>128</v>
@@ -4376,7 +4259,7 @@
     </row>
     <row r="3" s="3" customFormat="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="B3" s="3">
         <v>5</v>
@@ -4432,7 +4315,7 @@
     </row>
     <row r="10" s="3" customFormat="1" spans="1:2">
       <c r="A10" s="3" t="s">
-        <v>238</v>
+        <v>206</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -4440,19 +4323,19 @@
     </row>
     <row r="11" s="3" customFormat="1" spans="1:5">
       <c r="A11" s="4" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>314</v>
+        <v>282</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>315</v>
+        <v>283</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>316</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12" s="3" customFormat="1" spans="1:5">
@@ -4486,12 +4369,12 @@
         <v>0</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>317</v>
+        <v>285</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B15" s="3">
         <v>128</v>
@@ -4499,7 +4382,7 @@
     </row>
     <row r="16" s="3" customFormat="1" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="B16" s="3">
         <v>5</v>
@@ -4563,19 +4446,19 @@
     </row>
     <row r="24" s="3" customFormat="1" spans="1:5">
       <c r="A24" s="4" t="s">
-        <v>312</v>
+        <v>280</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>313</v>
+        <v>281</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>314</v>
+        <v>282</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>315</v>
+        <v>283</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>316</v>
+        <v>284</v>
       </c>
     </row>
     <row r="25" s="3" customFormat="1" spans="1:5">
@@ -4646,7 +4529,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>318</v>
+        <v>286</v>
       </c>
       <c r="C1" s="6"/>
       <c r="D1" s="6"/>
@@ -4664,7 +4547,7 @@
     </row>
     <row r="2" ht="15" spans="1:15">
       <c r="A2" s="7" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B2" s="7">
         <v>50</v>
@@ -4685,7 +4568,7 @@
     </row>
     <row r="3" ht="15" spans="1:15">
       <c r="A3" s="7" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="B3" s="7">
         <v>15</v>
@@ -4853,7 +4736,7 @@
     </row>
     <row r="11" ht="15" spans="1:15">
       <c r="A11" s="8" t="s">
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>1</v>
@@ -4865,37 +4748,37 @@
         <v>3</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>319</v>
+        <v>287</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>320</v>
+        <v>288</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>321</v>
+        <v>289</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>322</v>
+        <v>290</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>323</v>
+        <v>291</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>324</v>
+        <v>292</v>
       </c>
       <c r="K11" s="8" t="s">
         <v>30</v>
       </c>
       <c r="L11" s="8" t="s">
-        <v>325</v>
+        <v>293</v>
       </c>
       <c r="M11" s="8" t="s">
-        <v>326</v>
+        <v>294</v>
       </c>
       <c r="N11" s="8" t="s">
-        <v>327</v>
+        <v>295</v>
       </c>
       <c r="O11" s="8" t="s">
-        <v>328</v>
+        <v>296</v>
       </c>
     </row>
     <row r="12" ht="15" spans="1:15">
@@ -4950,7 +4833,7 @@
         <v>58</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>329</v>
+        <v>297</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="8"/>
@@ -4971,7 +4854,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>330</v>
+        <v>298</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
@@ -4989,7 +4872,7 @@
     </row>
     <row r="15" ht="15" spans="1:15">
       <c r="A15" s="7" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B15" s="7">
         <v>50</v>
@@ -5010,7 +4893,7 @@
     </row>
     <row r="16" ht="15" spans="1:15">
       <c r="A16" s="7" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="B16" s="7">
         <v>4</v>
@@ -5178,7 +5061,7 @@
     </row>
     <row r="24" ht="15" spans="1:15">
       <c r="A24" s="8" t="s">
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="B24" s="8" t="s">
         <v>1</v>
@@ -5187,7 +5070,7 @@
         <v>6</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>321</v>
+        <v>289</v>
       </c>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -5231,7 +5114,7 @@
         <v>58</v>
       </c>
       <c r="B26" s="8" t="s">
-        <v>329</v>
+        <v>297</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -5252,7 +5135,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>331</v>
+        <v>299</v>
       </c>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -5270,7 +5153,7 @@
     </row>
     <row r="28" ht="15" spans="1:15">
       <c r="A28" s="7" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B28" s="7">
         <v>50</v>
@@ -5291,7 +5174,7 @@
     </row>
     <row r="29" ht="15" spans="1:15">
       <c r="A29" s="7" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="B29" s="7">
         <v>3</v>
@@ -5459,7 +5342,7 @@
     </row>
     <row r="37" ht="15" spans="1:15">
       <c r="A37" s="8" t="s">
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="B37" s="8" t="s">
         <v>1</v>
@@ -5508,7 +5391,7 @@
         <v>58</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>329</v>
+        <v>297</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="7"/>
@@ -5529,7 +5412,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
@@ -5547,7 +5430,7 @@
     </row>
     <row r="41" ht="15" spans="1:15">
       <c r="A41" s="7" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B41" s="7">
         <v>50</v>
@@ -5568,7 +5451,7 @@
     </row>
     <row r="42" ht="15" spans="1:15">
       <c r="A42" s="7" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="B42" s="7">
         <v>2</v>
@@ -5736,7 +5619,7 @@
     </row>
     <row r="50" ht="15" spans="1:15">
       <c r="A50" s="8" t="s">
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="B50" s="8" t="s">
         <v>6</v>
@@ -5834,10 +5717,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="C1" t="s">
-        <v>334</v>
+        <v>302</v>
       </c>
       <c r="D1" t="s">
         <v>58</v>
@@ -5845,16 +5728,16 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="5" t="s">
-        <v>335</v>
+        <v>303</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>336</v>
+        <v>304</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>337</v>
+        <v>305</v>
       </c>
     </row>
   </sheetData>
@@ -5888,12 +5771,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>338</v>
+        <v>306</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B2" s="3">
         <v>8</v>
@@ -5901,7 +5784,7 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="B3" s="3">
         <v>2</v>
@@ -5965,10 +5848,10 @@
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="4" t="s">
-        <v>339</v>
+        <v>307</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>340</v>
+        <v>308</v>
       </c>
     </row>
     <row r="12" spans="1:2">
@@ -6019,210 +5902,210 @@
     <col min="1" max="1" width="13.6666666666667" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="48" customFormat="1" ht="27" spans="1:33">
-      <c r="A1" s="51" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="48" t="s">
+    <row r="1" s="43" customFormat="1" ht="27" spans="1:33">
+      <c r="A1" s="46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="C1" s="48" t="s">
+      <c r="C1" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="D1" s="48" t="s">
+      <c r="D1" s="43" t="s">
         <v>97</v>
       </c>
-      <c r="E1" s="48" t="s">
+      <c r="E1" s="43" t="s">
         <v>98</v>
       </c>
-      <c r="F1" s="48" t="s">
+      <c r="F1" s="43" t="s">
         <v>99</v>
       </c>
-      <c r="G1" s="48" t="s">
+      <c r="G1" s="43" t="s">
         <v>100</v>
       </c>
-      <c r="H1" s="48" t="s">
+      <c r="H1" s="43" t="s">
         <v>101</v>
       </c>
-      <c r="I1" s="48" t="s">
+      <c r="I1" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="J1" s="48" t="s">
+      <c r="J1" s="43" t="s">
         <v>103</v>
       </c>
-      <c r="K1" s="48" t="s">
+      <c r="K1" s="43" t="s">
         <v>104</v>
       </c>
-      <c r="L1" s="48" t="s">
+      <c r="L1" s="43" t="s">
         <v>105</v>
       </c>
-      <c r="M1" s="48" t="s">
+      <c r="M1" s="43" t="s">
         <v>106</v>
       </c>
-      <c r="N1" s="48" t="s">
+      <c r="N1" s="43" t="s">
         <v>107</v>
       </c>
-      <c r="O1" s="48" t="s">
+      <c r="O1" s="43" t="s">
         <v>108</v>
       </c>
-      <c r="P1" s="48" t="s">
+      <c r="P1" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="Q1" s="48" t="s">
+      <c r="Q1" s="43" t="s">
         <v>110</v>
       </c>
-      <c r="R1" s="48" t="s">
+      <c r="R1" s="43" t="s">
         <v>111</v>
       </c>
-      <c r="S1" s="48" t="s">
+      <c r="S1" s="43" t="s">
         <v>112</v>
       </c>
-      <c r="T1" s="48" t="s">
+      <c r="T1" s="43" t="s">
         <v>113</v>
       </c>
-      <c r="U1" s="48" t="s">
+      <c r="U1" s="43" t="s">
         <v>114</v>
       </c>
-      <c r="V1" s="48" t="s">
+      <c r="V1" s="43" t="s">
         <v>115</v>
       </c>
-      <c r="W1" s="48" t="s">
+      <c r="W1" s="43" t="s">
         <v>116</v>
       </c>
-      <c r="X1" s="48" t="s">
+      <c r="X1" s="43" t="s">
         <v>117</v>
       </c>
-      <c r="Y1" s="48" t="s">
+      <c r="Y1" s="43" t="s">
         <v>118</v>
       </c>
-      <c r="Z1" s="48" t="s">
+      <c r="Z1" s="43" t="s">
         <v>119</v>
       </c>
-      <c r="AA1" s="48" t="s">
+      <c r="AA1" s="43" t="s">
         <v>120</v>
       </c>
-      <c r="AB1" s="48" t="s">
+      <c r="AB1" s="43" t="s">
         <v>121</v>
       </c>
-      <c r="AC1" s="48" t="s">
+      <c r="AC1" s="43" t="s">
         <v>122</v>
       </c>
-      <c r="AD1" s="48" t="s">
+      <c r="AD1" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="AE1" s="48" t="s">
+      <c r="AE1" s="43" t="s">
         <v>124</v>
       </c>
-      <c r="AF1" s="48" t="s">
+      <c r="AF1" s="43" t="s">
         <v>125</v>
       </c>
-      <c r="AG1" s="48" t="s">
+      <c r="AG1" s="43" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="2" s="49" customFormat="1" spans="1:33">
-      <c r="A2" s="52" t="s">
+    <row r="2" s="44" customFormat="1" spans="1:33">
+      <c r="A2" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="D2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="F2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="H2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="J2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="L2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="N2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="O2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="P2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="R2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="S2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="T2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="U2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="V2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="W2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="X2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="AF2" s="49" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG2" s="49" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" s="49" customFormat="1" spans="1:33">
-      <c r="A3" s="52" t="s">
+      <c r="B2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="F2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="J2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="L2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="P2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="R2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="T2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="U2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="V2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="W2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="X2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="AB2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="AD2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="AF2" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG2" s="44" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" s="44" customFormat="1" spans="1:33">
+      <c r="A3" s="47" t="s">
         <v>51</v>
       </c>
       <c r="B3" s="27">
@@ -6234,7 +6117,7 @@
       <c r="D3" s="27">
         <v>0</v>
       </c>
-      <c r="E3" s="49">
+      <c r="E3" s="44">
         <v>1</v>
       </c>
       <c r="F3" s="27">
@@ -6258,7 +6141,7 @@
       <c r="L3" s="27">
         <v>0</v>
       </c>
-      <c r="M3" s="49">
+      <c r="M3" s="44">
         <v>1</v>
       </c>
       <c r="N3" s="27">
@@ -6300,328 +6183,328 @@
       <c r="Z3" s="27">
         <v>0</v>
       </c>
-      <c r="AA3" s="49">
-        <v>1</v>
-      </c>
-      <c r="AB3" s="49">
-        <v>1</v>
-      </c>
-      <c r="AC3" s="49">
-        <v>1</v>
-      </c>
-      <c r="AD3" s="49">
-        <v>1</v>
-      </c>
-      <c r="AE3" s="49">
-        <v>1</v>
-      </c>
-      <c r="AF3" s="49">
-        <v>1</v>
-      </c>
-      <c r="AG3" s="49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" s="49" customFormat="1" spans="1:33">
-      <c r="A4" s="52" t="s">
+      <c r="AA3" s="44">
+        <v>1</v>
+      </c>
+      <c r="AB3" s="44">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="44">
+        <v>1</v>
+      </c>
+      <c r="AD3" s="44">
+        <v>1</v>
+      </c>
+      <c r="AE3" s="44">
+        <v>1</v>
+      </c>
+      <c r="AF3" s="44">
+        <v>1</v>
+      </c>
+      <c r="AG3" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" s="44" customFormat="1" spans="1:33">
+      <c r="A4" s="47" t="s">
         <v>52</v>
       </c>
-      <c r="B4" s="49">
-        <v>1</v>
-      </c>
-      <c r="C4" s="49">
-        <v>1</v>
-      </c>
-      <c r="D4" s="49">
-        <v>1</v>
-      </c>
-      <c r="E4" s="49">
-        <v>1</v>
-      </c>
-      <c r="F4" s="49">
-        <v>1</v>
-      </c>
-      <c r="G4" s="49">
-        <v>1</v>
-      </c>
-      <c r="H4" s="49">
-        <v>1</v>
-      </c>
-      <c r="I4" s="49">
-        <v>1</v>
-      </c>
-      <c r="J4" s="49">
-        <v>1</v>
-      </c>
-      <c r="K4" s="49">
-        <v>1</v>
-      </c>
-      <c r="L4" s="49">
-        <v>1</v>
-      </c>
-      <c r="M4" s="49">
-        <v>1</v>
-      </c>
-      <c r="N4" s="49">
-        <v>1</v>
-      </c>
-      <c r="O4" s="49">
-        <v>1</v>
-      </c>
-      <c r="P4" s="49">
-        <v>1</v>
-      </c>
-      <c r="Q4" s="49">
-        <v>1</v>
-      </c>
-      <c r="R4" s="49">
-        <v>1</v>
-      </c>
-      <c r="S4" s="49">
-        <v>1</v>
-      </c>
-      <c r="T4" s="49">
-        <v>1</v>
-      </c>
-      <c r="U4" s="49">
-        <v>1</v>
-      </c>
-      <c r="V4" s="49">
-        <v>1</v>
-      </c>
-      <c r="W4" s="49">
-        <v>1</v>
-      </c>
-      <c r="X4" s="49">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="49">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="49">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="49">
-        <v>1</v>
-      </c>
-      <c r="AB4" s="49">
-        <v>1</v>
-      </c>
-      <c r="AC4" s="49">
-        <v>1</v>
-      </c>
-      <c r="AD4" s="49">
-        <v>1</v>
-      </c>
-      <c r="AE4" s="49">
-        <v>1</v>
-      </c>
-      <c r="AF4" s="49">
-        <v>1</v>
-      </c>
-      <c r="AG4" s="49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" s="49" customFormat="1" spans="1:33">
-      <c r="A5" s="52" t="s">
+      <c r="B4" s="44">
+        <v>1</v>
+      </c>
+      <c r="C4" s="44">
+        <v>1</v>
+      </c>
+      <c r="D4" s="44">
+        <v>1</v>
+      </c>
+      <c r="E4" s="44">
+        <v>1</v>
+      </c>
+      <c r="F4" s="44">
+        <v>1</v>
+      </c>
+      <c r="G4" s="44">
+        <v>1</v>
+      </c>
+      <c r="H4" s="44">
+        <v>1</v>
+      </c>
+      <c r="I4" s="44">
+        <v>1</v>
+      </c>
+      <c r="J4" s="44">
+        <v>1</v>
+      </c>
+      <c r="K4" s="44">
+        <v>1</v>
+      </c>
+      <c r="L4" s="44">
+        <v>1</v>
+      </c>
+      <c r="M4" s="44">
+        <v>1</v>
+      </c>
+      <c r="N4" s="44">
+        <v>1</v>
+      </c>
+      <c r="O4" s="44">
+        <v>1</v>
+      </c>
+      <c r="P4" s="44">
+        <v>1</v>
+      </c>
+      <c r="Q4" s="44">
+        <v>1</v>
+      </c>
+      <c r="R4" s="44">
+        <v>1</v>
+      </c>
+      <c r="S4" s="44">
+        <v>1</v>
+      </c>
+      <c r="T4" s="44">
+        <v>1</v>
+      </c>
+      <c r="U4" s="44">
+        <v>1</v>
+      </c>
+      <c r="V4" s="44">
+        <v>1</v>
+      </c>
+      <c r="W4" s="44">
+        <v>1</v>
+      </c>
+      <c r="X4" s="44">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="44">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="44">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="44">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="44">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="44">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="44">
+        <v>1</v>
+      </c>
+      <c r="AE4" s="44">
+        <v>1</v>
+      </c>
+      <c r="AF4" s="44">
+        <v>1</v>
+      </c>
+      <c r="AG4" s="44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" s="44" customFormat="1" spans="1:33">
+      <c r="A5" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="B5" s="49">
-        <v>0</v>
-      </c>
-      <c r="C5" s="49">
-        <v>0</v>
-      </c>
-      <c r="D5" s="49">
-        <v>0</v>
-      </c>
-      <c r="E5" s="49">
-        <v>0</v>
-      </c>
-      <c r="F5" s="49">
-        <v>0</v>
-      </c>
-      <c r="G5" s="49">
-        <v>0</v>
-      </c>
-      <c r="H5" s="49">
-        <v>0</v>
-      </c>
-      <c r="I5" s="49">
-        <v>0</v>
-      </c>
-      <c r="J5" s="49">
-        <v>0</v>
-      </c>
-      <c r="K5" s="49">
-        <v>0</v>
-      </c>
-      <c r="L5" s="49">
-        <v>0</v>
-      </c>
-      <c r="M5" s="49">
-        <v>0</v>
-      </c>
-      <c r="N5" s="49">
-        <v>0</v>
-      </c>
-      <c r="O5" s="49">
-        <v>0</v>
-      </c>
-      <c r="P5" s="49">
-        <v>0</v>
-      </c>
-      <c r="Q5" s="49">
-        <v>0</v>
-      </c>
-      <c r="R5" s="49">
-        <v>0</v>
-      </c>
-      <c r="S5" s="49">
-        <v>0</v>
-      </c>
-      <c r="T5" s="49">
-        <v>0</v>
-      </c>
-      <c r="U5" s="49">
-        <v>0</v>
-      </c>
-      <c r="V5" s="49">
-        <v>0</v>
-      </c>
-      <c r="W5" s="49">
-        <v>0</v>
-      </c>
-      <c r="X5" s="49">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="49">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="49">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="49">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="49">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="49">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="49">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="49">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="49">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="49">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" s="49" customFormat="1" spans="1:33">
-      <c r="A6" s="52" t="s">
+      <c r="B5" s="44">
+        <v>0</v>
+      </c>
+      <c r="C5" s="44">
+        <v>0</v>
+      </c>
+      <c r="D5" s="44">
+        <v>0</v>
+      </c>
+      <c r="E5" s="44">
+        <v>0</v>
+      </c>
+      <c r="F5" s="44">
+        <v>0</v>
+      </c>
+      <c r="G5" s="44">
+        <v>0</v>
+      </c>
+      <c r="H5" s="44">
+        <v>0</v>
+      </c>
+      <c r="I5" s="44">
+        <v>0</v>
+      </c>
+      <c r="J5" s="44">
+        <v>0</v>
+      </c>
+      <c r="K5" s="44">
+        <v>0</v>
+      </c>
+      <c r="L5" s="44">
+        <v>0</v>
+      </c>
+      <c r="M5" s="44">
+        <v>0</v>
+      </c>
+      <c r="N5" s="44">
+        <v>0</v>
+      </c>
+      <c r="O5" s="44">
+        <v>0</v>
+      </c>
+      <c r="P5" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q5" s="44">
+        <v>0</v>
+      </c>
+      <c r="R5" s="44">
+        <v>0</v>
+      </c>
+      <c r="S5" s="44">
+        <v>0</v>
+      </c>
+      <c r="T5" s="44">
+        <v>0</v>
+      </c>
+      <c r="U5" s="44">
+        <v>0</v>
+      </c>
+      <c r="V5" s="44">
+        <v>0</v>
+      </c>
+      <c r="W5" s="44">
+        <v>0</v>
+      </c>
+      <c r="X5" s="44">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="44">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="44">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="44">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="44">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="44">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="44">
+        <v>0</v>
+      </c>
+      <c r="AE5" s="44">
+        <v>0</v>
+      </c>
+      <c r="AF5" s="44">
+        <v>0</v>
+      </c>
+      <c r="AG5" s="44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" s="44" customFormat="1" spans="1:33">
+      <c r="A6" s="47" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="49">
-        <v>0</v>
-      </c>
-      <c r="C6" s="49">
-        <v>0</v>
-      </c>
-      <c r="D6" s="49">
-        <v>0</v>
-      </c>
-      <c r="E6" s="49">
-        <v>0</v>
-      </c>
-      <c r="F6" s="49">
-        <v>0</v>
-      </c>
-      <c r="G6" s="49">
-        <v>0</v>
-      </c>
-      <c r="H6" s="49">
-        <v>0</v>
-      </c>
-      <c r="I6" s="49">
-        <v>0</v>
-      </c>
-      <c r="J6" s="49">
-        <v>0</v>
-      </c>
-      <c r="K6" s="49">
-        <v>0</v>
-      </c>
-      <c r="L6" s="49">
-        <v>0</v>
-      </c>
-      <c r="M6" s="49">
-        <v>0</v>
-      </c>
-      <c r="N6" s="49">
-        <v>0</v>
-      </c>
-      <c r="O6" s="49">
-        <v>0</v>
-      </c>
-      <c r="P6" s="49">
-        <v>0</v>
-      </c>
-      <c r="Q6" s="49">
-        <v>0</v>
-      </c>
-      <c r="R6" s="49">
-        <v>0</v>
-      </c>
-      <c r="S6" s="49">
-        <v>0</v>
-      </c>
-      <c r="T6" s="49">
-        <v>0</v>
-      </c>
-      <c r="U6" s="49">
-        <v>0</v>
-      </c>
-      <c r="V6" s="49">
-        <v>0</v>
-      </c>
-      <c r="W6" s="49">
-        <v>0</v>
-      </c>
-      <c r="X6" s="49">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="49">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="49">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="49">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="49">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="49">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="49">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="49">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="49">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="49">
+      <c r="B6" s="44">
+        <v>0</v>
+      </c>
+      <c r="C6" s="44">
+        <v>0</v>
+      </c>
+      <c r="D6" s="44">
+        <v>0</v>
+      </c>
+      <c r="E6" s="44">
+        <v>0</v>
+      </c>
+      <c r="F6" s="44">
+        <v>0</v>
+      </c>
+      <c r="G6" s="44">
+        <v>0</v>
+      </c>
+      <c r="H6" s="44">
+        <v>0</v>
+      </c>
+      <c r="I6" s="44">
+        <v>0</v>
+      </c>
+      <c r="J6" s="44">
+        <v>0</v>
+      </c>
+      <c r="K6" s="44">
+        <v>0</v>
+      </c>
+      <c r="L6" s="44">
+        <v>0</v>
+      </c>
+      <c r="M6" s="44">
+        <v>0</v>
+      </c>
+      <c r="N6" s="44">
+        <v>0</v>
+      </c>
+      <c r="O6" s="44">
+        <v>0</v>
+      </c>
+      <c r="P6" s="44">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="44">
+        <v>0</v>
+      </c>
+      <c r="R6" s="44">
+        <v>0</v>
+      </c>
+      <c r="S6" s="44">
+        <v>0</v>
+      </c>
+      <c r="T6" s="44">
+        <v>0</v>
+      </c>
+      <c r="U6" s="44">
+        <v>0</v>
+      </c>
+      <c r="V6" s="44">
+        <v>0</v>
+      </c>
+      <c r="W6" s="44">
+        <v>0</v>
+      </c>
+      <c r="X6" s="44">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="44">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="44">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="44">
+        <v>0</v>
+      </c>
+      <c r="AB6" s="44">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="44">
+        <v>0</v>
+      </c>
+      <c r="AD6" s="44">
+        <v>0</v>
+      </c>
+      <c r="AE6" s="44">
+        <v>0</v>
+      </c>
+      <c r="AF6" s="44">
+        <v>0</v>
+      </c>
+      <c r="AG6" s="44">
         <v>0</v>
       </c>
     </row>
@@ -6928,95 +6811,95 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" s="50" customFormat="1" ht="54.75" spans="1:32">
+    <row r="10" s="45" customFormat="1" ht="54.75" spans="1:32">
       <c r="A10" s="41" t="s">
         <v>58</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="B10" s="45" t="s">
         <v>127</v>
       </c>
-      <c r="C10" s="50" t="s">
+      <c r="C10" s="45" t="s">
         <v>128</v>
       </c>
-      <c r="D10" s="50" t="s">
+      <c r="D10" s="45" t="s">
         <v>129</v>
       </c>
-      <c r="E10" s="50" t="s">
+      <c r="E10" s="45" t="s">
         <v>70</v>
       </c>
-      <c r="F10" s="50" t="s">
+      <c r="F10" s="45" t="s">
         <v>72</v>
       </c>
-      <c r="G10" s="50" t="s">
+      <c r="G10" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="H10" s="50" t="s">
+      <c r="H10" s="45" t="s">
         <v>130</v>
       </c>
-      <c r="I10" s="50" t="s">
+      <c r="I10" s="45" t="s">
         <v>131</v>
       </c>
-      <c r="J10" s="50" t="s">
+      <c r="J10" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="K10" s="50" t="s">
+      <c r="K10" s="45" t="s">
         <v>133</v>
       </c>
-      <c r="L10" s="50" t="s">
+      <c r="L10" s="45" t="s">
         <v>134</v>
       </c>
-      <c r="M10" s="50" t="s">
+      <c r="M10" s="45" t="s">
         <v>135</v>
       </c>
-      <c r="N10" s="50" t="s">
+      <c r="N10" s="45" t="s">
         <v>136</v>
       </c>
-      <c r="O10" s="50" t="s">
+      <c r="O10" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="P10" s="50" t="s">
+      <c r="P10" s="45" t="s">
         <v>138</v>
       </c>
-      <c r="S10" s="50" t="s">
+      <c r="S10" s="45" t="s">
         <v>139</v>
       </c>
-      <c r="T10" s="50" t="s">
+      <c r="T10" s="45" t="s">
         <v>140</v>
       </c>
-      <c r="U10" s="50" t="s">
+      <c r="U10" s="45" t="s">
         <v>141</v>
       </c>
-      <c r="V10" s="50" t="s">
+      <c r="V10" s="45" t="s">
         <v>142</v>
       </c>
-      <c r="W10" s="50" t="s">
+      <c r="W10" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="X10" s="50" t="s">
+      <c r="X10" s="45" t="s">
         <v>143</v>
       </c>
-      <c r="Y10" s="50" t="s">
+      <c r="Y10" s="45" t="s">
         <v>144</v>
       </c>
-      <c r="Z10" s="50" t="s">
+      <c r="Z10" s="45" t="s">
         <v>145</v>
       </c>
-      <c r="AA10" s="50" t="s">
+      <c r="AA10" s="45" t="s">
         <v>146</v>
       </c>
-      <c r="AB10" s="50" t="s">
+      <c r="AB10" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="AC10" s="50" t="s">
+      <c r="AC10" s="45" t="s">
         <v>148</v>
       </c>
-      <c r="AD10" s="50" t="s">
+      <c r="AD10" s="45" t="s">
         <v>149</v>
       </c>
-      <c r="AE10" s="50" t="s">
+      <c r="AE10" s="45" t="s">
         <v>150</v>
       </c>
-      <c r="AF10" s="50" t="s">
+      <c r="AF10" s="45" t="s">
         <v>151</v>
       </c>
     </row>
@@ -7096,38 +6979,30 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AQ10"/>
+  <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="Y1" sqref="Y$1:Y$1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J1" sqref="F$1:J$1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="23.6666666666667" customWidth="1"/>
-    <col min="2" max="6" width="18.3333333333333" customWidth="1"/>
-    <col min="7" max="10" width="16" customWidth="1"/>
-    <col min="11" max="24" width="17.3333333333333" customWidth="1"/>
-    <col min="25" max="25" width="25.1666666666667" customWidth="1"/>
-    <col min="26" max="35" width="17.3333333333333" customWidth="1"/>
-    <col min="36" max="37" width="18.3333333333333" customWidth="1"/>
-    <col min="38" max="40" width="17.3333333333333" customWidth="1"/>
-    <col min="41" max="41" width="15.6666666666667" customWidth="1"/>
-    <col min="42" max="42" width="19.6666666666667" customWidth="1"/>
-    <col min="43" max="43" width="16" customWidth="1"/>
-    <col min="44" max="45" width="18.3333333333333" customWidth="1"/>
-    <col min="46" max="46" width="26.3333333333333" customWidth="1"/>
-    <col min="47" max="47" width="26.6666666666667" customWidth="1"/>
-    <col min="48" max="48" width="23.3333333333333" customWidth="1"/>
-    <col min="49" max="49" width="26.3333333333333" customWidth="1"/>
-    <col min="50" max="50" width="26.6666666666667" customWidth="1"/>
-    <col min="51" max="51" width="17.3333333333333" customWidth="1"/>
-    <col min="52" max="52" width="26.3333333333333" customWidth="1"/>
-    <col min="53" max="53" width="26.6666666666667" customWidth="1"/>
-    <col min="54" max="54" width="17.3333333333333" customWidth="1"/>
+    <col min="2" max="5" width="18.3333333333333" customWidth="1"/>
+    <col min="6" max="16" width="17.3333333333333" customWidth="1"/>
+    <col min="17" max="18" width="18.3333333333333" customWidth="1"/>
+    <col min="19" max="19" width="26.3333333333333" customWidth="1"/>
+    <col min="20" max="20" width="26.6666666666667" customWidth="1"/>
+    <col min="21" max="21" width="23.3333333333333" customWidth="1"/>
+    <col min="22" max="22" width="26.3333333333333" customWidth="1"/>
+    <col min="23" max="23" width="26.6666666666667" customWidth="1"/>
+    <col min="24" max="24" width="17.3333333333333" customWidth="1"/>
+    <col min="25" max="25" width="26.3333333333333" customWidth="1"/>
+    <col min="26" max="26" width="26.6666666666667" customWidth="1"/>
+    <col min="27" max="27" width="17.3333333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="33" customFormat="1" spans="1:43">
+    <row r="1" s="33" customFormat="1" spans="1:16">
       <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
@@ -7143,19 +7018,19 @@
       <c r="E1" s="37" t="s">
         <v>155</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="F1" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="G1" s="37" t="s">
         <v>157</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="H1" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="I1" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="J1" s="37" t="s">
         <v>160</v>
       </c>
       <c r="K1" s="37" t="s">
@@ -7176,89 +7051,8 @@
       <c r="P1" s="37" t="s">
         <v>166</v>
       </c>
-      <c r="Q1" s="37" t="s">
-        <v>167</v>
-      </c>
-      <c r="R1" s="37" t="s">
-        <v>168</v>
-      </c>
-      <c r="S1" s="37" t="s">
-        <v>169</v>
-      </c>
-      <c r="T1" s="37" t="s">
-        <v>170</v>
-      </c>
-      <c r="U1" s="37" t="s">
-        <v>171</v>
-      </c>
-      <c r="V1" s="37" t="s">
-        <v>172</v>
-      </c>
-      <c r="W1" s="37" t="s">
-        <v>173</v>
-      </c>
-      <c r="X1" s="37" t="s">
-        <v>174</v>
-      </c>
-      <c r="Y1" s="33" t="s">
-        <v>175</v>
-      </c>
-      <c r="Z1" s="37" t="s">
-        <v>176</v>
-      </c>
-      <c r="AA1" s="37" t="s">
-        <v>177</v>
-      </c>
-      <c r="AB1" s="37" t="s">
-        <v>178</v>
-      </c>
-      <c r="AC1" s="37" t="s">
-        <v>179</v>
-      </c>
-      <c r="AD1" s="33" t="s">
-        <v>180</v>
-      </c>
-      <c r="AE1" s="33" t="s">
-        <v>181</v>
-      </c>
-      <c r="AF1" s="33" t="s">
-        <v>182</v>
-      </c>
-      <c r="AG1" s="33" t="s">
-        <v>183</v>
-      </c>
-      <c r="AH1" s="33" t="s">
-        <v>184</v>
-      </c>
-      <c r="AI1" s="37" t="s">
-        <v>185</v>
-      </c>
-      <c r="AJ1" s="37" t="s">
-        <v>186</v>
-      </c>
-      <c r="AK1" s="37" t="s">
-        <v>187</v>
-      </c>
-      <c r="AL1" s="37" t="s">
-        <v>188</v>
-      </c>
-      <c r="AM1" s="37" t="s">
-        <v>189</v>
-      </c>
-      <c r="AN1" s="37" t="s">
-        <v>190</v>
-      </c>
-      <c r="AO1" s="37" t="s">
-        <v>191</v>
-      </c>
-      <c r="AP1" s="37" t="s">
-        <v>192</v>
-      </c>
-      <c r="AQ1" s="37" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="2" s="34" customFormat="1" spans="1:43">
+    </row>
+    <row r="2" s="34" customFormat="1" spans="1:16">
       <c r="A2" s="38" t="s">
         <v>46</v>
       </c>
@@ -7275,121 +7069,40 @@
         <v>48</v>
       </c>
       <c r="F2" s="39" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="G2" s="39" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="H2" s="39" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="I2" s="39" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J2" s="39" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K2" s="39" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="L2" s="39" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="M2" s="39" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="N2" s="39" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O2" s="39" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="P2" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q2" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="R2" s="39" t="s">
-        <v>47</v>
-      </c>
-      <c r="S2" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="T2" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="U2" s="39" t="s">
-        <v>48</v>
-      </c>
-      <c r="V2" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="W2" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="X2" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y2" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="Z2" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA2" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB2" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC2" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD2" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE2" s="44" t="s">
-        <v>49</v>
-      </c>
-      <c r="AF2" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG2" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="AH2" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI2" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="AJ2" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="AK2" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="AL2" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="AM2" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="AN2" s="44" t="s">
-        <v>47</v>
-      </c>
-      <c r="AO2" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="AP2" s="44" t="s">
-        <v>48</v>
-      </c>
-      <c r="AQ2" s="44" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" s="34" customFormat="1" spans="1:43">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" s="34" customFormat="1" spans="1:16">
       <c r="A3" s="38" t="s">
         <v>51</v>
       </c>
@@ -7409,7 +7122,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" s="39">
         <v>0</v>
@@ -7421,7 +7134,7 @@
         <v>0</v>
       </c>
       <c r="K3" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="39">
         <v>0</v>
@@ -7433,94 +7146,13 @@
         <v>0</v>
       </c>
       <c r="O3" s="39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P3" s="39">
         <v>0</v>
       </c>
-      <c r="Q3" s="39">
-        <v>0</v>
-      </c>
-      <c r="R3" s="39">
-        <v>0</v>
-      </c>
-      <c r="S3" s="39">
-        <v>0</v>
-      </c>
-      <c r="T3" s="39">
-        <v>0</v>
-      </c>
-      <c r="U3" s="39">
-        <v>0</v>
-      </c>
-      <c r="V3" s="45">
-        <v>0</v>
-      </c>
-      <c r="W3" s="45">
-        <v>0</v>
-      </c>
-      <c r="X3" s="45">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="44">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="45">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="45">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="45">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="45">
-        <v>0</v>
-      </c>
-      <c r="AL3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="44">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="44">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" s="34" customFormat="1" spans="1:43">
+    </row>
+    <row r="4" s="34" customFormat="1" spans="1:16">
       <c r="A4" s="38" t="s">
         <v>52</v>
       </c>
@@ -7569,89 +7201,8 @@
       <c r="P4" s="39">
         <v>1</v>
       </c>
-      <c r="Q4" s="39">
-        <v>1</v>
-      </c>
-      <c r="R4" s="39">
-        <v>1</v>
-      </c>
-      <c r="S4" s="39">
-        <v>1</v>
-      </c>
-      <c r="T4" s="39">
-        <v>1</v>
-      </c>
-      <c r="U4" s="39">
-        <v>1</v>
-      </c>
-      <c r="V4" s="44">
-        <v>1</v>
-      </c>
-      <c r="W4" s="44">
-        <v>1</v>
-      </c>
-      <c r="X4" s="44">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="44">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AB4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AC4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AD4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AE4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AF4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AG4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AH4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AI4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AJ4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AK4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AL4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AM4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AN4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AO4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AP4" s="44">
-        <v>1</v>
-      </c>
-      <c r="AQ4" s="44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" s="34" customFormat="1" spans="1:43">
+    </row>
+    <row r="5" s="34" customFormat="1" spans="1:16">
       <c r="A5" s="38" t="s">
         <v>53</v>
       </c>
@@ -7667,19 +7218,19 @@
       <c r="E5" s="40">
         <v>0</v>
       </c>
-      <c r="F5" s="39">
-        <v>0</v>
-      </c>
-      <c r="G5" s="39">
-        <v>0</v>
-      </c>
-      <c r="H5" s="39">
-        <v>0</v>
-      </c>
-      <c r="I5" s="39">
-        <v>0</v>
-      </c>
-      <c r="J5" s="39">
+      <c r="F5" s="40">
+        <v>0</v>
+      </c>
+      <c r="G5" s="40">
+        <v>0</v>
+      </c>
+      <c r="H5" s="40">
+        <v>0</v>
+      </c>
+      <c r="I5" s="40">
+        <v>0</v>
+      </c>
+      <c r="J5" s="40">
         <v>0</v>
       </c>
       <c r="K5" s="40">
@@ -7700,89 +7251,8 @@
       <c r="P5" s="40">
         <v>0</v>
       </c>
-      <c r="Q5" s="40">
-        <v>0</v>
-      </c>
-      <c r="R5" s="40">
-        <v>0</v>
-      </c>
-      <c r="S5" s="40">
-        <v>0</v>
-      </c>
-      <c r="T5" s="40">
-        <v>0</v>
-      </c>
-      <c r="U5" s="40">
-        <v>0</v>
-      </c>
-      <c r="V5" s="45">
-        <v>0</v>
-      </c>
-      <c r="W5" s="45">
-        <v>0</v>
-      </c>
-      <c r="X5" s="45">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="45">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AE5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AF5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AG5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AH5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AI5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AJ5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AK5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AL5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AM5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AN5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AO5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AP5" s="45">
-        <v>0</v>
-      </c>
-      <c r="AQ5" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" s="34" customFormat="1" spans="1:43">
+    </row>
+    <row r="6" s="34" customFormat="1" spans="1:16">
       <c r="A6" s="38" t="s">
         <v>54</v>
       </c>
@@ -7798,20 +7268,20 @@
       <c r="E6" s="39">
         <v>1</v>
       </c>
-      <c r="F6" s="39">
-        <v>1</v>
-      </c>
-      <c r="G6" s="39">
-        <v>0</v>
-      </c>
-      <c r="H6" s="39">
-        <v>0</v>
-      </c>
-      <c r="I6" s="39">
-        <v>0</v>
-      </c>
-      <c r="J6" s="39">
-        <v>0</v>
+      <c r="F6" s="40">
+        <v>1</v>
+      </c>
+      <c r="G6" s="40">
+        <v>1</v>
+      </c>
+      <c r="H6" s="40">
+        <v>1</v>
+      </c>
+      <c r="I6" s="40">
+        <v>1</v>
+      </c>
+      <c r="J6" s="40">
+        <v>1</v>
       </c>
       <c r="K6" s="40">
         <v>1</v>
@@ -7831,89 +7301,8 @@
       <c r="P6" s="40">
         <v>1</v>
       </c>
-      <c r="Q6" s="40">
-        <v>1</v>
-      </c>
-      <c r="R6" s="40">
-        <v>1</v>
-      </c>
-      <c r="S6" s="40">
-        <v>1</v>
-      </c>
-      <c r="T6" s="40">
-        <v>1</v>
-      </c>
-      <c r="U6" s="40">
-        <v>1</v>
-      </c>
-      <c r="V6" s="45">
-        <v>0</v>
-      </c>
-      <c r="W6" s="45">
-        <v>0</v>
-      </c>
-      <c r="X6" s="45">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="45">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AB6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AC6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AD6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AE6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AF6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AG6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AI6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AJ6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AK6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AL6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AM6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AN6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AO6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AP6" s="45">
-        <v>0</v>
-      </c>
-      <c r="AQ6" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" s="27" customFormat="1" spans="1:43">
+    </row>
+    <row r="7" s="27" customFormat="1" spans="1:16">
       <c r="A7" s="31" t="s">
         <v>55</v>
       </c>
@@ -7962,89 +7351,8 @@
       <c r="P7" s="40">
         <v>0</v>
       </c>
-      <c r="Q7" s="40">
-        <v>0</v>
-      </c>
-      <c r="R7" s="40">
-        <v>0</v>
-      </c>
-      <c r="S7" s="40">
-        <v>0</v>
-      </c>
-      <c r="T7" s="40">
-        <v>0</v>
-      </c>
-      <c r="U7" s="40">
-        <v>0</v>
-      </c>
-      <c r="V7" s="45">
-        <v>0</v>
-      </c>
-      <c r="W7" s="45">
-        <v>0</v>
-      </c>
-      <c r="X7" s="45">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="45">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AD7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AE7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AF7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AG7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AH7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AI7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AJ7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AK7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AL7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AM7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AN7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AO7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AP7" s="45">
-        <v>0</v>
-      </c>
-      <c r="AQ7" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" s="27" customFormat="1" spans="1:43">
+    </row>
+    <row r="8" s="27" customFormat="1" spans="1:16">
       <c r="A8" s="31" t="s">
         <v>56</v>
       </c>
@@ -8093,89 +7401,8 @@
       <c r="P8" s="40">
         <v>0</v>
       </c>
-      <c r="Q8" s="40">
-        <v>0</v>
-      </c>
-      <c r="R8" s="40">
-        <v>0</v>
-      </c>
-      <c r="S8" s="40">
-        <v>0</v>
-      </c>
-      <c r="T8" s="40">
-        <v>0</v>
-      </c>
-      <c r="U8" s="40">
-        <v>0</v>
-      </c>
-      <c r="V8" s="45">
-        <v>0</v>
-      </c>
-      <c r="W8" s="45">
-        <v>0</v>
-      </c>
-      <c r="X8" s="45">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="45">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AD8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AE8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AF8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AG8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AH8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AI8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AJ8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AK8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AL8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AM8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AN8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AO8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AP8" s="45">
-        <v>0</v>
-      </c>
-      <c r="AQ8" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" s="27" customFormat="1" spans="1:43">
+    </row>
+    <row r="9" s="27" customFormat="1" spans="1:16">
       <c r="A9" s="31" t="s">
         <v>57</v>
       </c>
@@ -8224,89 +7451,8 @@
       <c r="P9" s="40">
         <v>0</v>
       </c>
-      <c r="Q9" s="40">
-        <v>0</v>
-      </c>
-      <c r="R9" s="40">
-        <v>0</v>
-      </c>
-      <c r="S9" s="40">
-        <v>0</v>
-      </c>
-      <c r="T9" s="40">
-        <v>0</v>
-      </c>
-      <c r="U9" s="40">
-        <v>0</v>
-      </c>
-      <c r="V9" s="45">
-        <v>0</v>
-      </c>
-      <c r="W9" s="45">
-        <v>0</v>
-      </c>
-      <c r="X9" s="45">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="45">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AD9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AE9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AF9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AG9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AI9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AJ9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AK9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AL9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AM9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AN9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AO9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AP9" s="45">
-        <v>0</v>
-      </c>
-      <c r="AQ9" s="45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" s="35" customFormat="1" ht="27.75" spans="1:43">
+    </row>
+    <row r="10" s="35" customFormat="1" ht="27.75" spans="1:16">
       <c r="A10" s="41" t="s">
         <v>58</v>
       </c>
@@ -8320,110 +7466,45 @@
         <v>152</v>
       </c>
       <c r="E10" s="42" t="s">
-        <v>194</v>
-      </c>
-      <c r="F10" s="43"/>
-      <c r="G10" s="43"/>
-      <c r="H10" s="43"/>
-      <c r="I10" s="43"/>
-      <c r="J10" s="43"/>
+        <v>167</v>
+      </c>
+      <c r="F10" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="G10" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="H10" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="I10" s="42" t="s">
+        <v>168</v>
+      </c>
+      <c r="J10" s="42" t="s">
+        <v>168</v>
+      </c>
       <c r="K10" s="42" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="L10" s="42" t="s">
-        <v>195</v>
+        <v>168</v>
       </c>
       <c r="M10" s="42" t="s">
-        <v>196</v>
+        <v>168</v>
       </c>
       <c r="N10" s="42" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
       <c r="O10" s="42" t="s">
-        <v>198</v>
+        <v>168</v>
       </c>
       <c r="P10" s="42" t="s">
-        <v>198</v>
-      </c>
-      <c r="Q10" s="42" t="s">
-        <v>198</v>
-      </c>
-      <c r="R10" s="42" t="s">
-        <v>198</v>
-      </c>
-      <c r="S10" s="42" t="s">
-        <v>198</v>
-      </c>
-      <c r="T10" s="42" t="s">
-        <v>198</v>
-      </c>
-      <c r="U10" s="42" t="s">
-        <v>198</v>
-      </c>
-      <c r="V10" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="W10" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="X10" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="Y10" s="46" t="s">
-        <v>199</v>
-      </c>
-      <c r="Z10" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="AA10" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="AB10" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="AC10" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="AD10" s="47" t="s">
-        <v>180</v>
-      </c>
-      <c r="AE10" s="46" t="s">
-        <v>200</v>
-      </c>
-      <c r="AF10" s="47"/>
-      <c r="AG10" s="47"/>
-      <c r="AH10" s="47"/>
-      <c r="AI10" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="AJ10" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="AK10" s="46" t="s">
-        <v>152</v>
-      </c>
-      <c r="AL10" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="AM10" s="46" t="s">
-        <v>196</v>
-      </c>
-      <c r="AN10" s="46" t="s">
-        <v>197</v>
-      </c>
-      <c r="AO10" s="46" t="s">
-        <v>195</v>
-      </c>
-      <c r="AP10" s="46" t="s">
-        <v>196</v>
-      </c>
-      <c r="AQ10" s="46" t="s">
-        <v>197</v>
+        <v>168</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5 C5 D5 E5 K5:U5 V5 W5 X5 Y5:AD5 AE5 AF5:AH5 AI5:AK5 AL5:AQ5 K6:U6 AH6 AJ6 AK6 F7:F9 I7:I9 J7:J9 V7:V9 W7:W9 X7:X9 AE7:AE9 G7:H9 K7:U9 Y7:AD9 AF7:AH9 AL7:AQ9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B5 C5 D5 E5 F5 G5 H5:J5 K5:P5 F6 G6 H6:J6 K6:P6 F7:F9 G7:G9 H7:J9 K7:P9">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>
@@ -8467,55 +7548,55 @@
         <v>0</v>
       </c>
       <c r="B1" s="26" t="s">
-        <v>201</v>
+        <v>169</v>
       </c>
       <c r="C1" s="26" t="s">
-        <v>202</v>
+        <v>170</v>
       </c>
       <c r="D1" s="26" t="s">
-        <v>203</v>
+        <v>171</v>
       </c>
       <c r="E1" s="26" t="s">
-        <v>204</v>
+        <v>172</v>
       </c>
       <c r="F1" s="26" t="s">
-        <v>205</v>
+        <v>173</v>
       </c>
       <c r="G1" s="26" t="s">
-        <v>206</v>
+        <v>174</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>207</v>
+        <v>175</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>208</v>
+        <v>176</v>
       </c>
       <c r="J1" s="26" t="s">
-        <v>209</v>
+        <v>177</v>
       </c>
       <c r="K1" s="26" t="s">
-        <v>210</v>
+        <v>178</v>
       </c>
       <c r="L1" s="26" t="s">
-        <v>211</v>
+        <v>179</v>
       </c>
       <c r="M1" s="26" t="s">
-        <v>212</v>
+        <v>180</v>
       </c>
       <c r="N1" s="26" t="s">
-        <v>213</v>
+        <v>181</v>
       </c>
       <c r="O1" s="26" t="s">
-        <v>214</v>
+        <v>182</v>
       </c>
       <c r="P1" s="26" t="s">
-        <v>215</v>
+        <v>183</v>
       </c>
       <c r="Q1" s="26" t="s">
-        <v>216</v>
+        <v>184</v>
       </c>
       <c r="R1" s="26" t="s">
-        <v>217</v>
+        <v>185</v>
       </c>
     </row>
     <row r="2" s="7" customFormat="1" ht="15" spans="1:18">
@@ -8971,55 +8052,55 @@
         <v>58</v>
       </c>
       <c r="B10" s="28" t="s">
-        <v>218</v>
+        <v>186</v>
       </c>
       <c r="C10" s="28" t="s">
-        <v>219</v>
+        <v>187</v>
       </c>
       <c r="D10" s="28" t="s">
-        <v>220</v>
+        <v>188</v>
       </c>
       <c r="E10" s="28" t="s">
-        <v>221</v>
+        <v>189</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>222</v>
+        <v>190</v>
       </c>
       <c r="G10" s="28" t="s">
-        <v>223</v>
+        <v>191</v>
       </c>
       <c r="H10" s="28" t="s">
-        <v>224</v>
+        <v>192</v>
       </c>
       <c r="I10" s="28" t="s">
-        <v>225</v>
+        <v>193</v>
       </c>
       <c r="J10" s="28" t="s">
-        <v>226</v>
+        <v>194</v>
       </c>
       <c r="K10" s="28" t="s">
-        <v>227</v>
+        <v>195</v>
       </c>
       <c r="L10" s="28" t="s">
-        <v>228</v>
+        <v>196</v>
       </c>
       <c r="M10" s="28" t="s">
-        <v>229</v>
+        <v>197</v>
       </c>
       <c r="N10" s="28" t="s">
-        <v>230</v>
+        <v>198</v>
       </c>
       <c r="O10" s="28" t="s">
-        <v>231</v>
+        <v>199</v>
       </c>
       <c r="P10" s="28" t="s">
-        <v>232</v>
+        <v>200</v>
       </c>
       <c r="Q10" s="28" t="s">
-        <v>233</v>
+        <v>201</v>
       </c>
       <c r="R10" s="28" t="s">
-        <v>234</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -9079,12 +8160,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>235</v>
+        <v>203</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B2" s="3">
         <v>15</v>
@@ -9092,7 +8173,7 @@
     </row>
     <row r="3" s="3" customFormat="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="B3" s="3">
         <v>32</v>
@@ -9148,7 +8229,7 @@
     </row>
     <row r="10" s="3" customFormat="1" spans="1:2">
       <c r="A10" s="3" t="s">
-        <v>238</v>
+        <v>206</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -9355,7 +8436,7 @@
         <v>58</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>239</v>
+        <v>207</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -9421,7 +8502,7 @@
   <sheetPr/>
   <dimension ref="A1:AF26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
@@ -9462,12 +8543,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>240</v>
+        <v>208</v>
       </c>
     </row>
     <row r="2" s="3" customFormat="1" spans="1:2">
       <c r="A2" s="3" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B2" s="3">
         <v>64</v>
@@ -9475,7 +8556,7 @@
     </row>
     <row r="3" s="3" customFormat="1" spans="1:2">
       <c r="A3" s="3" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="B3" s="3">
         <v>13</v>
@@ -9539,43 +8620,43 @@
     </row>
     <row r="11" s="3" customFormat="1" spans="1:14">
       <c r="A11" s="4" t="s">
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>242</v>
+        <v>210</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>243</v>
+        <v>211</v>
       </c>
       <c r="D11" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>244</v>
+        <v>212</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>245</v>
+        <v>213</v>
       </c>
       <c r="G11" s="4" t="s">
         <v>13</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>246</v>
+        <v>214</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>247</v>
+        <v>215</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>248</v>
+        <v>216</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>249</v>
+        <v>217</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>250</v>
+        <v>218</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>251</v>
+        <v>219</v>
       </c>
       <c r="N11" s="4"/>
     </row>
@@ -9651,12 +8732,12 @@
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>252</v>
+        <v>220</v>
       </c>
     </row>
     <row r="15" s="3" customFormat="1" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B15" s="3">
         <v>64</v>
@@ -9664,7 +8745,7 @@
     </row>
     <row r="16" s="3" customFormat="1" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="B16" s="3">
         <v>32</v>
@@ -9927,7 +9008,7 @@
         <v>58</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>253</v>
+        <v>221</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -10012,7 +9093,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>254</v>
+        <v>222</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -10038,7 +9119,7 @@
     </row>
     <row r="2" s="23" customFormat="1" spans="1:23">
       <c r="A2" s="3" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B2" s="3">
         <v>256</v>
@@ -10067,7 +9148,7 @@
     </row>
     <row r="3" s="23" customFormat="1" spans="1:23">
       <c r="A3" s="3" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="B3" s="3">
         <v>23</v>
@@ -10257,73 +9338,73 @@
     </row>
     <row r="11" s="23" customFormat="1" spans="1:23">
       <c r="A11" s="4" t="s">
+        <v>209</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="C11" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>227</v>
+      </c>
+      <c r="H11" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="I11" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="J11" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>231</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>233</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="O11" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="P11" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="Q11" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="R11" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="S11" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="T11" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="U11" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>255</v>
-      </c>
-      <c r="C11" s="4" t="s">
+      <c r="V11" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>256</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>257</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>258</v>
-      </c>
-      <c r="G11" s="4" t="s">
-        <v>259</v>
-      </c>
-      <c r="H11" s="4" t="s">
-        <v>260</v>
-      </c>
-      <c r="I11" s="4" t="s">
-        <v>261</v>
-      </c>
-      <c r="J11" s="4" t="s">
-        <v>262</v>
-      </c>
-      <c r="K11" s="4" t="s">
-        <v>263</v>
-      </c>
-      <c r="L11" s="4" t="s">
-        <v>264</v>
-      </c>
-      <c r="M11" s="4" t="s">
-        <v>265</v>
-      </c>
-      <c r="N11" s="4" t="s">
-        <v>266</v>
-      </c>
-      <c r="O11" s="4" t="s">
-        <v>267</v>
-      </c>
-      <c r="P11" s="4" t="s">
-        <v>268</v>
-      </c>
-      <c r="Q11" s="4" t="s">
-        <v>269</v>
-      </c>
-      <c r="R11" s="4" t="s">
-        <v>270</v>
-      </c>
-      <c r="S11" s="4" t="s">
-        <v>271</v>
-      </c>
-      <c r="T11" s="4" t="s">
-        <v>272</v>
-      </c>
-      <c r="U11" s="4" t="s">
-        <v>273</v>
-      </c>
-      <c r="V11" s="4" t="s">
-        <v>274</v>
-      </c>
       <c r="W11" s="4" t="s">
-        <v>275</v>
+        <v>243</v>
       </c>
     </row>
     <row r="12" s="23" customFormat="1" spans="1:23">
@@ -10402,7 +9483,7 @@
         <v>58</v>
       </c>
       <c r="B13" s="25" t="s">
-        <v>276</v>
+        <v>244</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
@@ -10431,7 +9512,7 @@
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>277</v>
+        <v>245</v>
       </c>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
@@ -10457,7 +9538,7 @@
     </row>
     <row r="15" s="24" customFormat="1" spans="1:23">
       <c r="A15" s="3" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B15" s="3">
         <v>512</v>
@@ -10486,7 +9567,7 @@
     </row>
     <row r="16" s="24" customFormat="1" spans="1:23">
       <c r="A16" s="3" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="B16" s="3">
         <v>5</v>
@@ -10676,19 +9757,19 @@
     </row>
     <row r="24" s="24" customFormat="1" spans="1:5">
       <c r="A24" s="4" t="s">
-        <v>242</v>
+        <v>210</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>278</v>
+        <v>246</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>279</v>
+        <v>247</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>256</v>
+        <v>224</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>257</v>
+        <v>225</v>
       </c>
     </row>
     <row r="25" s="24" customFormat="1" spans="1:5">
@@ -10713,7 +9794,7 @@
         <v>58</v>
       </c>
       <c r="B26" s="25" t="s">
-        <v>276</v>
+        <v>244</v>
       </c>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
@@ -10742,7 +9823,7 @@
         <v>0</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>280</v>
+        <v>248</v>
       </c>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
@@ -10765,7 +9846,7 @@
     </row>
     <row r="28" s="24" customFormat="1" spans="1:20">
       <c r="A28" s="3" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B28" s="3">
         <v>8</v>
@@ -10791,7 +9872,7 @@
     </row>
     <row r="29" s="24" customFormat="1" spans="1:20">
       <c r="A29" s="3" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="B29" s="3">
         <v>2</v>
@@ -10963,10 +10044,10 @@
     </row>
     <row r="37" s="24" customFormat="1" spans="1:2">
       <c r="A37" s="4" t="s">
-        <v>242</v>
+        <v>210</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>278</v>
+        <v>246</v>
       </c>
     </row>
     <row r="38" s="24" customFormat="1" spans="1:2">
@@ -10982,7 +10063,7 @@
         <v>58</v>
       </c>
       <c r="B39" s="25" t="s">
-        <v>276</v>
+        <v>244</v>
       </c>
       <c r="C39" s="3"/>
       <c r="D39" s="3"/>
@@ -11008,7 +10089,7 @@
         <v>0</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>281</v>
+        <v>249</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
@@ -11034,7 +10115,7 @@
     </row>
     <row r="41" s="24" customFormat="1" spans="1:23">
       <c r="A41" s="3" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B41" s="3">
         <v>128</v>
@@ -11063,7 +10144,7 @@
     </row>
     <row r="42" s="24" customFormat="1" spans="1:23">
       <c r="A42" s="3" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="B42" s="3">
         <v>4</v>
@@ -11253,16 +10334,16 @@
     </row>
     <row r="50" s="24" customFormat="1" spans="1:4">
       <c r="A50" s="4" t="s">
-        <v>241</v>
+        <v>209</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>242</v>
+        <v>210</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>278</v>
+        <v>246</v>
       </c>
       <c r="D50" s="25" t="s">
-        <v>282</v>
+        <v>250</v>
       </c>
     </row>
     <row r="51" s="24" customFormat="1" spans="1:4">
@@ -11354,12 +10435,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>283</v>
+        <v>251</v>
       </c>
     </row>
     <row r="2" s="11" customFormat="1" spans="1:2">
       <c r="A2" s="14" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B2" s="14">
         <v>512</v>
@@ -11367,7 +10448,7 @@
     </row>
     <row r="3" s="11" customFormat="1" spans="1:2">
       <c r="A3" s="14" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="B3" s="14">
         <v>4</v>
@@ -11423,7 +10504,7 @@
     </row>
     <row r="10" s="11" customFormat="1" spans="1:2">
       <c r="A10" s="14" t="s">
-        <v>284</v>
+        <v>252</v>
       </c>
       <c r="B10" s="14">
         <v>0</v>
@@ -11431,16 +10512,16 @@
     </row>
     <row r="11" s="11" customFormat="1" spans="1:4">
       <c r="A11" s="19" t="s">
-        <v>285</v>
+        <v>253</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>286</v>
+        <v>254</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>287</v>
+        <v>255</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>288</v>
+        <v>256</v>
       </c>
     </row>
     <row r="12" s="11" customFormat="1" spans="1:4">
@@ -11520,12 +10601,12 @@
         <v>0</v>
       </c>
       <c r="B1" s="13" t="s">
-        <v>289</v>
+        <v>257</v>
       </c>
     </row>
     <row r="2" s="11" customFormat="1" spans="1:2">
       <c r="A2" s="14" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B2" s="14">
         <v>10</v>
@@ -11533,7 +10614,7 @@
     </row>
     <row r="3" s="11" customFormat="1" spans="1:2">
       <c r="A3" s="14" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="B3" s="14">
         <v>20</v>
@@ -11589,7 +10670,7 @@
     </row>
     <row r="10" s="11" customFormat="1" ht="14.25" spans="1:2">
       <c r="A10" s="14" t="s">
-        <v>284</v>
+        <v>252</v>
       </c>
       <c r="B10" s="14">
         <v>0</v>
@@ -11597,43 +10678,43 @@
     </row>
     <row r="11" s="11" customFormat="1" ht="30" spans="1:20">
       <c r="A11" s="15" t="s">
-        <v>290</v>
+        <v>258</v>
       </c>
       <c r="B11" s="16" t="s">
-        <v>291</v>
+        <v>259</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>292</v>
+        <v>260</v>
       </c>
       <c r="D11" s="16" t="s">
-        <v>293</v>
+        <v>261</v>
       </c>
       <c r="E11" s="16" t="s">
-        <v>294</v>
+        <v>262</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>295</v>
+        <v>263</v>
       </c>
       <c r="G11" s="16" t="s">
-        <v>296</v>
+        <v>264</v>
       </c>
       <c r="H11" s="16" t="s">
-        <v>297</v>
+        <v>265</v>
       </c>
       <c r="I11" s="16" t="s">
-        <v>298</v>
+        <v>266</v>
       </c>
       <c r="J11" s="16" t="s">
-        <v>299</v>
+        <v>267</v>
       </c>
       <c r="K11" s="16" t="s">
-        <v>300</v>
+        <v>268</v>
       </c>
       <c r="L11" s="16" t="s">
-        <v>301</v>
+        <v>269</v>
       </c>
       <c r="M11" s="16" t="s">
-        <v>302</v>
+        <v>270</v>
       </c>
       <c r="N11" s="16" t="s">
         <v>16</v>
@@ -11642,19 +10723,19 @@
         <v>17</v>
       </c>
       <c r="P11" s="16" t="s">
-        <v>303</v>
+        <v>271</v>
       </c>
       <c r="Q11" s="16" t="s">
-        <v>304</v>
+        <v>272</v>
       </c>
       <c r="R11" s="16" t="s">
-        <v>305</v>
+        <v>273</v>
       </c>
       <c r="S11" s="16" t="s">
-        <v>306</v>
+        <v>274</v>
       </c>
       <c r="T11" s="16" t="s">
-        <v>307</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" s="11" customFormat="1" ht="15" spans="1:20">
@@ -11786,12 +10867,12 @@
         <v>0</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>308</v>
+        <v>276</v>
       </c>
     </row>
     <row r="15" s="11" customFormat="1" spans="1:2">
       <c r="A15" s="14" t="s">
-        <v>236</v>
+        <v>204</v>
       </c>
       <c r="B15" s="14">
         <v>100</v>
@@ -11799,7 +10880,7 @@
     </row>
     <row r="16" s="11" customFormat="1" spans="1:2">
       <c r="A16" s="14" t="s">
-        <v>237</v>
+        <v>205</v>
       </c>
       <c r="B16" s="14">
         <v>2</v>
@@ -11855,7 +10936,7 @@
     </row>
     <row r="23" s="11" customFormat="1" ht="14.25" spans="1:2">
       <c r="A23" s="14" t="s">
-        <v>284</v>
+        <v>252</v>
       </c>
       <c r="B23" s="14">
         <v>0</v>
@@ -11863,10 +10944,10 @@
     </row>
     <row r="24" s="11" customFormat="1" ht="15" spans="1:3">
       <c r="A24" s="15" t="s">
-        <v>309</v>
+        <v>277</v>
       </c>
       <c r="B24" s="16" t="s">
-        <v>310</v>
+        <v>278</v>
       </c>
       <c r="C24" s="3"/>
     </row>

</xml_diff>

<commit_message>
ad battle point field for players
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Player.xlsx
+++ b/_Out/NFDataCfg/Excel/Player.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowHeight="23360" activeTab="2"/>
+    <workbookView windowHeight="23360"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100">
   <si>
     <t>Id</t>
   </si>
@@ -159,6 +159,9 @@
     <t>Gold</t>
   </si>
   <si>
+    <t>BattlePoint</t>
+  </si>
+  <si>
     <t>Diamond</t>
   </si>
   <si>
@@ -376,6 +379,12 @@
   </si>
   <si>
     <t>Stone4</t>
+  </si>
+  <si>
+    <t>Lock</t>
+  </si>
+  <si>
+    <t>Future</t>
   </si>
   <si>
     <t>UserData</t>
@@ -425,10 +434,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -460,9 +469,31 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -491,22 +522,15 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -528,37 +552,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
@@ -567,8 +560,46 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -583,29 +614,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -644,7 +653,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -656,61 +803,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -722,109 +827,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -969,6 +978,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1017,21 +1041,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1049,15 +1058,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -1066,153 +1066,162 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="14" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1280,6 +1289,9 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1287,9 +1299,6 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1704,12 +1713,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AA10"/>
+  <dimension ref="A1:AB10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="T2" sqref="T2"/>
+      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1718,17 +1727,17 @@
     <col min="2" max="2" width="10.4615384615385" customWidth="1"/>
     <col min="4" max="4" width="11.6634615384615" customWidth="1"/>
     <col min="5" max="5" width="9.33653846153846" customWidth="1"/>
-    <col min="13" max="13" width="11.3365384615385" customWidth="1"/>
-    <col min="14" max="14" width="10.7307692307692" customWidth="1"/>
-    <col min="15" max="15" width="13.6634615384615" customWidth="1"/>
-    <col min="16" max="16" width="10.3365384615385" customWidth="1"/>
-    <col min="17" max="17" width="17.1346153846154" customWidth="1"/>
-    <col min="18" max="18" width="12.3365384615385" customWidth="1"/>
-    <col min="23" max="23" width="18.3365384615385" customWidth="1"/>
-    <col min="24" max="27" width="17.3365384615385" customWidth="1"/>
+    <col min="14" max="14" width="11.3365384615385" customWidth="1"/>
+    <col min="15" max="15" width="10.7307692307692" customWidth="1"/>
+    <col min="16" max="16" width="13.6634615384615" customWidth="1"/>
+    <col min="17" max="17" width="10.3365384615385" customWidth="1"/>
+    <col min="18" max="18" width="17.1346153846154" customWidth="1"/>
+    <col min="19" max="19" width="12.3365384615385" customWidth="1"/>
+    <col min="24" max="24" width="18.3365384615385" customWidth="1"/>
+    <col min="25" max="28" width="17.3365384615385" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="1" ht="17" spans="1:27">
+    <row r="1" s="11" customFormat="1" ht="17" spans="1:28">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1798,105 +1807,111 @@
       <c r="W1" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="20" t="s">
+      <c r="X1" s="15" t="s">
         <v>23</v>
       </c>
       <c r="Y1" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="24" t="s">
+      <c r="Z1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="24" t="s">
+      <c r="AA1" s="21" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="2" s="12" customFormat="1" spans="1:27">
+      <c r="AB1" s="21" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" s="12" customFormat="1" spans="1:28">
       <c r="A2" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>29</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>28</v>
-      </c>
       <c r="P2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="W2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="X2" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="Y2" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="Z2" s="21" t="s">
-        <v>29</v>
-      </c>
-      <c r="AA2" s="21" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" s="12" customFormat="1" spans="1:27">
+      <c r="X2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="Y2" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z2" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="AA2" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB2" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" s="12" customFormat="1" spans="1:28">
       <c r="A3" s="16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -1949,11 +1964,11 @@
       <c r="R3" s="8">
         <v>0</v>
       </c>
-      <c r="S3" s="3">
-        <v>1</v>
+      <c r="S3" s="8">
+        <v>0</v>
       </c>
       <c r="T3" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U3" s="3">
         <v>0</v>
@@ -1961,25 +1976,28 @@
       <c r="V3" s="3">
         <v>0</v>
       </c>
-      <c r="W3" s="8">
-        <v>0</v>
-      </c>
-      <c r="X3" s="21">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="21">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="21">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="21">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" s="12" customFormat="1" spans="1:27">
+      <c r="W3" s="3">
+        <v>0</v>
+      </c>
+      <c r="X3" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="22">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="22">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="22">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" s="12" customFormat="1" spans="1:28">
       <c r="A4" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -2036,7 +2054,7 @@
         <v>1</v>
       </c>
       <c r="T4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U4" s="3">
         <v>0</v>
@@ -2045,24 +2063,27 @@
         <v>0</v>
       </c>
       <c r="W4" s="3">
-        <v>1</v>
-      </c>
-      <c r="X4" s="21">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="21">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="21">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" s="12" customFormat="1" spans="1:27">
+        <v>0</v>
+      </c>
+      <c r="X4" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y4" s="22">
+        <v>1</v>
+      </c>
+      <c r="Z4" s="22">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="22">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" s="12" customFormat="1" spans="1:28">
       <c r="A5" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" s="8">
         <v>0</v>
@@ -2130,22 +2151,25 @@
       <c r="W5" s="8">
         <v>0</v>
       </c>
-      <c r="X5" s="22">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="22">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="22">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" s="12" customFormat="1" spans="1:27">
+      <c r="X5" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="23">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="23">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" s="12" customFormat="1" spans="1:28">
       <c r="A6" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
@@ -2202,7 +2226,7 @@
         <v>1</v>
       </c>
       <c r="T6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6" s="3">
         <v>0</v>
@@ -2211,24 +2235,27 @@
         <v>0</v>
       </c>
       <c r="W6" s="3">
-        <v>1</v>
-      </c>
-      <c r="X6" s="22">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="22">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="22">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" s="8" customFormat="1" ht="17" spans="1:27">
+        <v>0</v>
+      </c>
+      <c r="X6" s="3">
+        <v>1</v>
+      </c>
+      <c r="Y6" s="23">
+        <v>1</v>
+      </c>
+      <c r="Z6" s="23">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="23">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" s="8" customFormat="1" ht="17" spans="1:28">
       <c r="A7" s="17" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -2296,22 +2323,25 @@
       <c r="W7" s="8">
         <v>0</v>
       </c>
-      <c r="X7" s="22">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="22">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="22">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" s="8" customFormat="1" ht="17" spans="1:27">
+      <c r="X7" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="23">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="23">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" s="8" customFormat="1" ht="17" spans="1:28">
       <c r="A8" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -2379,22 +2409,25 @@
       <c r="W8" s="8">
         <v>0</v>
       </c>
-      <c r="X8" s="22">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="22">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="22">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" s="8" customFormat="1" ht="17" spans="1:27">
+      <c r="X8" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="23">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="23">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" s="8" customFormat="1" ht="17" spans="1:28">
       <c r="A9" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9" s="8">
         <v>0</v>
@@ -2462,53 +2495,54 @@
       <c r="W9" s="8">
         <v>0</v>
       </c>
-      <c r="X9" s="22">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="22">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="22">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" s="13" customFormat="1" ht="101.75" spans="1:27">
+      <c r="X9" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="23">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="23">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="23">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" s="13" customFormat="1" ht="101.75" spans="1:28">
       <c r="A10" s="18" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>47</v>
-      </c>
-      <c r="K10" s="19" t="s">
         <v>48</v>
       </c>
+      <c r="K10" s="19"/>
       <c r="L10" s="19" t="s">
         <v>49</v>
       </c>
@@ -2537,7 +2571,7 @@
         <v>57</v>
       </c>
       <c r="U10" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="V10" s="19" t="s">
         <v>58</v>
@@ -2545,22 +2579,25 @@
       <c r="W10" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="X10" s="23" t="s">
+      <c r="X10" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="Y10" s="23" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z10" s="23" t="s">
+      <c r="Y10" s="24" t="s">
         <v>61</v>
       </c>
-      <c r="AA10" s="23" t="s">
+      <c r="Z10" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="AA10" s="24" t="s">
         <v>62</v>
+      </c>
+      <c r="AB10" s="24" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 H3:R3 B5:S5 T5 U5:AA5 T7:T9 B7:S9 X6:AA9 U7:V9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 H3:J3 K3 L3:S3 B5:J5 K5 L5:T5 U5 V5:AB5 K7:K9 U7:U9 B7:J9 L7:T9 Y6:AB9 V7:W9">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>
@@ -2589,30 +2626,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="10" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2633,10 +2670,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:L26"/>
+  <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -2647,7 +2684,7 @@
     <col min="4" max="5" width="20.2307692307692" customWidth="1"/>
     <col min="6" max="6" width="14.5384615384615" customWidth="1"/>
     <col min="7" max="7" width="10.3076923076923" customWidth="1"/>
-    <col min="12" max="12" width="10.2307692307692" customWidth="1"/>
+    <col min="12" max="14" width="10.2307692307692" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" s="6" customFormat="1" spans="1:6">
@@ -2655,7 +2692,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2664,7 +2701,7 @@
     </row>
     <row r="2" s="7" customFormat="1" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3">
         <v>256</v>
@@ -2676,10 +2713,10 @@
     </row>
     <row r="3" s="7" customFormat="1" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B3" s="3">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -2688,7 +2725,7 @@
     </row>
     <row r="4" s="7" customFormat="1" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -2700,7 +2737,7 @@
     </row>
     <row r="5" s="7" customFormat="1" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
@@ -2712,7 +2749,7 @@
     </row>
     <row r="6" s="7" customFormat="1" spans="1:6">
       <c r="A6" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -2724,7 +2761,7 @@
     </row>
     <row r="7" s="8" customFormat="1" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -2736,7 +2773,7 @@
     </row>
     <row r="8" s="8" customFormat="1" ht="18" customHeight="1" spans="1:6">
       <c r="A8" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -2748,7 +2785,7 @@
     </row>
     <row r="9" s="8" customFormat="1" ht="18" customHeight="1" spans="1:6">
       <c r="A9" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -2760,7 +2797,7 @@
     </row>
     <row r="10" s="9" customFormat="1" ht="17.55" spans="1:6">
       <c r="A10" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -2770,85 +2807,97 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" customFormat="1" spans="1:12">
+    <row r="11" customFormat="1" spans="1:14">
       <c r="A11" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" customFormat="1" spans="1:12">
+        <v>84</v>
+      </c>
+      <c r="M11" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="N11" s="4" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="12" customFormat="1" spans="1:14">
       <c r="A12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I12" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L12" s="4" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="13" customFormat="1" spans="1:12">
+      <c r="M12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="N12" s="4" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" customFormat="1" spans="1:14">
       <c r="A13" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2861,18 +2910,20 @@
       <c r="J13" s="4"/>
       <c r="K13" s="4"/>
       <c r="L13" s="4"/>
+      <c r="M13" s="4"/>
+      <c r="N13" s="4"/>
     </row>
     <row r="14" customFormat="1" spans="1:2">
       <c r="A14" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
     </row>
     <row r="15" customFormat="1" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B15" s="3">
         <v>512</v>
@@ -2880,7 +2931,7 @@
     </row>
     <row r="16" customFormat="1" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B16" s="3">
         <v>2</v>
@@ -2888,7 +2939,7 @@
     </row>
     <row r="17" customFormat="1" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -2896,7 +2947,7 @@
     </row>
     <row r="18" customFormat="1" spans="1:2">
       <c r="A18" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
@@ -2904,7 +2955,7 @@
     </row>
     <row r="19" customFormat="1" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
@@ -2912,7 +2963,7 @@
     </row>
     <row r="20" customFormat="1" spans="1:2">
       <c r="A20" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
@@ -2920,7 +2971,7 @@
     </row>
     <row r="21" customFormat="1" spans="1:2">
       <c r="A21" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -2928,7 +2979,7 @@
     </row>
     <row r="22" customFormat="1" spans="1:2">
       <c r="A22" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B22" s="3">
         <v>0</v>
@@ -2936,7 +2987,7 @@
     </row>
     <row r="23" customFormat="1" spans="1:2">
       <c r="A23" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B23" s="3">
         <v>0</v>
@@ -2944,23 +2995,23 @@
     </row>
     <row r="24" customFormat="1" spans="1:2">
       <c r="A24" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
     </row>
     <row r="25" customFormat="1" spans="1:2">
       <c r="A25" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>29</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="26" customFormat="1" spans="1:2">
       <c r="A26" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26" s="5"/>
     </row>
@@ -2972,7 +3023,7 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E10 F10 D12 E12 F12 D13 E13 F13 A11:A12 B11:B12 E1:E7 E8:E9 F1:F7 F8:F9 A24:B25">
       <formula1>"int,string,float,object"</formula1>
     </dataValidation>
-    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="D11 E11 F11 G11 H11 I11 J11 K11 L11 H12 I12 J12 K12 L12 C11:C12"/>
+    <dataValidation showInputMessage="1" showErrorMessage="1" sqref="D11 E11 F11 G11 H11 I11 J11 K11 L11 M11 N11 H12 I12 J12 K12 L12 M12 N12 C11:C12"/>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A2:B3 A15:B16">
       <formula1>0</formula1>
     </dataValidation>
@@ -3002,7 +3053,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -3013,7 +3064,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B2" s="3">
         <v>64</v>
@@ -3027,7 +3078,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B3" s="3">
         <v>8</v>
@@ -3041,7 +3092,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -3055,7 +3106,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
@@ -3069,7 +3120,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -3083,7 +3134,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -3097,7 +3148,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -3111,7 +3162,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -3125,7 +3176,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -3139,25 +3190,25 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>6</v>
@@ -3165,33 +3216,33 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
@@ -3206,13 +3257,13 @@
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B15" s="3">
         <v>512</v>
@@ -3221,7 +3272,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B16" s="3">
         <v>3</v>
@@ -3230,7 +3281,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -3239,7 +3290,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
@@ -3248,7 +3299,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
@@ -3257,7 +3308,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
@@ -3266,7 +3317,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -3275,7 +3326,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B22" s="3">
         <v>0</v>
@@ -3284,7 +3335,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B23" s="3">
         <v>0</v>
@@ -3293,29 +3344,29 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="4" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -3351,12 +3402,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix bug for WS module(can't trigger binary network callback function) add new interface named UsedRow() for record code improvement
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Player.xlsx
+++ b/_Out/NFDataCfg/Excel/Player.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowHeight="23360"/>
+    <workbookView windowWidth="30880" windowHeight="13360"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101">
   <si>
     <t>Id</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>NoticeID</t>
+  </si>
+  <si>
+    <t>ClanID</t>
   </si>
   <si>
     <t>GameID</t>
@@ -434,10 +437,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -469,9 +472,15 @@
       <charset val="134"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -485,36 +494,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -523,14 +504,6 @@
     <font>
       <b/>
       <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -546,7 +519,60 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -560,46 +586,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -614,11 +602,26 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="37">
     <fill>
@@ -653,7 +656,169 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -665,175 +830,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -978,35 +981,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1041,6 +1020,32 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1058,11 +1063,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1070,8 +1073,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1080,148 +1083,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="11" borderId="14" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1713,12 +1716,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AB10"/>
+  <dimension ref="A1:AC10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+      <selection pane="bottomLeft" activeCell="V6" sqref="V6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1733,11 +1736,11 @@
     <col min="17" max="17" width="10.3365384615385" customWidth="1"/>
     <col min="18" max="18" width="17.1346153846154" customWidth="1"/>
     <col min="19" max="19" width="12.3365384615385" customWidth="1"/>
-    <col min="24" max="24" width="18.3365384615385" customWidth="1"/>
-    <col min="25" max="28" width="17.3365384615385" customWidth="1"/>
+    <col min="25" max="25" width="18.3365384615385" customWidth="1"/>
+    <col min="26" max="29" width="17.3365384615385" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="1" ht="17" spans="1:28">
+    <row r="1" s="11" customFormat="1" ht="17" spans="1:29">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1810,108 +1813,114 @@
       <c r="X1" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="20" t="s">
+      <c r="Y1" s="15" t="s">
         <v>24</v>
       </c>
       <c r="Z1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="21" t="s">
+      <c r="AA1" s="20" t="s">
         <v>26</v>
       </c>
       <c r="AB1" s="21" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="2" s="12" customFormat="1" spans="1:28">
+      <c r="AC1" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" s="12" customFormat="1" spans="1:29">
       <c r="A2" s="16" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="Q2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="X2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Y2" s="22" t="s">
-        <v>30</v>
+      <c r="Y2" s="3" t="s">
+        <v>31</v>
       </c>
       <c r="Z2" s="22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AA2" s="22" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AB2" s="22" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" s="12" customFormat="1" spans="1:28">
+        <v>31</v>
+      </c>
+      <c r="AC2" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" s="12" customFormat="1" spans="1:29">
       <c r="A3" s="16" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -1979,10 +1988,10 @@
       <c r="W3" s="3">
         <v>0</v>
       </c>
-      <c r="X3" s="8">
-        <v>0</v>
-      </c>
-      <c r="Y3" s="22">
+      <c r="X3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y3" s="8">
         <v>0</v>
       </c>
       <c r="Z3" s="22">
@@ -1994,10 +2003,13 @@
       <c r="AB3" s="22">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" s="12" customFormat="1" spans="1:28">
+      <c r="AC3" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" s="12" customFormat="1" spans="1:29">
       <c r="A4" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -2057,18 +2069,18 @@
         <v>1</v>
       </c>
       <c r="U4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W4" s="3">
         <v>0</v>
       </c>
       <c r="X4" s="3">
-        <v>1</v>
-      </c>
-      <c r="Y4" s="22">
+        <v>0</v>
+      </c>
+      <c r="Y4" s="3">
         <v>1</v>
       </c>
       <c r="Z4" s="22">
@@ -2080,10 +2092,13 @@
       <c r="AB4" s="22">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" s="12" customFormat="1" spans="1:28">
+      <c r="AC4" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" s="12" customFormat="1" spans="1:29">
       <c r="A5" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B5" s="8">
         <v>0</v>
@@ -2154,7 +2169,7 @@
       <c r="X5" s="8">
         <v>0</v>
       </c>
-      <c r="Y5" s="23">
+      <c r="Y5" s="8">
         <v>0</v>
       </c>
       <c r="Z5" s="23">
@@ -2166,10 +2181,13 @@
       <c r="AB5" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" s="12" customFormat="1" spans="1:28">
+      <c r="AC5" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" s="12" customFormat="1" spans="1:29">
       <c r="A6" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
@@ -2232,15 +2250,15 @@
         <v>0</v>
       </c>
       <c r="V6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6" s="3">
         <v>0</v>
       </c>
       <c r="X6" s="3">
-        <v>1</v>
-      </c>
-      <c r="Y6" s="23">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="3">
         <v>1</v>
       </c>
       <c r="Z6" s="23">
@@ -2252,10 +2270,13 @@
       <c r="AB6" s="23">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" s="8" customFormat="1" ht="17" spans="1:28">
+      <c r="AC6" s="23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" s="8" customFormat="1" ht="17" spans="1:29">
       <c r="A7" s="17" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -2326,7 +2347,7 @@
       <c r="X7" s="8">
         <v>0</v>
       </c>
-      <c r="Y7" s="23">
+      <c r="Y7" s="8">
         <v>0</v>
       </c>
       <c r="Z7" s="23">
@@ -2338,10 +2359,13 @@
       <c r="AB7" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" s="8" customFormat="1" ht="17" spans="1:28">
+      <c r="AC7" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" s="8" customFormat="1" ht="17" spans="1:29">
       <c r="A8" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -2412,7 +2436,7 @@
       <c r="X8" s="8">
         <v>0</v>
       </c>
-      <c r="Y8" s="23">
+      <c r="Y8" s="8">
         <v>0</v>
       </c>
       <c r="Z8" s="23">
@@ -2424,10 +2448,13 @@
       <c r="AB8" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" s="8" customFormat="1" ht="17" spans="1:28">
+      <c r="AC8" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" s="8" customFormat="1" ht="17" spans="1:29">
       <c r="A9" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B9" s="8">
         <v>0</v>
@@ -2498,7 +2525,7 @@
       <c r="X9" s="8">
         <v>0</v>
       </c>
-      <c r="Y9" s="23">
+      <c r="Y9" s="8">
         <v>0</v>
       </c>
       <c r="Z9" s="23">
@@ -2510,71 +2537,74 @@
       <c r="AB9" s="23">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" s="13" customFormat="1" ht="101.75" spans="1:28">
+      <c r="AC9" s="23">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" s="13" customFormat="1" ht="101.75" spans="1:29">
       <c r="A10" s="18" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="K10" s="19"/>
       <c r="L10" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="M10" s="19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="N10" s="19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="O10" s="19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="Q10" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="R10" s="19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="S10" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="T10" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="U10" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="V10" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="W10" s="19" t="s">
         <v>59</v>
@@ -2582,11 +2612,11 @@
       <c r="X10" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="Y10" s="24" t="s">
+      <c r="Y10" s="19" t="s">
         <v>61</v>
       </c>
       <c r="Z10" s="24" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="AA10" s="24" t="s">
         <v>62</v>
@@ -2594,10 +2624,13 @@
       <c r="AB10" s="24" t="s">
         <v>63</v>
       </c>
+      <c r="AC10" s="24" t="s">
+        <v>64</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 H3:J3 K3 L3:S3 B5:J5 K5 L5:T5 U5 V5:AB5 K7:K9 U7:U9 B7:J9 L7:T9 Y6:AB9 V7:W9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 H3:J3 K3 L3:S3 B5:J5 K5 L5:T5 U5 V5 W5:AC5 K7:K9 U7:U9 V7:V9 B7:J9 L7:T9 Z6:AC9 W7:X9">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>
@@ -2626,30 +2659,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="10" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>
@@ -2692,7 +2725,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2701,7 +2734,7 @@
     </row>
     <row r="2" s="7" customFormat="1" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B2" s="3">
         <v>256</v>
@@ -2713,7 +2746,7 @@
     </row>
     <row r="3" s="7" customFormat="1" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B3" s="3">
         <v>14</v>
@@ -2725,7 +2758,7 @@
     </row>
     <row r="4" s="7" customFormat="1" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -2737,7 +2770,7 @@
     </row>
     <row r="5" s="7" customFormat="1" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
@@ -2749,7 +2782,7 @@
     </row>
     <row r="6" s="7" customFormat="1" spans="1:6">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -2761,7 +2794,7 @@
     </row>
     <row r="7" s="8" customFormat="1" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -2773,7 +2806,7 @@
     </row>
     <row r="8" s="8" customFormat="1" ht="18" customHeight="1" spans="1:6">
       <c r="A8" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -2785,7 +2818,7 @@
     </row>
     <row r="9" s="8" customFormat="1" ht="18" customHeight="1" spans="1:6">
       <c r="A9" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -2797,7 +2830,7 @@
     </row>
     <row r="10" s="9" customFormat="1" ht="17.55" spans="1:6">
       <c r="A10" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -2809,95 +2842,95 @@
     </row>
     <row r="11" customFormat="1" spans="1:14">
       <c r="A11" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="12" customFormat="1" spans="1:14">
       <c r="A12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="M12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="J12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="N12" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" customFormat="1" spans="1:14">
       <c r="A13" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2918,12 +2951,12 @@
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="15" customFormat="1" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B15" s="3">
         <v>512</v>
@@ -2931,7 +2964,7 @@
     </row>
     <row r="16" customFormat="1" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B16" s="3">
         <v>2</v>
@@ -2939,7 +2972,7 @@
     </row>
     <row r="17" customFormat="1" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -2947,7 +2980,7 @@
     </row>
     <row r="18" customFormat="1" spans="1:2">
       <c r="A18" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
@@ -2955,7 +2988,7 @@
     </row>
     <row r="19" customFormat="1" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
@@ -2963,7 +2996,7 @@
     </row>
     <row r="20" customFormat="1" spans="1:2">
       <c r="A20" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
@@ -2971,7 +3004,7 @@
     </row>
     <row r="21" customFormat="1" spans="1:2">
       <c r="A21" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -2979,7 +3012,7 @@
     </row>
     <row r="22" customFormat="1" spans="1:2">
       <c r="A22" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B22" s="3">
         <v>0</v>
@@ -2987,7 +3020,7 @@
     </row>
     <row r="23" customFormat="1" spans="1:2">
       <c r="A23" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B23" s="3">
         <v>0</v>
@@ -2995,23 +3028,23 @@
     </row>
     <row r="24" customFormat="1" spans="1:2">
       <c r="A24" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" customFormat="1" spans="1:2">
       <c r="A25" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>30</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="26" customFormat="1" spans="1:2">
       <c r="A26" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B26" s="5"/>
     </row>
@@ -3053,7 +3086,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -3064,7 +3097,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B2" s="3">
         <v>64</v>
@@ -3078,7 +3111,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B3" s="3">
         <v>8</v>
@@ -3092,7 +3125,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -3106,7 +3139,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
@@ -3120,7 +3153,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -3134,7 +3167,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -3148,7 +3181,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -3162,7 +3195,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -3176,7 +3209,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -3190,25 +3223,25 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>6</v>
@@ -3216,33 +3249,33 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>29</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
@@ -3257,13 +3290,13 @@
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B15" s="3">
         <v>512</v>
@@ -3272,7 +3305,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B16" s="3">
         <v>3</v>
@@ -3281,7 +3314,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -3290,7 +3323,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
@@ -3299,7 +3332,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
@@ -3308,7 +3341,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
@@ -3317,7 +3350,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -3326,7 +3359,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B22" s="3">
         <v>0</v>
@@ -3335,7 +3368,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B23" s="3">
         <v>0</v>
@@ -3344,29 +3377,29 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -3402,12 +3435,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add team id as a default property for player
</commit_message>
<xml_diff>
--- a/_Out/NFDataCfg/Excel/Player.xlsx
+++ b/_Out/NFDataCfg/Excel/Player.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView windowWidth="30880" windowHeight="13360"/>
+    <workbookView windowHeight="16820"/>
   </bookViews>
   <sheets>
     <sheet name="Property1" sheetId="1" r:id="rId1"/>
@@ -127,7 +127,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102">
   <si>
     <t>Id</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>NoticeID</t>
+  </si>
+  <si>
+    <t>TeamID</t>
   </si>
   <si>
     <t>ClanID</t>
@@ -437,10 +440,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;$&quot;* #,##0_-;\-&quot;$&quot;* #,##0_-;_-&quot;$&quot;* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -479,8 +482,32 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -494,11 +521,92 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -517,111 +625,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="37">
     <fill>
@@ -656,7 +659,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -668,61 +797,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -734,109 +839,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -981,6 +984,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1020,6 +1038,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -1046,30 +1073,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1083,148 +1086,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="13" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="14" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="16" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="12" borderId="13" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="15" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1292,9 +1295,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1302,6 +1302,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1716,12 +1719,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:AC10"/>
+  <dimension ref="A1:AD10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="10" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="V6" sqref="V6"/>
+      <selection pane="bottomLeft" activeCell="V3" sqref="V3:V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8"/>
@@ -1736,11 +1739,11 @@
     <col min="17" max="17" width="10.3365384615385" customWidth="1"/>
     <col min="18" max="18" width="17.1346153846154" customWidth="1"/>
     <col min="19" max="19" width="12.3365384615385" customWidth="1"/>
-    <col min="25" max="25" width="18.3365384615385" customWidth="1"/>
-    <col min="26" max="29" width="17.3365384615385" customWidth="1"/>
+    <col min="26" max="26" width="18.3365384615385" customWidth="1"/>
+    <col min="27" max="30" width="17.3365384615385" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="1" ht="17" spans="1:29">
+    <row r="1" s="11" customFormat="1" ht="17" spans="1:30">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1816,111 +1819,117 @@
       <c r="Y1" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="20" t="s">
+      <c r="Z1" s="15" t="s">
         <v>25</v>
       </c>
       <c r="AA1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="21" t="s">
+      <c r="AB1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="AC1" s="21" t="s">
+      <c r="AC1" s="24" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="2" s="12" customFormat="1" spans="1:29">
+      <c r="AD1" s="24" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" s="12" customFormat="1" spans="1:30">
       <c r="A2" s="16" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="M2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="Q2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="Y2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="Z2" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="AA2" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB2" s="22" t="s">
-        <v>31</v>
-      </c>
-      <c r="AC2" s="22" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" s="12" customFormat="1" spans="1:29">
+      <c r="Z2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AA2" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="AB2" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="AC2" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD2" s="21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" s="12" customFormat="1" spans="1:30">
       <c r="A3" s="16" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B3" s="3">
         <v>1</v>
@@ -1991,25 +2000,28 @@
       <c r="X3" s="3">
         <v>0</v>
       </c>
-      <c r="Y3" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="22">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="22">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="22">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="22">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" s="12" customFormat="1" spans="1:29">
+      <c r="Y3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="21">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="21">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" s="12" customFormat="1" spans="1:30">
       <c r="A4" s="16" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B4" s="3">
         <v>1</v>
@@ -2075,30 +2087,33 @@
         <v>1</v>
       </c>
       <c r="W4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X4" s="3">
         <v>0</v>
       </c>
       <c r="Y4" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z4" s="22">
-        <v>1</v>
-      </c>
-      <c r="AA4" s="22">
-        <v>1</v>
-      </c>
-      <c r="AB4" s="22">
-        <v>1</v>
-      </c>
-      <c r="AC4" s="22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" s="12" customFormat="1" spans="1:29">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA4" s="21">
+        <v>1</v>
+      </c>
+      <c r="AB4" s="21">
+        <v>1</v>
+      </c>
+      <c r="AC4" s="21">
+        <v>1</v>
+      </c>
+      <c r="AD4" s="21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" s="12" customFormat="1" spans="1:30">
       <c r="A5" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B5" s="8">
         <v>0</v>
@@ -2172,22 +2187,25 @@
       <c r="Y5" s="8">
         <v>0</v>
       </c>
-      <c r="Z5" s="23">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB5" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" s="12" customFormat="1" spans="1:29">
+      <c r="Z5" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="22">
+        <v>0</v>
+      </c>
+      <c r="AB5" s="22">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="22">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" s="12" customFormat="1" spans="1:30">
       <c r="A6" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B6" s="3">
         <v>1</v>
@@ -2253,30 +2271,33 @@
         <v>1</v>
       </c>
       <c r="W6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X6" s="3">
         <v>0</v>
       </c>
       <c r="Y6" s="3">
-        <v>1</v>
-      </c>
-      <c r="Z6" s="23">
-        <v>1</v>
-      </c>
-      <c r="AA6" s="23">
-        <v>1</v>
-      </c>
-      <c r="AB6" s="23">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="23">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" s="8" customFormat="1" ht="17" spans="1:29">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA6" s="22">
+        <v>1</v>
+      </c>
+      <c r="AB6" s="22">
+        <v>1</v>
+      </c>
+      <c r="AC6" s="22">
+        <v>1</v>
+      </c>
+      <c r="AD6" s="22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" s="8" customFormat="1" ht="17" spans="1:30">
       <c r="A7" s="17" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B7" s="8">
         <v>0</v>
@@ -2350,22 +2371,25 @@
       <c r="Y7" s="8">
         <v>0</v>
       </c>
-      <c r="Z7" s="23">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB7" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC7" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" s="8" customFormat="1" ht="17" spans="1:29">
+      <c r="Z7" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="22">
+        <v>0</v>
+      </c>
+      <c r="AB7" s="22">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="22">
+        <v>0</v>
+      </c>
+      <c r="AD7" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" s="8" customFormat="1" ht="17" spans="1:30">
       <c r="A8" s="17" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B8" s="8">
         <v>0</v>
@@ -2439,22 +2463,25 @@
       <c r="Y8" s="8">
         <v>0</v>
       </c>
-      <c r="Z8" s="23">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB8" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC8" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" s="8" customFormat="1" ht="17" spans="1:29">
+      <c r="Z8" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="22">
+        <v>0</v>
+      </c>
+      <c r="AB8" s="22">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="22">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" s="8" customFormat="1" ht="17" spans="1:30">
       <c r="A9" s="17" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B9" s="8">
         <v>0</v>
@@ -2528,86 +2555,89 @@
       <c r="Y9" s="8">
         <v>0</v>
       </c>
-      <c r="Z9" s="23">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="23">
-        <v>0</v>
-      </c>
-      <c r="AB9" s="23">
-        <v>0</v>
-      </c>
-      <c r="AC9" s="23">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" s="13" customFormat="1" ht="101.75" spans="1:29">
+      <c r="Z9" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="22">
+        <v>0</v>
+      </c>
+      <c r="AB9" s="22">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="22">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" s="13" customFormat="1" ht="101.75" spans="1:30">
       <c r="A10" s="18" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E10" s="19" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="F10" s="19" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H10" s="19" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="I10" s="19" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="J10" s="19" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="K10" s="19"/>
       <c r="L10" s="19" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="M10" s="19" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="N10" s="19" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="O10" s="19" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="P10" s="19" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="Q10" s="19" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="R10" s="19" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="S10" s="19" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="T10" s="19" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="U10" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="V10" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="W10" s="19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="X10" s="19" t="s">
         <v>60</v>
@@ -2615,22 +2645,25 @@
       <c r="Y10" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="Z10" s="24" t="s">
+      <c r="Z10" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="AA10" s="24" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB10" s="24" t="s">
+      <c r="AA10" s="23" t="s">
         <v>63</v>
       </c>
-      <c r="AC10" s="24" t="s">
+      <c r="AB10" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC10" s="23" t="s">
         <v>64</v>
+      </c>
+      <c r="AD10" s="23" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 H3:J3 K3 L3:S3 B5:J5 K5 L5:T5 U5 V5 W5:AC5 K7:K9 U7:U9 V7:V9 B7:J9 L7:T9 Z6:AC9 W7:X9">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F3 H3:J3 K3 L3:S3 B5:J5 K5 L5:T5 U5 V5 W5 X5:AD5 K7:K9 U7:U9 V7:V9 W7:W9 B7:J9 L7:T9 AA6:AD9 X7:Y9">
       <formula1>"TRUE,FALSE"</formula1>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A7:A9"/>
@@ -2659,30 +2692,30 @@
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C1" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="10" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
   </sheetData>
@@ -2725,7 +2758,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -2734,7 +2767,7 @@
     </row>
     <row r="2" s="7" customFormat="1" spans="1:6">
       <c r="A2" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B2" s="3">
         <v>256</v>
@@ -2746,7 +2779,7 @@
     </row>
     <row r="3" s="7" customFormat="1" spans="1:6">
       <c r="A3" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B3" s="3">
         <v>14</v>
@@ -2758,7 +2791,7 @@
     </row>
     <row r="4" s="7" customFormat="1" spans="1:6">
       <c r="A4" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -2770,7 +2803,7 @@
     </row>
     <row r="5" s="7" customFormat="1" spans="1:6">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
@@ -2782,7 +2815,7 @@
     </row>
     <row r="6" s="7" customFormat="1" spans="1:6">
       <c r="A6" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -2794,7 +2827,7 @@
     </row>
     <row r="7" s="8" customFormat="1" spans="1:6">
       <c r="A7" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -2806,7 +2839,7 @@
     </row>
     <row r="8" s="8" customFormat="1" ht="18" customHeight="1" spans="1:6">
       <c r="A8" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -2818,7 +2851,7 @@
     </row>
     <row r="9" s="8" customFormat="1" ht="18" customHeight="1" spans="1:6">
       <c r="A9" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -2830,7 +2863,7 @@
     </row>
     <row r="10" s="9" customFormat="1" ht="17.55" spans="1:6">
       <c r="A10" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -2842,95 +2875,95 @@
     </row>
     <row r="11" customFormat="1" spans="1:14">
       <c r="A11" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="I11" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="N11" s="4" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" customFormat="1" spans="1:14">
       <c r="A12" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="I12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="L12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="I12" s="4" t="s">
+      <c r="M12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="J12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="K12" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="L12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="M12" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="N12" s="4" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
     </row>
     <row r="13" customFormat="1" spans="1:14">
       <c r="A13" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -2951,12 +2984,12 @@
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" customFormat="1" spans="1:2">
       <c r="A15" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B15" s="3">
         <v>512</v>
@@ -2964,7 +2997,7 @@
     </row>
     <row r="16" customFormat="1" spans="1:2">
       <c r="A16" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B16" s="3">
         <v>2</v>
@@ -2972,7 +3005,7 @@
     </row>
     <row r="17" customFormat="1" spans="1:2">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -2980,7 +3013,7 @@
     </row>
     <row r="18" customFormat="1" spans="1:2">
       <c r="A18" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
@@ -2988,7 +3021,7 @@
     </row>
     <row r="19" customFormat="1" spans="1:2">
       <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
@@ -2996,7 +3029,7 @@
     </row>
     <row r="20" customFormat="1" spans="1:2">
       <c r="A20" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
@@ -3004,7 +3037,7 @@
     </row>
     <row r="21" customFormat="1" spans="1:2">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -3012,7 +3045,7 @@
     </row>
     <row r="22" customFormat="1" spans="1:2">
       <c r="A22" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B22" s="3">
         <v>0</v>
@@ -3020,7 +3053,7 @@
     </row>
     <row r="23" customFormat="1" spans="1:2">
       <c r="A23" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B23" s="3">
         <v>0</v>
@@ -3028,23 +3061,23 @@
     </row>
     <row r="24" customFormat="1" spans="1:2">
       <c r="A24" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="25" customFormat="1" spans="1:2">
       <c r="A25" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="26" customFormat="1" spans="1:2">
       <c r="A26" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B26" s="5"/>
     </row>
@@ -3086,7 +3119,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
@@ -3097,7 +3130,7 @@
     </row>
     <row r="2" spans="1:8">
       <c r="A2" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B2" s="3">
         <v>64</v>
@@ -3111,7 +3144,7 @@
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B3" s="3">
         <v>8</v>
@@ -3125,7 +3158,7 @@
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B4" s="3">
         <v>0</v>
@@ -3139,7 +3172,7 @@
     </row>
     <row r="5" spans="1:8">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B5" s="3">
         <v>1</v>
@@ -3153,7 +3186,7 @@
     </row>
     <row r="6" spans="1:8">
       <c r="A6" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6" s="3">
         <v>0</v>
@@ -3167,7 +3200,7 @@
     </row>
     <row r="7" spans="1:8">
       <c r="A7" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B7" s="3">
         <v>1</v>
@@ -3181,7 +3214,7 @@
     </row>
     <row r="8" spans="1:8">
       <c r="A8" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B8" s="3">
         <v>0</v>
@@ -3195,7 +3228,7 @@
     </row>
     <row r="9" spans="1:8">
       <c r="A9" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B9" s="3">
         <v>0</v>
@@ -3209,7 +3242,7 @@
     </row>
     <row r="10" spans="1:8">
       <c r="A10" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B10" s="3">
         <v>0</v>
@@ -3223,25 +3256,25 @@
     </row>
     <row r="11" spans="1:8">
       <c r="A11" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E11" s="4" t="s">
         <v>4</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="H11" s="4" t="s">
         <v>6</v>
@@ -3249,33 +3282,33 @@
     </row>
     <row r="12" spans="1:8">
       <c r="A12" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="C12" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="E12" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>30</v>
-      </c>
       <c r="F12" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:8">
       <c r="A13" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="5"/>
@@ -3290,13 +3323,13 @@
         <v>0</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C14" s="2"/>
     </row>
     <row r="15" spans="1:3">
       <c r="A15" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="B15" s="3">
         <v>512</v>
@@ -3305,7 +3338,7 @@
     </row>
     <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B16" s="3">
         <v>3</v>
@@ -3314,7 +3347,7 @@
     </row>
     <row r="17" spans="1:3">
       <c r="A17" s="3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B17" s="3">
         <v>0</v>
@@ -3323,7 +3356,7 @@
     </row>
     <row r="18" spans="1:3">
       <c r="A18" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B18" s="3">
         <v>1</v>
@@ -3332,7 +3365,7 @@
     </row>
     <row r="19" spans="1:3">
       <c r="A19" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B19" s="3">
         <v>0</v>
@@ -3341,7 +3374,7 @@
     </row>
     <row r="20" spans="1:3">
       <c r="A20" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3">
         <v>1</v>
@@ -3350,7 +3383,7 @@
     </row>
     <row r="21" spans="1:3">
       <c r="A21" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B21" s="3">
         <v>0</v>
@@ -3359,7 +3392,7 @@
     </row>
     <row r="22" spans="1:3">
       <c r="A22" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B22" s="3">
         <v>0</v>
@@ -3368,7 +3401,7 @@
     </row>
     <row r="23" spans="1:3">
       <c r="A23" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B23" s="3">
         <v>0</v>
@@ -3377,29 +3410,29 @@
     </row>
     <row r="24" spans="1:3">
       <c r="A24" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="25" spans="1:3">
       <c r="A25" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="26" spans="1:3">
       <c r="A26" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -3435,12 +3468,12 @@
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>

</xml_diff>